<commit_message>
CIERRE 19 OCT 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
+++ b/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="328">
   <si>
     <t xml:space="preserve">RELACION DE UNIDADES Y ASIGNACION </t>
   </si>
@@ -1028,9 +1028,6 @@
     <t>25 AGO-21      211,900  KM</t>
   </si>
   <si>
-    <t>SEPT.,2021</t>
-  </si>
-  <si>
     <t>20-JUL.,2021    154,745  KM</t>
   </si>
   <si>
@@ -1050,6 +1047,18 @@
   </si>
   <si>
     <t>3-SEPT-2021    67,052  KM</t>
+  </si>
+  <si>
+    <t>12 OCT.,2021     61,574 KM</t>
+  </si>
+  <si>
+    <t>12-OCT-,2021   253,113 KM</t>
+  </si>
+  <si>
+    <t>11-OCT-,2021  139,811 KM</t>
+  </si>
+  <si>
+    <t>4-OCT-,2021   190,057 KM</t>
   </si>
 </sst>
 </file>
@@ -1737,7 +1746,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="352">
+  <cellXfs count="353">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2680,13 +2689,7 @@
     <xf numFmtId="15" fontId="12" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="12" fillId="21" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="12" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="21" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2715,6 +2718,15 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="38" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="12" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3600,14 +3612,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="344" t="s">
+      <c r="B1" s="342" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="344"/>
-      <c r="D1" s="344"/>
-      <c r="E1" s="345"/>
-      <c r="F1" s="344"/>
-      <c r="G1" s="344"/>
+      <c r="C1" s="342"/>
+      <c r="D1" s="342"/>
+      <c r="E1" s="343"/>
+      <c r="F1" s="342"/>
+      <c r="G1" s="342"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -3968,10 +3980,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="346" t="s">
+      <c r="L12" s="344" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="347"/>
+      <c r="M12" s="345"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -5166,14 +5178,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="344" t="s">
+      <c r="B1" s="342" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="344"/>
-      <c r="D1" s="344"/>
-      <c r="E1" s="345"/>
-      <c r="F1" s="344"/>
-      <c r="G1" s="344"/>
+      <c r="C1" s="342"/>
+      <c r="D1" s="342"/>
+      <c r="E1" s="343"/>
+      <c r="F1" s="342"/>
+      <c r="G1" s="342"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -5512,10 +5524,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="346" t="s">
+      <c r="L12" s="344" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="347"/>
+      <c r="M12" s="345"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -6467,8 +6479,8 @@
   </sheetPr>
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -6495,14 +6507,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="348" t="s">
+      <c r="B1" s="346" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="348"/>
-      <c r="D1" s="348"/>
-      <c r="E1" s="349"/>
-      <c r="F1" s="348"/>
-      <c r="G1" s="348"/>
+      <c r="C1" s="346"/>
+      <c r="D1" s="346"/>
+      <c r="E1" s="347"/>
+      <c r="F1" s="346"/>
+      <c r="G1" s="346"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
@@ -6825,8 +6837,8 @@
       <c r="H12" s="229"/>
       <c r="I12" s="137"/>
       <c r="J12" s="137"/>
-      <c r="K12" s="350"/>
-      <c r="L12" s="351"/>
+      <c r="K12" s="348"/>
+      <c r="L12" s="349"/>
       <c r="M12" s="213"/>
       <c r="N12" s="213"/>
       <c r="O12" s="213"/>
@@ -6974,7 +6986,7 @@
         <v>292</v>
       </c>
       <c r="I16" s="321" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="J16" s="137"/>
       <c r="K16" s="213"/>
@@ -7053,7 +7065,7 @@
       <c r="H18" s="100" t="s">
         <v>293</v>
       </c>
-      <c r="I18" s="343" t="s">
+      <c r="I18" s="341" t="s">
         <v>312</v>
       </c>
       <c r="J18" s="240"/>
@@ -7138,8 +7150,8 @@
       <c r="I20" s="338" t="s">
         <v>303</v>
       </c>
-      <c r="J20" s="341" t="s">
-        <v>322</v>
+      <c r="J20" s="340" t="s">
+        <v>321</v>
       </c>
       <c r="K20" s="106"/>
       <c r="L20" s="137"/>
@@ -7173,11 +7185,11 @@
       <c r="G21" s="234" t="s">
         <v>79</v>
       </c>
-      <c r="H21" s="325" t="s">
+      <c r="H21" s="338" t="s">
         <v>285</v>
       </c>
-      <c r="I21" s="342" t="s">
-        <v>317</v>
+      <c r="I21" s="321" t="s">
+        <v>324</v>
       </c>
       <c r="J21" s="106"/>
       <c r="K21" s="213"/>
@@ -7215,7 +7227,7 @@
         <v>283</v>
       </c>
       <c r="I22" s="105" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J22" s="137"/>
       <c r="K22" s="213"/>
@@ -7365,7 +7377,7 @@
         <v>247</v>
       </c>
       <c r="I26" s="321" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J26" s="137"/>
       <c r="K26" s="213"/>
@@ -7401,11 +7413,11 @@
       <c r="G27" s="218" t="s">
         <v>69</v>
       </c>
-      <c r="H27" s="100" t="s">
+      <c r="H27" s="106" t="s">
         <v>290</v>
       </c>
-      <c r="I27" s="340" t="s">
-        <v>317</v>
+      <c r="I27" s="352" t="s">
+        <v>327</v>
       </c>
       <c r="J27" s="299"/>
       <c r="K27" s="221"/>
@@ -7485,7 +7497,7 @@
         <v>281</v>
       </c>
       <c r="I29" s="321" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J29" s="213"/>
       <c r="K29" s="213"/>
@@ -7531,7 +7543,7 @@
         <v>307</v>
       </c>
       <c r="K30" s="325" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="L30" s="106"/>
       <c r="M30" s="137"/>
@@ -7569,7 +7581,7 @@
         <v>246</v>
       </c>
       <c r="I31" s="339" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J31" s="137"/>
       <c r="K31" s="152"/>
@@ -7614,10 +7626,12 @@
       <c r="J32" s="338" t="s">
         <v>304</v>
       </c>
-      <c r="K32" s="339" t="s">
+      <c r="K32" s="350" t="s">
         <v>313</v>
       </c>
-      <c r="L32" s="106"/>
+      <c r="L32" s="100" t="s">
+        <v>325</v>
+      </c>
       <c r="M32" s="106"/>
       <c r="N32" s="106"/>
       <c r="O32" s="137"/>
@@ -7655,10 +7669,12 @@
       <c r="I33" s="249" t="s">
         <v>306</v>
       </c>
-      <c r="J33" s="100" t="s">
+      <c r="J33" s="106" t="s">
         <v>309</v>
       </c>
-      <c r="K33" s="250"/>
+      <c r="K33" s="351" t="s">
+        <v>326</v>
+      </c>
       <c r="L33" s="137"/>
       <c r="M33" s="137"/>
       <c r="N33" s="137"/>
@@ -7689,7 +7705,7 @@
         <v>245</v>
       </c>
       <c r="G34" s="218"/>
-      <c r="H34" s="325" t="s">
+      <c r="H34" s="321" t="s">
         <v>302</v>
       </c>
       <c r="I34" s="249"/>
@@ -7827,14 +7843,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="348" t="s">
+      <c r="B1" s="346" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="348"/>
-      <c r="D1" s="348"/>
-      <c r="E1" s="349"/>
-      <c r="F1" s="348"/>
-      <c r="G1" s="348"/>
+      <c r="C1" s="346"/>
+      <c r="D1" s="346"/>
+      <c r="E1" s="347"/>
+      <c r="F1" s="346"/>
+      <c r="G1" s="346"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>

</xml_diff>

<commit_message>
CIERRE 9 DIC 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
+++ b/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="343">
   <si>
     <t xml:space="preserve">RELACION DE UNIDADES Y ASIGNACION </t>
   </si>
@@ -1089,6 +1089,21 @@
   </si>
   <si>
     <t>NORMA   $262,000.00</t>
+  </si>
+  <si>
+    <t>16-Nov-21   253,958 KM</t>
+  </si>
+  <si>
+    <t>17 Nov-2021    92,576  KM</t>
+  </si>
+  <si>
+    <t>23 Nov-2021   134,513  KM</t>
+  </si>
+  <si>
+    <t>23-Nov-2021   309,842  KM</t>
+  </si>
+  <si>
+    <t>29 Nov-2021   208,502 KM</t>
   </si>
 </sst>
 </file>
@@ -1777,7 +1792,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="358">
+  <cellXfs count="359">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2735,6 +2750,21 @@
     <xf numFmtId="15" fontId="12" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="8" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2759,19 +2789,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="8" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3658,14 +3676,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="345" t="s">
+      <c r="B1" s="350" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="345"/>
-      <c r="D1" s="345"/>
-      <c r="E1" s="346"/>
-      <c r="F1" s="345"/>
-      <c r="G1" s="345"/>
+      <c r="C1" s="350"/>
+      <c r="D1" s="350"/>
+      <c r="E1" s="351"/>
+      <c r="F1" s="350"/>
+      <c r="G1" s="350"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -4026,10 +4044,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="347" t="s">
+      <c r="L12" s="352" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="348"/>
+      <c r="M12" s="353"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -5224,14 +5242,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="345" t="s">
+      <c r="B1" s="350" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="345"/>
-      <c r="D1" s="345"/>
-      <c r="E1" s="346"/>
-      <c r="F1" s="345"/>
-      <c r="G1" s="345"/>
+      <c r="C1" s="350"/>
+      <c r="D1" s="350"/>
+      <c r="E1" s="351"/>
+      <c r="F1" s="350"/>
+      <c r="G1" s="350"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -5570,10 +5588,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="347" t="s">
+      <c r="L12" s="352" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="348"/>
+      <c r="M12" s="353"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -6525,8 +6543,8 @@
   </sheetPr>
   <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="D17" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -6553,14 +6571,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="349" t="s">
+      <c r="B1" s="354" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="349"/>
-      <c r="D1" s="349"/>
-      <c r="E1" s="350"/>
-      <c r="F1" s="349"/>
-      <c r="G1" s="349"/>
+      <c r="C1" s="354"/>
+      <c r="D1" s="354"/>
+      <c r="E1" s="355"/>
+      <c r="F1" s="354"/>
+      <c r="G1" s="354"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
@@ -6883,8 +6901,8 @@
       <c r="H12" s="229"/>
       <c r="I12" s="137"/>
       <c r="J12" s="137"/>
-      <c r="K12" s="351"/>
-      <c r="L12" s="352"/>
+      <c r="K12" s="356"/>
+      <c r="L12" s="357"/>
       <c r="M12" s="213"/>
       <c r="N12" s="213"/>
       <c r="O12" s="213"/>
@@ -6953,10 +6971,12 @@
       <c r="H14" s="137" t="s">
         <v>289</v>
       </c>
-      <c r="I14" s="321" t="s">
+      <c r="I14" s="299" t="s">
         <v>313</v>
       </c>
-      <c r="J14" s="106"/>
+      <c r="J14" s="100" t="s">
+        <v>339</v>
+      </c>
       <c r="K14" s="106"/>
       <c r="L14" s="213"/>
       <c r="M14" s="212"/>
@@ -6995,10 +7015,12 @@
       <c r="I15" s="137" t="s">
         <v>304</v>
       </c>
-      <c r="J15" s="321" t="s">
+      <c r="J15" s="299" t="s">
         <v>314</v>
       </c>
-      <c r="K15" s="235"/>
+      <c r="K15" s="358" t="s">
+        <v>340</v>
+      </c>
       <c r="L15" s="106"/>
       <c r="M15" s="106"/>
       <c r="N15" s="106"/>
@@ -7073,10 +7095,12 @@
       <c r="I17" s="106" t="s">
         <v>295</v>
       </c>
-      <c r="J17" s="100" t="s">
+      <c r="J17" s="106" t="s">
         <v>310</v>
       </c>
-      <c r="K17" s="137"/>
+      <c r="K17" s="325" t="s">
+        <v>342</v>
+      </c>
       <c r="L17" s="106"/>
       <c r="M17" s="137"/>
       <c r="N17" s="238"/>
@@ -7156,10 +7180,12 @@
       <c r="J19" s="338" t="s">
         <v>307</v>
       </c>
-      <c r="K19" s="100" t="s">
+      <c r="K19" s="106" t="s">
         <v>309</v>
       </c>
-      <c r="L19" s="137"/>
+      <c r="L19" s="325" t="s">
+        <v>338</v>
+      </c>
       <c r="M19" s="137"/>
       <c r="N19" s="137"/>
       <c r="O19" s="106"/>
@@ -7588,10 +7614,12 @@
       <c r="J30" s="137" t="s">
         <v>306</v>
       </c>
-      <c r="K30" s="325" t="s">
+      <c r="K30" s="338" t="s">
         <v>317</v>
       </c>
-      <c r="L30" s="106"/>
+      <c r="L30" s="321" t="s">
+        <v>341</v>
+      </c>
       <c r="M30" s="137"/>
       <c r="N30" s="137"/>
       <c r="O30" s="137"/>
@@ -7771,7 +7799,7 @@
       <c r="A35" s="205">
         <v>30</v>
       </c>
-      <c r="B35" s="356" t="s">
+      <c r="B35" s="348" t="s">
         <v>336</v>
       </c>
       <c r="C35" s="331" t="s">
@@ -7807,7 +7835,7 @@
       <c r="A36" s="205">
         <v>31</v>
       </c>
-      <c r="B36" s="356" t="s">
+      <c r="B36" s="348" t="s">
         <v>335</v>
       </c>
       <c r="C36" s="251" t="s">
@@ -7846,16 +7874,16 @@
       <c r="B37" s="330" t="s">
         <v>332</v>
       </c>
-      <c r="C37" s="355" t="s">
+      <c r="C37" s="347" t="s">
         <v>334</v>
       </c>
-      <c r="D37" s="353" t="s">
+      <c r="D37" s="345" t="s">
         <v>333</v>
       </c>
-      <c r="E37" s="357" t="s">
+      <c r="E37" s="349" t="s">
         <v>337</v>
       </c>
-      <c r="F37" s="354" t="s">
+      <c r="F37" s="346" t="s">
         <v>26</v>
       </c>
       <c r="G37" s="218"/>
@@ -7931,14 +7959,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="349" t="s">
+      <c r="B1" s="354" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="349"/>
-      <c r="D1" s="349"/>
-      <c r="E1" s="350"/>
-      <c r="F1" s="349"/>
-      <c r="G1" s="349"/>
+      <c r="C1" s="354"/>
+      <c r="D1" s="354"/>
+      <c r="E1" s="355"/>
+      <c r="F1" s="354"/>
+      <c r="G1" s="354"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>

</xml_diff>

<commit_message>
cierre de 13 dic 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
+++ b/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="345">
   <si>
     <t xml:space="preserve">RELACION DE UNIDADES Y ASIGNACION </t>
   </si>
@@ -1104,6 +1104,12 @@
   </si>
   <si>
     <t>29 Nov-2021   208,502 KM</t>
+  </si>
+  <si>
+    <t>PEPE</t>
+  </si>
+  <si>
+    <t>9-Dic-2021   39,481  KM</t>
   </si>
 </sst>
 </file>
@@ -1792,7 +1798,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="359">
+  <cellXfs count="360">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2765,6 +2771,9 @@
     <xf numFmtId="8" fontId="8" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="37" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2789,8 +2798,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="12" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3676,14 +3685,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="350" t="s">
+      <c r="B1" s="351" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="350"/>
-      <c r="D1" s="350"/>
-      <c r="E1" s="351"/>
-      <c r="F1" s="350"/>
-      <c r="G1" s="350"/>
+      <c r="C1" s="351"/>
+      <c r="D1" s="351"/>
+      <c r="E1" s="352"/>
+      <c r="F1" s="351"/>
+      <c r="G1" s="351"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -4044,10 +4053,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="352" t="s">
+      <c r="L12" s="353" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="353"/>
+      <c r="M12" s="354"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -5242,14 +5251,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="350" t="s">
+      <c r="B1" s="351" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="350"/>
-      <c r="D1" s="350"/>
-      <c r="E1" s="351"/>
-      <c r="F1" s="350"/>
-      <c r="G1" s="350"/>
+      <c r="C1" s="351"/>
+      <c r="D1" s="351"/>
+      <c r="E1" s="352"/>
+      <c r="F1" s="351"/>
+      <c r="G1" s="351"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -5588,10 +5597,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="352" t="s">
+      <c r="L12" s="353" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="353"/>
+      <c r="M12" s="354"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -6543,8 +6552,8 @@
   </sheetPr>
   <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D17" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="B32" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -6571,14 +6580,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="354" t="s">
+      <c r="B1" s="355" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="354"/>
-      <c r="D1" s="354"/>
-      <c r="E1" s="355"/>
-      <c r="F1" s="354"/>
-      <c r="G1" s="354"/>
+      <c r="C1" s="355"/>
+      <c r="D1" s="355"/>
+      <c r="E1" s="356"/>
+      <c r="F1" s="355"/>
+      <c r="G1" s="355"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
@@ -6901,8 +6910,8 @@
       <c r="H12" s="229"/>
       <c r="I12" s="137"/>
       <c r="J12" s="137"/>
-      <c r="K12" s="356"/>
-      <c r="L12" s="357"/>
+      <c r="K12" s="357"/>
+      <c r="L12" s="358"/>
       <c r="M12" s="213"/>
       <c r="N12" s="213"/>
       <c r="O12" s="213"/>
@@ -7018,7 +7027,7 @@
       <c r="J15" s="299" t="s">
         <v>314</v>
       </c>
-      <c r="K15" s="358" t="s">
+      <c r="K15" s="350" t="s">
         <v>340</v>
       </c>
       <c r="L15" s="106"/>
@@ -7776,13 +7785,15 @@
         <v>74</v>
       </c>
       <c r="F34" s="333" t="s">
-        <v>245</v>
+        <v>343</v>
       </c>
       <c r="G34" s="218"/>
-      <c r="H34" s="321" t="s">
+      <c r="H34" s="299" t="s">
         <v>301</v>
       </c>
-      <c r="I34" s="249"/>
+      <c r="I34" s="359" t="s">
+        <v>344</v>
+      </c>
       <c r="J34" s="106"/>
       <c r="K34" s="250"/>
       <c r="L34" s="137"/>
@@ -7959,14 +7970,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="354" t="s">
+      <c r="B1" s="355" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="354"/>
-      <c r="D1" s="354"/>
-      <c r="E1" s="355"/>
-      <c r="F1" s="354"/>
-      <c r="G1" s="354"/>
+      <c r="C1" s="355"/>
+      <c r="D1" s="355"/>
+      <c r="E1" s="356"/>
+      <c r="F1" s="355"/>
+      <c r="G1" s="355"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>

</xml_diff>

<commit_message>
cierre del 3 de enero 2022
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
+++ b/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="347">
   <si>
     <t xml:space="preserve">RELACION DE UNIDADES Y ASIGNACION </t>
   </si>
@@ -1010,9 +1010,6 @@
     <t>24-Ago-21      198,894  KM</t>
   </si>
   <si>
-    <t xml:space="preserve">CORRALON    </t>
-  </si>
-  <si>
     <t>27-JUL-21   237,404 KM</t>
   </si>
   <si>
@@ -1113,6 +1110,12 @@
   </si>
   <si>
     <t>7-Diciembre-2021   17,855 KM</t>
+  </si>
+  <si>
+    <t>16-Dic-21  222,105  KM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Julio 2021    CORRALON    </t>
   </si>
 </sst>
 </file>
@@ -1801,7 +1804,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="360">
+  <cellXfs count="361">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2747,9 +2750,6 @@
     <xf numFmtId="16" fontId="12" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="21" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="15" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2803,6 +2803,12 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="21" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3688,14 +3694,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="352" t="s">
+      <c r="B1" s="351" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="352"/>
-      <c r="D1" s="352"/>
-      <c r="E1" s="353"/>
-      <c r="F1" s="352"/>
-      <c r="G1" s="352"/>
+      <c r="C1" s="351"/>
+      <c r="D1" s="351"/>
+      <c r="E1" s="352"/>
+      <c r="F1" s="351"/>
+      <c r="G1" s="351"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -4056,10 +4062,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="354" t="s">
+      <c r="L12" s="353" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="355"/>
+      <c r="M12" s="354"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -5254,14 +5260,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="352" t="s">
+      <c r="B1" s="351" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="352"/>
-      <c r="D1" s="352"/>
-      <c r="E1" s="353"/>
-      <c r="F1" s="352"/>
-      <c r="G1" s="352"/>
+      <c r="C1" s="351"/>
+      <c r="D1" s="351"/>
+      <c r="E1" s="352"/>
+      <c r="F1" s="351"/>
+      <c r="G1" s="351"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -5600,10 +5606,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="354" t="s">
+      <c r="L12" s="353" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="355"/>
+      <c r="M12" s="354"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -6555,8 +6561,8 @@
   </sheetPr>
   <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -6583,14 +6589,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="356" t="s">
+      <c r="B1" s="355" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="356"/>
-      <c r="D1" s="356"/>
-      <c r="E1" s="357"/>
-      <c r="F1" s="356"/>
-      <c r="G1" s="356"/>
+      <c r="C1" s="355"/>
+      <c r="D1" s="355"/>
+      <c r="E1" s="356"/>
+      <c r="F1" s="355"/>
+      <c r="G1" s="355"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
@@ -6876,7 +6882,7 @@
       </c>
       <c r="G11" s="224"/>
       <c r="H11" s="105" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I11" s="212"/>
       <c r="J11" s="212"/>
@@ -6915,8 +6921,8 @@
       <c r="H12" s="229"/>
       <c r="I12" s="137"/>
       <c r="J12" s="137"/>
-      <c r="K12" s="358"/>
-      <c r="L12" s="359"/>
+      <c r="K12" s="357"/>
+      <c r="L12" s="358"/>
       <c r="M12" s="213"/>
       <c r="N12" s="213"/>
       <c r="O12" s="213"/>
@@ -6986,10 +6992,10 @@
         <v>289</v>
       </c>
       <c r="I14" s="299" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J14" s="100" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="K14" s="106"/>
       <c r="L14" s="213"/>
@@ -7030,10 +7036,10 @@
         <v>304</v>
       </c>
       <c r="J15" s="299" t="s">
-        <v>314</v>
-      </c>
-      <c r="K15" s="350" t="s">
-        <v>340</v>
+        <v>313</v>
+      </c>
+      <c r="K15" s="349" t="s">
+        <v>339</v>
       </c>
       <c r="L15" s="106"/>
       <c r="M15" s="106"/>
@@ -7068,7 +7074,7 @@
         <v>292</v>
       </c>
       <c r="I16" s="321" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J16" s="137"/>
       <c r="K16" s="213"/>
@@ -7113,7 +7119,7 @@
         <v>310</v>
       </c>
       <c r="K17" s="325" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L17" s="106"/>
       <c r="M17" s="137"/>
@@ -7146,13 +7152,15 @@
       <c r="G18" s="218" t="s">
         <v>71</v>
       </c>
-      <c r="H18" s="100" t="s">
+      <c r="H18" s="106" t="s">
         <v>293</v>
       </c>
-      <c r="I18" s="341" t="s">
-        <v>311</v>
-      </c>
-      <c r="J18" s="240"/>
+      <c r="I18" s="360" t="s">
+        <v>346</v>
+      </c>
+      <c r="J18" s="359" t="s">
+        <v>345</v>
+      </c>
       <c r="K18" s="231"/>
       <c r="L18" s="106"/>
       <c r="M18" s="99"/>
@@ -7198,7 +7206,7 @@
         <v>309</v>
       </c>
       <c r="L19" s="325" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="M19" s="137"/>
       <c r="N19" s="137"/>
@@ -7237,7 +7245,7 @@
         <v>302</v>
       </c>
       <c r="J20" s="340" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K20" s="106"/>
       <c r="L20" s="137"/>
@@ -7275,7 +7283,7 @@
         <v>285</v>
       </c>
       <c r="I21" s="321" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="J21" s="106"/>
       <c r="K21" s="213"/>
@@ -7313,7 +7321,7 @@
         <v>283</v>
       </c>
       <c r="I22" s="105" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J22" s="137"/>
       <c r="K22" s="213"/>
@@ -7463,7 +7471,7 @@
         <v>247</v>
       </c>
       <c r="I26" s="321" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J26" s="137"/>
       <c r="K26" s="213"/>
@@ -7502,8 +7510,8 @@
       <c r="H27" s="106" t="s">
         <v>290</v>
       </c>
-      <c r="I27" s="344" t="s">
-        <v>326</v>
+      <c r="I27" s="343" t="s">
+        <v>325</v>
       </c>
       <c r="J27" s="299"/>
       <c r="K27" s="221"/>
@@ -7543,7 +7551,7 @@
         <v>282</v>
       </c>
       <c r="I28" s="105" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="J28" s="137"/>
       <c r="K28" s="137"/>
@@ -7583,7 +7591,7 @@
         <v>281</v>
       </c>
       <c r="I29" s="321" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J29" s="213"/>
       <c r="K29" s="213"/>
@@ -7629,10 +7637,10 @@
         <v>306</v>
       </c>
       <c r="K30" s="338" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="L30" s="321" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="M30" s="137"/>
       <c r="N30" s="137"/>
@@ -7669,7 +7677,7 @@
         <v>246</v>
       </c>
       <c r="I31" s="339" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J31" s="137"/>
       <c r="K31" s="152"/>
@@ -7714,11 +7722,11 @@
       <c r="J32" s="338" t="s">
         <v>303</v>
       </c>
-      <c r="K32" s="342" t="s">
-        <v>312</v>
+      <c r="K32" s="341" t="s">
+        <v>311</v>
       </c>
       <c r="L32" s="100" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M32" s="106"/>
       <c r="N32" s="106"/>
@@ -7760,8 +7768,8 @@
       <c r="J33" s="106" t="s">
         <v>308</v>
       </c>
-      <c r="K33" s="343" t="s">
-        <v>325</v>
+      <c r="K33" s="342" t="s">
+        <v>324</v>
       </c>
       <c r="L33" s="137"/>
       <c r="M33" s="137"/>
@@ -7790,14 +7798,14 @@
         <v>74</v>
       </c>
       <c r="F34" s="333" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G34" s="218"/>
       <c r="H34" s="299" t="s">
         <v>301</v>
       </c>
-      <c r="I34" s="351" t="s">
-        <v>344</v>
+      <c r="I34" s="350" t="s">
+        <v>343</v>
       </c>
       <c r="J34" s="106"/>
       <c r="K34" s="250"/>
@@ -7815,24 +7823,24 @@
       <c r="A35" s="205">
         <v>30</v>
       </c>
-      <c r="B35" s="348" t="s">
-        <v>336</v>
+      <c r="B35" s="347" t="s">
+        <v>335</v>
       </c>
       <c r="C35" s="331" t="s">
         <v>299</v>
       </c>
       <c r="D35" s="336" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E35" s="337" t="s">
         <v>300</v>
       </c>
       <c r="F35" s="305" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G35" s="218"/>
       <c r="H35" s="105" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I35" s="249"/>
       <c r="J35" s="106"/>
@@ -7851,14 +7859,14 @@
       <c r="A36" s="205">
         <v>31</v>
       </c>
-      <c r="B36" s="348" t="s">
-        <v>335</v>
+      <c r="B36" s="347" t="s">
+        <v>334</v>
       </c>
       <c r="C36" s="251" t="s">
         <v>299</v>
       </c>
       <c r="D36" s="336" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E36" s="337" t="s">
         <v>300</v>
@@ -7868,7 +7876,7 @@
       </c>
       <c r="G36" s="218"/>
       <c r="H36" s="105" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I36" s="249"/>
       <c r="J36" s="106"/>
@@ -7888,18 +7896,18 @@
         <v>32</v>
       </c>
       <c r="B37" s="330" t="s">
+        <v>331</v>
+      </c>
+      <c r="C37" s="346" t="s">
+        <v>333</v>
+      </c>
+      <c r="D37" s="344" t="s">
         <v>332</v>
       </c>
-      <c r="C37" s="347" t="s">
-        <v>334</v>
-      </c>
-      <c r="D37" s="345" t="s">
-        <v>333</v>
-      </c>
-      <c r="E37" s="349" t="s">
-        <v>337</v>
-      </c>
-      <c r="F37" s="346" t="s">
+      <c r="E37" s="348" t="s">
+        <v>336</v>
+      </c>
+      <c r="F37" s="345" t="s">
         <v>26</v>
       </c>
       <c r="G37" s="218"/>
@@ -7975,14 +7983,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="356" t="s">
+      <c r="B1" s="355" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="356"/>
-      <c r="D1" s="356"/>
-      <c r="E1" s="357"/>
-      <c r="F1" s="356"/>
-      <c r="G1" s="356"/>
+      <c r="C1" s="355"/>
+      <c r="D1" s="355"/>
+      <c r="E1" s="356"/>
+      <c r="F1" s="355"/>
+      <c r="G1" s="355"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>

</xml_diff>

<commit_message>
CIERRE 3 FEB 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
+++ b/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="352">
   <si>
     <t xml:space="preserve">RELACION DE UNIDADES Y ASIGNACION </t>
   </si>
@@ -1125,6 +1125,12 @@
   </si>
   <si>
     <t>11-Ene-22   150,331 KM</t>
+  </si>
+  <si>
+    <t>24-Ene-2022   179,712 KM</t>
+  </si>
+  <si>
+    <t>25-ENE-22   319,841 KM</t>
   </si>
 </sst>
 </file>
@@ -2792,6 +2798,9 @@
     <xf numFmtId="16" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="38" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2815,9 +2824,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="38" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3703,14 +3709,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="352" t="s">
+      <c r="B1" s="353" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="352"/>
-      <c r="D1" s="352"/>
-      <c r="E1" s="353"/>
-      <c r="F1" s="352"/>
-      <c r="G1" s="352"/>
+      <c r="C1" s="353"/>
+      <c r="D1" s="353"/>
+      <c r="E1" s="354"/>
+      <c r="F1" s="353"/>
+      <c r="G1" s="353"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -4071,10 +4077,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="354" t="s">
+      <c r="L12" s="355" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="355"/>
+      <c r="M12" s="356"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -5269,14 +5275,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="352" t="s">
+      <c r="B1" s="353" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="352"/>
-      <c r="D1" s="352"/>
-      <c r="E1" s="353"/>
-      <c r="F1" s="352"/>
-      <c r="G1" s="352"/>
+      <c r="C1" s="353"/>
+      <c r="D1" s="353"/>
+      <c r="E1" s="354"/>
+      <c r="F1" s="353"/>
+      <c r="G1" s="353"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -5615,10 +5621,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="354" t="s">
+      <c r="L12" s="355" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="355"/>
+      <c r="M12" s="356"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -6570,8 +6576,8 @@
   </sheetPr>
   <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E29" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -6598,14 +6604,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="356" t="s">
+      <c r="B1" s="357" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="356"/>
-      <c r="D1" s="356"/>
-      <c r="E1" s="357"/>
-      <c r="F1" s="356"/>
-      <c r="G1" s="356"/>
+      <c r="C1" s="357"/>
+      <c r="D1" s="357"/>
+      <c r="E1" s="358"/>
+      <c r="F1" s="357"/>
+      <c r="G1" s="357"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
@@ -6930,8 +6936,8 @@
       <c r="H12" s="229"/>
       <c r="I12" s="137"/>
       <c r="J12" s="137"/>
-      <c r="K12" s="358"/>
-      <c r="L12" s="359"/>
+      <c r="K12" s="359"/>
+      <c r="L12" s="360"/>
       <c r="M12" s="213"/>
       <c r="N12" s="213"/>
       <c r="O12" s="213"/>
@@ -7601,10 +7607,12 @@
       <c r="H29" s="137" t="s">
         <v>281</v>
       </c>
-      <c r="I29" s="321" t="s">
+      <c r="I29" s="299" t="s">
         <v>315</v>
       </c>
-      <c r="J29" s="213"/>
+      <c r="J29" s="105" t="s">
+        <v>350</v>
+      </c>
       <c r="K29" s="213"/>
       <c r="L29" s="137"/>
       <c r="M29" s="137"/>
@@ -7650,10 +7658,12 @@
       <c r="K30" s="338" t="s">
         <v>316</v>
       </c>
-      <c r="L30" s="321" t="s">
+      <c r="L30" s="299" t="s">
         <v>340</v>
       </c>
-      <c r="M30" s="137"/>
+      <c r="M30" s="105" t="s">
+        <v>351</v>
+      </c>
       <c r="N30" s="137"/>
       <c r="O30" s="137"/>
       <c r="P30" s="213"/>
@@ -7779,7 +7789,7 @@
       <c r="J33" s="106" t="s">
         <v>308</v>
       </c>
-      <c r="K33" s="360" t="s">
+      <c r="K33" s="352" t="s">
         <v>324</v>
       </c>
       <c r="L33" s="325" t="s">
@@ -7998,14 +8008,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="356" t="s">
+      <c r="B1" s="357" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="356"/>
-      <c r="D1" s="356"/>
-      <c r="E1" s="357"/>
-      <c r="F1" s="356"/>
-      <c r="G1" s="356"/>
+      <c r="C1" s="357"/>
+      <c r="D1" s="357"/>
+      <c r="E1" s="358"/>
+      <c r="F1" s="357"/>
+      <c r="G1" s="357"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>

</xml_diff>

<commit_message>
CIERRE 10 FEB 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
+++ b/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
@@ -6576,8 +6576,8 @@
   </sheetPr>
   <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -7970,8 +7970,8 @@
     <mergeCell ref="K12:L12"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.22" right="0.16" top="0.36" bottom="0.38" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup scale="70" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -7980,7 +7980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
CIERRE 16 FEB 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
+++ b/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="353">
   <si>
     <t xml:space="preserve">RELACION DE UNIDADES Y ASIGNACION </t>
   </si>
@@ -1131,6 +1131,9 @@
   </si>
   <si>
     <t>25-ENE-22   319,841 KM</t>
+  </si>
+  <si>
+    <t>1 Feb-2022   264,950 KM</t>
   </si>
 </sst>
 </file>
@@ -6576,8 +6579,8 @@
   </sheetPr>
   <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="F29" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -7220,10 +7223,12 @@
       <c r="K19" s="106" t="s">
         <v>309</v>
       </c>
-      <c r="L19" s="325" t="s">
+      <c r="L19" s="338" t="s">
         <v>337</v>
       </c>
-      <c r="M19" s="137"/>
+      <c r="M19" s="105" t="s">
+        <v>352</v>
+      </c>
       <c r="N19" s="137"/>
       <c r="O19" s="106"/>
       <c r="P19" s="106"/>
@@ -7749,7 +7754,7 @@
       <c r="L32" s="100" t="s">
         <v>323</v>
       </c>
-      <c r="M32" s="106"/>
+      <c r="M32" s="211"/>
       <c r="N32" s="106"/>
       <c r="O32" s="137"/>
       <c r="P32" s="137"/>

</xml_diff>

<commit_message>
CIERRE 2 MAR 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
+++ b/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="360">
   <si>
     <t xml:space="preserve">RELACION DE UNIDADES Y ASIGNACION </t>
   </si>
@@ -1140,6 +1140,21 @@
   </si>
   <si>
     <t>28 FEB-22   VENDIDA   BAJA</t>
+  </si>
+  <si>
+    <t>19-ENERO-22  42,069 KM</t>
+  </si>
+  <si>
+    <t>23-FEB-22   104,054  KM</t>
+  </si>
+  <si>
+    <t>23 FEB-2022  63, 706  KM</t>
+  </si>
+  <si>
+    <t>22 FEB-22 219,739  KM</t>
+  </si>
+  <si>
+    <t>VENDIDA</t>
   </si>
 </sst>
 </file>
@@ -1462,7 +1477,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1582,6 +1597,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF9999FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1828,7 +1849,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="362">
+  <cellXfs count="367">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2834,8 +2855,21 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6588,8 +6622,8 @@
   </sheetPr>
   <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H29" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView tabSelected="1" topLeftCell="F32" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -7021,11 +7055,13 @@
       <c r="I14" s="299" t="s">
         <v>312</v>
       </c>
-      <c r="J14" s="100" t="s">
+      <c r="J14" s="106" t="s">
         <v>338</v>
       </c>
-      <c r="K14" s="106"/>
-      <c r="L14" s="213"/>
+      <c r="K14" s="100" t="s">
+        <v>356</v>
+      </c>
+      <c r="L14" s="362"/>
       <c r="M14" s="212"/>
       <c r="N14" s="212"/>
       <c r="O14" s="212"/>
@@ -7068,7 +7104,7 @@
       <c r="K15" s="347" t="s">
         <v>339</v>
       </c>
-      <c r="L15" s="106"/>
+      <c r="L15" s="361"/>
       <c r="M15" s="106"/>
       <c r="N15" s="106"/>
       <c r="O15" s="212"/>
@@ -7100,11 +7136,13 @@
       <c r="H16" s="106" t="s">
         <v>292</v>
       </c>
-      <c r="I16" s="321" t="s">
+      <c r="I16" s="299" t="s">
         <v>320</v>
       </c>
-      <c r="J16" s="137"/>
-      <c r="K16" s="213"/>
+      <c r="J16" s="105" t="s">
+        <v>355</v>
+      </c>
+      <c r="K16" s="362"/>
       <c r="L16" s="212"/>
       <c r="M16" s="212"/>
       <c r="N16" s="212"/>
@@ -7145,10 +7183,12 @@
       <c r="J17" s="106" t="s">
         <v>310</v>
       </c>
-      <c r="K17" s="325" t="s">
+      <c r="K17" s="338" t="s">
         <v>341</v>
       </c>
-      <c r="L17" s="106"/>
+      <c r="L17" s="100" t="s">
+        <v>358</v>
+      </c>
       <c r="M17" s="137"/>
       <c r="N17" s="238"/>
       <c r="O17" s="212"/>
@@ -7188,7 +7228,7 @@
       <c r="J18" s="349" t="s">
         <v>345</v>
       </c>
-      <c r="K18" s="231"/>
+      <c r="K18" s="363"/>
       <c r="L18" s="106"/>
       <c r="M18" s="99"/>
       <c r="N18" s="137"/>
@@ -7279,7 +7319,7 @@
       <c r="K20" s="100" t="s">
         <v>348</v>
       </c>
-      <c r="L20" s="137"/>
+      <c r="L20" s="364"/>
       <c r="M20" s="213"/>
       <c r="N20" s="213"/>
       <c r="O20" s="137"/>
@@ -7316,7 +7356,7 @@
       <c r="I21" s="321" t="s">
         <v>322</v>
       </c>
-      <c r="J21" s="106"/>
+      <c r="J21" s="361"/>
       <c r="K21" s="213"/>
       <c r="L21" s="213"/>
       <c r="M21" s="213"/>
@@ -7501,10 +7541,12 @@
       <c r="H26" s="106" t="s">
         <v>247</v>
       </c>
-      <c r="I26" s="321" t="s">
+      <c r="I26" s="299" t="s">
         <v>318</v>
       </c>
-      <c r="J26" s="137"/>
+      <c r="J26" s="105" t="s">
+        <v>357</v>
+      </c>
       <c r="K26" s="213"/>
       <c r="L26" s="213"/>
       <c r="M26" s="213"/>
@@ -7544,7 +7586,9 @@
       <c r="I27" s="341" t="s">
         <v>325</v>
       </c>
-      <c r="J27" s="299"/>
+      <c r="J27" s="365" t="s">
+        <v>359</v>
+      </c>
       <c r="K27" s="221"/>
       <c r="L27" s="137"/>
       <c r="M27" s="137"/>
@@ -7587,7 +7631,7 @@
       <c r="J28" s="100" t="s">
         <v>353</v>
       </c>
-      <c r="K28" s="137"/>
+      <c r="K28" s="364"/>
       <c r="L28" s="106"/>
       <c r="M28" s="137"/>
       <c r="N28" s="137"/>
@@ -7629,7 +7673,7 @@
       <c r="J29" s="105" t="s">
         <v>350</v>
       </c>
-      <c r="K29" s="213"/>
+      <c r="K29" s="362"/>
       <c r="L29" s="137"/>
       <c r="M29" s="137"/>
       <c r="N29" s="99"/>
@@ -7680,7 +7724,7 @@
       <c r="M30" s="137" t="s">
         <v>351</v>
       </c>
-      <c r="N30" s="361" t="s">
+      <c r="N30" s="365" t="s">
         <v>354</v>
       </c>
       <c r="O30" s="137"/>
@@ -7718,7 +7762,7 @@
       <c r="I31" s="339" t="s">
         <v>317</v>
       </c>
-      <c r="J31" s="137"/>
+      <c r="J31" s="366"/>
       <c r="K31" s="152"/>
       <c r="L31" s="106"/>
       <c r="M31" s="137"/>
@@ -7813,7 +7857,7 @@
       <c r="L33" s="325" t="s">
         <v>349</v>
       </c>
-      <c r="M33" s="137"/>
+      <c r="M33" s="366"/>
       <c r="N33" s="137"/>
       <c r="O33" s="256"/>
       <c r="P33" s="106"/>

</xml_diff>

<commit_message>
cierre 4 Abril 2022
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
+++ b/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="365">
   <si>
     <t xml:space="preserve">RELACION DE UNIDADES Y ASIGNACION </t>
   </si>
@@ -1167,6 +1167,9 @@
   </si>
   <si>
     <t>SM 46586-/-*SN-81-676</t>
+  </si>
+  <si>
+    <t>29-Mar-22  44,031  KM</t>
   </si>
 </sst>
 </file>
@@ -6637,8 +6640,8 @@
   </sheetPr>
   <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D17" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -6768,7 +6771,9 @@
         <v>227</v>
       </c>
       <c r="G4" s="51"/>
-      <c r="H4" s="106"/>
+      <c r="H4" s="100" t="s">
+        <v>364</v>
+      </c>
       <c r="I4" s="106"/>
       <c r="J4" s="106"/>
       <c r="K4" s="213"/>

</xml_diff>

<commit_message>
cierre 2 mayo 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
+++ b/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="354">
   <si>
     <t xml:space="preserve">RELACION DE UNIDADES Y ASIGNACION </t>
   </si>
@@ -1121,9 +1121,6 @@
     <t>4-ABRIL-2022   23,034 KM</t>
   </si>
   <si>
-    <t>SM 46586-/-SN-81-676</t>
-  </si>
-  <si>
     <t>XXXXX</t>
   </si>
   <si>
@@ -1131,6 +1128,15 @@
   </si>
   <si>
     <t>19-Abr-22           190,866  KM</t>
+  </si>
+  <si>
+    <t>26-Abr-22  162,282 KM</t>
+  </si>
+  <si>
+    <t>SM 46586-/------------SN-81-676</t>
+  </si>
+  <si>
+    <t>26-Abr-22  232,866  KM</t>
   </si>
 </sst>
 </file>
@@ -1831,7 +1837,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="365">
+  <cellXfs count="366">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2482,9 +2488,6 @@
     <xf numFmtId="17" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2850,6 +2853,12 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3725,14 +3734,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="357" t="s">
+      <c r="B1" s="356" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="357"/>
-      <c r="D1" s="357"/>
-      <c r="E1" s="358"/>
-      <c r="F1" s="357"/>
-      <c r="G1" s="357"/>
+      <c r="C1" s="356"/>
+      <c r="D1" s="356"/>
+      <c r="E1" s="357"/>
+      <c r="F1" s="356"/>
+      <c r="G1" s="356"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -4093,10 +4102,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="359" t="s">
+      <c r="L12" s="358" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="360"/>
+      <c r="M12" s="359"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -5291,14 +5300,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="357" t="s">
+      <c r="B1" s="356" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="357"/>
-      <c r="D1" s="357"/>
-      <c r="E1" s="358"/>
-      <c r="F1" s="357"/>
-      <c r="G1" s="357"/>
+      <c r="C1" s="356"/>
+      <c r="D1" s="356"/>
+      <c r="E1" s="357"/>
+      <c r="F1" s="356"/>
+      <c r="G1" s="356"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -5637,10 +5646,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="359" t="s">
+      <c r="L12" s="358" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="360"/>
+      <c r="M12" s="359"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -6598,7 +6607,7 @@
     <col min="1" max="1" width="5.5703125" style="198" customWidth="1"/>
     <col min="2" max="2" width="22.140625" style="199" customWidth="1"/>
     <col min="3" max="3" width="15" style="199" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" style="267" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="266" customWidth="1"/>
     <col min="5" max="5" width="18.140625" style="199" customWidth="1"/>
     <col min="6" max="6" width="22.85546875" style="199" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" style="199" hidden="1" customWidth="1"/>
@@ -6617,14 +6626,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="361" t="s">
+      <c r="B1" s="360" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="361"/>
-      <c r="D1" s="361"/>
-      <c r="E1" s="362"/>
-      <c r="F1" s="361"/>
-      <c r="G1" s="361"/>
+      <c r="C1" s="360"/>
+      <c r="D1" s="360"/>
+      <c r="E1" s="361"/>
+      <c r="F1" s="360"/>
+      <c r="G1" s="360"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
@@ -6658,11 +6667,11 @@
       <c r="K2" s="204" t="s">
         <v>64</v>
       </c>
-      <c r="L2" s="255" t="s">
+      <c r="L2" s="254" t="s">
         <v>64</v>
       </c>
-      <c r="M2" s="256"/>
-      <c r="N2" s="256"/>
+      <c r="M2" s="255"/>
+      <c r="N2" s="255"/>
     </row>
     <row r="3" spans="1:19" ht="71.25" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="205">
@@ -6674,7 +6683,7 @@
       <c r="C3" s="207">
         <v>2015</v>
       </c>
-      <c r="D3" s="257" t="s">
+      <c r="D3" s="256" t="s">
         <v>32</v>
       </c>
       <c r="E3" s="208" t="s">
@@ -6710,7 +6719,7 @@
       <c r="C4" s="207">
         <v>2019</v>
       </c>
-      <c r="D4" s="315" t="s">
+      <c r="D4" s="314" t="s">
         <v>256</v>
       </c>
       <c r="E4" s="208" t="s">
@@ -6740,7 +6749,7 @@
       <c r="C5" s="215">
         <v>2012</v>
       </c>
-      <c r="D5" s="258" t="s">
+      <c r="D5" s="257" t="s">
         <v>180</v>
       </c>
       <c r="E5" s="216" t="s">
@@ -6792,7 +6801,7 @@
       <c r="C7" s="220">
         <v>2012</v>
       </c>
-      <c r="D7" s="259" t="s">
+      <c r="D7" s="258" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="216" t="s">
@@ -6820,7 +6829,7 @@
       <c r="C8" s="222">
         <v>2011</v>
       </c>
-      <c r="D8" s="260" t="s">
+      <c r="D8" s="259" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="223" t="s">
@@ -6848,7 +6857,7 @@
       <c r="C9" s="219">
         <v>2017</v>
       </c>
-      <c r="D9" s="314" t="s">
+      <c r="D9" s="313" t="s">
         <v>44</v>
       </c>
       <c r="E9" s="216" t="s">
@@ -6875,7 +6884,7 @@
       <c r="C10" s="226">
         <v>2010</v>
       </c>
-      <c r="D10" s="261" t="s">
+      <c r="D10" s="260" t="s">
         <v>75</v>
       </c>
       <c r="E10" s="216" t="s">
@@ -6897,13 +6906,13 @@
       <c r="A11" s="205">
         <v>8</v>
       </c>
-      <c r="B11" s="351" t="s">
+      <c r="B11" s="350" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="351">
+      <c r="C11" s="350">
         <v>2020</v>
       </c>
-      <c r="D11" s="352" t="s">
+      <c r="D11" s="351" t="s">
         <v>346</v>
       </c>
       <c r="E11" s="216" t="s">
@@ -6916,7 +6925,7 @@
       <c r="H11" s="106" t="s">
         <v>325</v>
       </c>
-      <c r="I11" s="312" t="s">
+      <c r="I11" s="311" t="s">
         <v>347</v>
       </c>
       <c r="J11" s="212"/>
@@ -6940,7 +6949,7 @@
       <c r="C12" s="215">
         <v>2018</v>
       </c>
-      <c r="D12" s="263" t="s">
+      <c r="D12" s="262" t="s">
         <v>56</v>
       </c>
       <c r="E12" s="216" t="s">
@@ -6955,8 +6964,8 @@
       <c r="H12" s="228"/>
       <c r="I12" s="137"/>
       <c r="J12" s="137"/>
-      <c r="K12" s="363"/>
-      <c r="L12" s="364"/>
+      <c r="K12" s="362"/>
+      <c r="L12" s="363"/>
       <c r="M12" s="213"/>
       <c r="N12" s="213"/>
       <c r="O12" s="213"/>
@@ -6975,7 +6984,7 @@
       <c r="C13" s="215">
         <v>2020</v>
       </c>
-      <c r="D13" s="263" t="s">
+      <c r="D13" s="262" t="s">
         <v>236</v>
       </c>
       <c r="E13" s="216" t="s">
@@ -7010,7 +7019,7 @@
       <c r="C14" s="232">
         <v>2018</v>
       </c>
-      <c r="D14" s="264" t="s">
+      <c r="D14" s="263" t="s">
         <v>60</v>
       </c>
       <c r="E14" s="208" t="s">
@@ -7025,7 +7034,7 @@
       <c r="H14" s="137" t="s">
         <v>270</v>
       </c>
-      <c r="I14" s="294" t="s">
+      <c r="I14" s="293" t="s">
         <v>293</v>
       </c>
       <c r="J14" s="106" t="s">
@@ -7034,7 +7043,7 @@
       <c r="K14" s="100" t="s">
         <v>337</v>
       </c>
-      <c r="L14" s="345"/>
+      <c r="L14" s="344"/>
       <c r="M14" s="212"/>
       <c r="N14" s="212"/>
       <c r="O14" s="212"/>
@@ -7053,7 +7062,7 @@
       <c r="C15" s="232">
         <v>2018</v>
       </c>
-      <c r="D15" s="264" t="s">
+      <c r="D15" s="263" t="s">
         <v>91</v>
       </c>
       <c r="E15" s="208" t="s">
@@ -7071,13 +7080,13 @@
       <c r="I15" s="137" t="s">
         <v>285</v>
       </c>
-      <c r="J15" s="294" t="s">
+      <c r="J15" s="293" t="s">
         <v>294</v>
       </c>
-      <c r="K15" s="338" t="s">
+      <c r="K15" s="337" t="s">
         <v>320</v>
       </c>
-      <c r="L15" s="344"/>
+      <c r="L15" s="343"/>
       <c r="M15" s="106"/>
       <c r="N15" s="106"/>
       <c r="O15" s="212"/>
@@ -7096,7 +7105,7 @@
       <c r="C16" s="232">
         <v>2019</v>
       </c>
-      <c r="D16" s="264" t="s">
+      <c r="D16" s="263" t="s">
         <v>129</v>
       </c>
       <c r="E16" s="208" t="s">
@@ -7109,13 +7118,13 @@
       <c r="H16" s="106" t="s">
         <v>273</v>
       </c>
-      <c r="I16" s="294" t="s">
+      <c r="I16" s="293" t="s">
         <v>301</v>
       </c>
       <c r="J16" s="105" t="s">
         <v>336</v>
       </c>
-      <c r="K16" s="345"/>
+      <c r="K16" s="344"/>
       <c r="L16" s="212"/>
       <c r="M16" s="212"/>
       <c r="N16" s="212"/>
@@ -7135,7 +7144,7 @@
       <c r="C17" s="232">
         <v>2015</v>
       </c>
-      <c r="D17" s="264" t="s">
+      <c r="D17" s="263" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="236" t="s">
@@ -7156,7 +7165,7 @@
       <c r="J17" s="106" t="s">
         <v>291</v>
       </c>
-      <c r="K17" s="329" t="s">
+      <c r="K17" s="328" t="s">
         <v>322</v>
       </c>
       <c r="L17" s="100" t="s">
@@ -7180,7 +7189,7 @@
       <c r="C18" s="232">
         <v>2015</v>
       </c>
-      <c r="D18" s="350" t="s">
+      <c r="D18" s="349" t="s">
         <v>344</v>
       </c>
       <c r="E18" s="236" t="s">
@@ -7195,13 +7204,13 @@
       <c r="H18" s="106" t="s">
         <v>274</v>
       </c>
-      <c r="I18" s="341" t="s">
+      <c r="I18" s="340" t="s">
         <v>327</v>
       </c>
-      <c r="J18" s="340" t="s">
+      <c r="J18" s="339" t="s">
         <v>326</v>
       </c>
-      <c r="K18" s="346"/>
+      <c r="K18" s="345"/>
       <c r="L18" s="106"/>
       <c r="M18" s="99"/>
       <c r="N18" s="137"/>
@@ -7221,7 +7230,7 @@
       <c r="C19" s="232">
         <v>2017</v>
       </c>
-      <c r="D19" s="264" t="s">
+      <c r="D19" s="263" t="s">
         <v>36</v>
       </c>
       <c r="E19" s="236" t="s">
@@ -7233,19 +7242,19 @@
       <c r="G19" s="233" t="s">
         <v>82</v>
       </c>
-      <c r="H19" s="294" t="s">
+      <c r="H19" s="293" t="s">
         <v>257</v>
       </c>
-      <c r="I19" s="329" t="s">
+      <c r="I19" s="328" t="s">
         <v>267</v>
       </c>
-      <c r="J19" s="329" t="s">
+      <c r="J19" s="328" t="s">
         <v>288</v>
       </c>
       <c r="K19" s="106" t="s">
         <v>290</v>
       </c>
-      <c r="L19" s="329" t="s">
+      <c r="L19" s="328" t="s">
         <v>318</v>
       </c>
       <c r="M19" s="105" t="s">
@@ -7268,31 +7277,31 @@
       <c r="C20" s="232">
         <v>2017</v>
       </c>
-      <c r="D20" s="264" t="s">
+      <c r="D20" s="263" t="s">
         <v>38</v>
       </c>
       <c r="E20" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F20" s="240" t="s">
+      <c r="F20" s="239" t="s">
         <v>19</v>
       </c>
       <c r="G20" s="233" t="s">
         <v>83</v>
       </c>
-      <c r="H20" s="329" t="s">
+      <c r="H20" s="328" t="s">
         <v>275</v>
       </c>
-      <c r="I20" s="329" t="s">
+      <c r="I20" s="328" t="s">
         <v>283</v>
       </c>
-      <c r="J20" s="342" t="s">
+      <c r="J20" s="341" t="s">
         <v>300</v>
       </c>
       <c r="K20" s="100" t="s">
         <v>329</v>
       </c>
-      <c r="L20" s="347"/>
+      <c r="L20" s="346"/>
       <c r="M20" s="213"/>
       <c r="N20" s="213"/>
       <c r="O20" s="137"/>
@@ -7311,22 +7320,22 @@
       <c r="C21" s="232">
         <v>2017</v>
       </c>
-      <c r="D21" s="264" t="s">
+      <c r="D21" s="263" t="s">
         <v>40</v>
       </c>
       <c r="E21" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F21" s="241" t="s">
+      <c r="F21" s="240" t="s">
         <v>5</v>
       </c>
       <c r="G21" s="233" t="s">
         <v>79</v>
       </c>
-      <c r="H21" s="329" t="s">
+      <c r="H21" s="328" t="s">
         <v>266</v>
       </c>
-      <c r="I21" s="312" t="s">
+      <c r="I21" s="311" t="s">
         <v>303</v>
       </c>
       <c r="J21" s="100" t="s">
@@ -7347,13 +7356,13 @@
       <c r="A22" s="205">
         <v>19</v>
       </c>
-      <c r="B22" s="259" t="s">
+      <c r="B22" s="258" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="232">
         <v>2018</v>
       </c>
-      <c r="D22" s="313" t="s">
+      <c r="D22" s="312" t="s">
         <v>54</v>
       </c>
       <c r="E22" s="208" t="s">
@@ -7363,7 +7372,7 @@
         <v>27</v>
       </c>
       <c r="G22" s="224"/>
-      <c r="H22" s="329" t="s">
+      <c r="H22" s="328" t="s">
         <v>264</v>
       </c>
       <c r="I22" s="105" t="s">
@@ -7385,13 +7394,13 @@
       <c r="A23" s="205">
         <v>20</v>
       </c>
-      <c r="B23" s="242" t="s">
+      <c r="B23" s="241" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="242">
+      <c r="C23" s="241">
         <v>2006</v>
       </c>
-      <c r="D23" s="265" t="s">
+      <c r="D23" s="264" t="s">
         <v>16</v>
       </c>
       <c r="E23" s="216" t="s">
@@ -7419,13 +7428,13 @@
       <c r="A24" s="205">
         <v>21</v>
       </c>
-      <c r="B24" s="243" t="s">
+      <c r="B24" s="242" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="243">
+      <c r="C24" s="242">
         <v>2016</v>
       </c>
-      <c r="D24" s="266" t="s">
+      <c r="D24" s="265" t="s">
         <v>23</v>
       </c>
       <c r="E24" s="216" t="s">
@@ -7434,10 +7443,10 @@
       <c r="F24" s="209" t="s">
         <v>55</v>
       </c>
-      <c r="G24" s="244" t="s">
+      <c r="G24" s="243" t="s">
         <v>80</v>
       </c>
-      <c r="H24" s="318" t="s">
+      <c r="H24" s="317" t="s">
         <v>279</v>
       </c>
       <c r="I24" s="137"/>
@@ -7463,7 +7472,7 @@
       <c r="C25" s="219">
         <v>2017</v>
       </c>
-      <c r="D25" s="262" t="s">
+      <c r="D25" s="261" t="s">
         <v>25</v>
       </c>
       <c r="E25" s="216" t="s">
@@ -7475,7 +7484,7 @@
       <c r="G25" s="206" t="s">
         <v>78</v>
       </c>
-      <c r="H25" s="317" t="s">
+      <c r="H25" s="316" t="s">
         <v>278</v>
       </c>
       <c r="I25" s="137"/>
@@ -7501,13 +7510,13 @@
       <c r="C26" s="219">
         <v>2018</v>
       </c>
-      <c r="D26" s="314" t="s">
+      <c r="D26" s="313" t="s">
         <v>58</v>
       </c>
       <c r="E26" s="216" t="s">
         <v>74</v>
       </c>
-      <c r="F26" s="245" t="s">
+      <c r="F26" s="244" t="s">
         <v>199</v>
       </c>
       <c r="G26" s="206" t="s">
@@ -7516,13 +7525,13 @@
       <c r="H26" s="106" t="s">
         <v>247</v>
       </c>
-      <c r="I26" s="294" t="s">
+      <c r="I26" s="293" t="s">
         <v>299</v>
       </c>
       <c r="J26" s="105" t="s">
         <v>338</v>
       </c>
-      <c r="K26" s="345"/>
+      <c r="K26" s="344"/>
       <c r="L26" s="213"/>
       <c r="M26" s="213"/>
       <c r="N26" s="213"/>
@@ -7543,13 +7552,13 @@
       <c r="C27" s="232">
         <v>2015</v>
       </c>
-      <c r="D27" s="264" t="s">
+      <c r="D27" s="263" t="s">
         <v>2</v>
       </c>
       <c r="E27" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F27" s="246" t="s">
+      <c r="F27" s="245" t="s">
         <v>142</v>
       </c>
       <c r="G27" s="218" t="s">
@@ -7558,10 +7567,10 @@
       <c r="H27" s="106" t="s">
         <v>271</v>
       </c>
-      <c r="I27" s="332" t="s">
+      <c r="I27" s="331" t="s">
         <v>306</v>
       </c>
-      <c r="J27" s="348" t="s">
+      <c r="J27" s="347" t="s">
         <v>340</v>
       </c>
       <c r="K27" s="221"/>
@@ -7585,7 +7594,7 @@
       <c r="C28" s="232">
         <v>2015</v>
       </c>
-      <c r="D28" s="264" t="s">
+      <c r="D28" s="263" t="s">
         <v>3</v>
       </c>
       <c r="E28" s="236" t="s">
@@ -7597,7 +7606,7 @@
       <c r="G28" s="218" t="s">
         <v>70</v>
       </c>
-      <c r="H28" s="294" t="s">
+      <c r="H28" s="293" t="s">
         <v>263</v>
       </c>
       <c r="I28" s="137" t="s">
@@ -7606,7 +7615,7 @@
       <c r="J28" s="100" t="s">
         <v>334</v>
       </c>
-      <c r="K28" s="347"/>
+      <c r="K28" s="346"/>
       <c r="L28" s="106"/>
       <c r="M28" s="137"/>
       <c r="N28" s="137"/>
@@ -7627,13 +7636,13 @@
       <c r="C29" s="232">
         <v>2015</v>
       </c>
-      <c r="D29" s="264" t="s">
+      <c r="D29" s="263" t="s">
         <v>4</v>
       </c>
       <c r="E29" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F29" s="247" t="s">
+      <c r="F29" s="246" t="s">
         <v>110</v>
       </c>
       <c r="G29" s="218" t="s">
@@ -7642,13 +7651,13 @@
       <c r="H29" s="137" t="s">
         <v>262</v>
       </c>
-      <c r="I29" s="294" t="s">
+      <c r="I29" s="293" t="s">
         <v>296</v>
       </c>
       <c r="J29" s="105" t="s">
         <v>331</v>
       </c>
-      <c r="K29" s="345"/>
+      <c r="K29" s="344"/>
       <c r="L29" s="137"/>
       <c r="M29" s="137"/>
       <c r="N29" s="99"/>
@@ -7669,7 +7678,7 @@
       <c r="C30" s="232">
         <v>2015</v>
       </c>
-      <c r="D30" s="264" t="s">
+      <c r="D30" s="263" t="s">
         <v>6</v>
       </c>
       <c r="E30" s="236" t="s">
@@ -7690,16 +7699,16 @@
       <c r="J30" s="137" t="s">
         <v>287</v>
       </c>
-      <c r="K30" s="329" t="s">
+      <c r="K30" s="328" t="s">
         <v>297</v>
       </c>
-      <c r="L30" s="294" t="s">
+      <c r="L30" s="293" t="s">
         <v>321</v>
       </c>
       <c r="M30" s="137" t="s">
         <v>332</v>
       </c>
-      <c r="N30" s="348" t="s">
+      <c r="N30" s="347" t="s">
         <v>335</v>
       </c>
       <c r="O30" s="137"/>
@@ -7719,13 +7728,13 @@
       <c r="C31" s="232">
         <v>2015</v>
       </c>
-      <c r="D31" s="264" t="s">
+      <c r="D31" s="263" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="245" t="s">
+      <c r="F31" s="244" t="s">
         <v>151</v>
       </c>
       <c r="G31" s="218" t="s">
@@ -7734,10 +7743,10 @@
       <c r="H31" s="106" t="s">
         <v>246</v>
       </c>
-      <c r="I31" s="330" t="s">
+      <c r="I31" s="329" t="s">
         <v>298</v>
       </c>
-      <c r="J31" s="349" t="s">
+      <c r="J31" s="348" t="s">
         <v>342</v>
       </c>
       <c r="K31" s="152"/>
@@ -7761,7 +7770,7 @@
       <c r="C32" s="232">
         <v>2016</v>
       </c>
-      <c r="D32" s="264" t="s">
+      <c r="D32" s="263" t="s">
         <v>20</v>
       </c>
       <c r="E32" s="236" t="s">
@@ -7779,10 +7788,10 @@
       <c r="I32" s="106" t="s">
         <v>268</v>
       </c>
-      <c r="J32" s="329" t="s">
+      <c r="J32" s="328" t="s">
         <v>284</v>
       </c>
-      <c r="K32" s="331" t="s">
+      <c r="K32" s="330" t="s">
         <v>292</v>
       </c>
       <c r="L32" s="106" t="s">
@@ -7809,7 +7818,7 @@
       <c r="C33" s="232">
         <v>2018</v>
       </c>
-      <c r="D33" s="264" t="s">
+      <c r="D33" s="263" t="s">
         <v>61</v>
       </c>
       <c r="E33" s="208" t="s">
@@ -7824,21 +7833,21 @@
       <c r="H33" s="137" t="s">
         <v>269</v>
       </c>
-      <c r="I33" s="248" t="s">
+      <c r="I33" s="247" t="s">
         <v>286</v>
       </c>
       <c r="J33" s="106" t="s">
         <v>289</v>
       </c>
-      <c r="K33" s="343" t="s">
+      <c r="K33" s="342" t="s">
         <v>305</v>
       </c>
-      <c r="L33" s="316" t="s">
+      <c r="L33" s="315" t="s">
         <v>330</v>
       </c>
-      <c r="M33" s="349"/>
+      <c r="M33" s="348"/>
       <c r="N33" s="137"/>
-      <c r="O33" s="254"/>
+      <c r="O33" s="253"/>
       <c r="P33" s="106"/>
       <c r="Q33" s="137"/>
       <c r="R33" s="213"/>
@@ -7852,27 +7861,27 @@
       <c r="B34" s="207" t="s">
         <v>184</v>
       </c>
-      <c r="C34" s="250" t="s">
+      <c r="C34" s="249" t="s">
         <v>195</v>
       </c>
-      <c r="D34" s="257" t="s">
+      <c r="D34" s="256" t="s">
         <v>185</v>
       </c>
-      <c r="E34" s="323" t="s">
-        <v>74</v>
-      </c>
-      <c r="F34" s="324" t="s">
+      <c r="E34" s="322" t="s">
+        <v>74</v>
+      </c>
+      <c r="F34" s="323" t="s">
         <v>323</v>
       </c>
       <c r="G34" s="218"/>
-      <c r="H34" s="294" t="s">
+      <c r="H34" s="293" t="s">
         <v>282</v>
       </c>
-      <c r="I34" s="339" t="s">
+      <c r="I34" s="338" t="s">
         <v>324</v>
       </c>
       <c r="J34" s="106"/>
-      <c r="K34" s="249"/>
+      <c r="K34" s="248"/>
       <c r="L34" s="137"/>
       <c r="M34" s="137"/>
       <c r="N34" s="213"/>
@@ -7887,118 +7896,118 @@
       <c r="A35" s="205">
         <v>30</v>
       </c>
-      <c r="B35" s="336" t="s">
+      <c r="B35" s="335" t="s">
         <v>316</v>
       </c>
-      <c r="C35" s="322" t="s">
+      <c r="C35" s="321" t="s">
         <v>280</v>
       </c>
-      <c r="D35" s="327" t="s">
+      <c r="D35" s="326" t="s">
         <v>307</v>
       </c>
-      <c r="E35" s="328" t="s">
+      <c r="E35" s="327" t="s">
         <v>281</v>
       </c>
-      <c r="F35" s="300" t="s">
+      <c r="F35" s="299" t="s">
         <v>309</v>
       </c>
       <c r="G35" s="218"/>
       <c r="H35" s="137" t="s">
         <v>310</v>
       </c>
-      <c r="I35" s="339" t="s">
+      <c r="I35" s="338" t="s">
         <v>328</v>
       </c>
       <c r="J35" s="106"/>
-      <c r="K35" s="249"/>
+      <c r="K35" s="248"/>
       <c r="L35" s="137"/>
-      <c r="M35" s="319"/>
-      <c r="N35" s="320"/>
-      <c r="O35" s="320"/>
-      <c r="P35" s="320"/>
-      <c r="Q35" s="320"/>
-      <c r="R35" s="320"/>
-      <c r="S35" s="320"/>
+      <c r="M35" s="318"/>
+      <c r="N35" s="319"/>
+      <c r="O35" s="319"/>
+      <c r="P35" s="319"/>
+      <c r="Q35" s="319"/>
+      <c r="R35" s="319"/>
+      <c r="S35" s="319"/>
       <c r="T35" s="214"/>
     </row>
     <row r="36" spans="1:20" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="205">
         <v>31</v>
       </c>
-      <c r="B36" s="336" t="s">
+      <c r="B36" s="335" t="s">
         <v>315</v>
       </c>
-      <c r="C36" s="250" t="s">
+      <c r="C36" s="249" t="s">
         <v>280</v>
       </c>
-      <c r="D36" s="327" t="s">
+      <c r="D36" s="326" t="s">
         <v>308</v>
       </c>
-      <c r="E36" s="328" t="s">
+      <c r="E36" s="327" t="s">
         <v>281</v>
       </c>
-      <c r="F36" s="300" t="s">
+      <c r="F36" s="299" t="s">
         <v>55</v>
       </c>
       <c r="G36" s="218"/>
       <c r="H36" s="105" t="s">
         <v>311</v>
       </c>
-      <c r="I36" s="248"/>
+      <c r="I36" s="247"/>
       <c r="J36" s="106"/>
-      <c r="K36" s="249"/>
+      <c r="K36" s="248"/>
       <c r="L36" s="137"/>
-      <c r="M36" s="319"/>
-      <c r="N36" s="320"/>
-      <c r="O36" s="320"/>
-      <c r="P36" s="320"/>
-      <c r="Q36" s="320"/>
-      <c r="R36" s="320"/>
-      <c r="S36" s="320"/>
+      <c r="M36" s="318"/>
+      <c r="N36" s="319"/>
+      <c r="O36" s="319"/>
+      <c r="P36" s="319"/>
+      <c r="Q36" s="319"/>
+      <c r="R36" s="319"/>
+      <c r="S36" s="319"/>
       <c r="T36" s="214"/>
     </row>
     <row r="37" spans="1:20" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="205">
         <v>32</v>
       </c>
-      <c r="B37" s="321" t="s">
+      <c r="B37" s="320" t="s">
         <v>312</v>
       </c>
-      <c r="C37" s="335" t="s">
+      <c r="C37" s="334" t="s">
         <v>314</v>
       </c>
-      <c r="D37" s="333" t="s">
+      <c r="D37" s="332" t="s">
         <v>313</v>
       </c>
-      <c r="E37" s="337" t="s">
+      <c r="E37" s="336" t="s">
         <v>317</v>
       </c>
-      <c r="F37" s="334" t="s">
+      <c r="F37" s="333" t="s">
         <v>26</v>
       </c>
       <c r="G37" s="218"/>
-      <c r="H37" s="349"/>
-      <c r="I37" s="248"/>
+      <c r="H37" s="348"/>
+      <c r="I37" s="247"/>
       <c r="J37" s="106"/>
-      <c r="K37" s="249"/>
+      <c r="K37" s="248"/>
       <c r="L37" s="137"/>
-      <c r="M37" s="319"/>
-      <c r="N37" s="320"/>
-      <c r="O37" s="320"/>
-      <c r="P37" s="320"/>
-      <c r="Q37" s="320"/>
-      <c r="R37" s="320"/>
-      <c r="S37" s="320"/>
+      <c r="M37" s="318"/>
+      <c r="N37" s="319"/>
+      <c r="O37" s="319"/>
+      <c r="P37" s="319"/>
+      <c r="Q37" s="319"/>
+      <c r="R37" s="319"/>
+      <c r="S37" s="319"/>
       <c r="T37" s="214"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A38" s="205"/>
-      <c r="B38" s="251"/>
-      <c r="C38" s="251"/>
-      <c r="D38" s="325"/>
-      <c r="E38" s="252"/>
-      <c r="F38" s="326"/>
-      <c r="G38" s="253"/>
+      <c r="B38" s="250"/>
+      <c r="C38" s="250"/>
+      <c r="D38" s="324"/>
+      <c r="E38" s="251"/>
+      <c r="F38" s="325"/>
+      <c r="G38" s="252"/>
       <c r="H38" s="212"/>
       <c r="I38" s="212"/>
       <c r="J38" s="212"/>
@@ -8024,8 +8033,8 @@
   </sheetPr>
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -8033,11 +8042,11 @@
     <col min="1" max="1" width="5.5703125" style="198" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" style="199" customWidth="1"/>
     <col min="3" max="3" width="15" style="214" customWidth="1"/>
-    <col min="4" max="4" width="16" style="311" customWidth="1"/>
+    <col min="4" max="4" width="16" style="310" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" style="199" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.85546875" style="199" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" style="199" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" style="292" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" style="291" customWidth="1"/>
     <col min="9" max="9" width="21.85546875" style="214" customWidth="1"/>
     <col min="10" max="10" width="23.28515625" style="214" customWidth="1"/>
     <col min="11" max="11" width="18.28515625" style="214" customWidth="1"/>
@@ -8052,24 +8061,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="361" t="s">
+      <c r="B1" s="360" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="361"/>
-      <c r="D1" s="361"/>
-      <c r="E1" s="362"/>
-      <c r="F1" s="361"/>
-      <c r="G1" s="361"/>
+      <c r="C1" s="360"/>
+      <c r="D1" s="360"/>
+      <c r="E1" s="361"/>
+      <c r="F1" s="360"/>
+      <c r="G1" s="360"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
       <c r="B2" s="201" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="293" t="s">
+      <c r="C2" s="292" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="297" t="s">
+      <c r="D2" s="296" t="s">
         <v>49</v>
       </c>
       <c r="E2" s="202" t="s">
@@ -8093,11 +8102,11 @@
       <c r="K2" s="204" t="s">
         <v>64</v>
       </c>
-      <c r="L2" s="255" t="s">
+      <c r="L2" s="254" t="s">
         <v>64</v>
       </c>
-      <c r="M2" s="256"/>
-      <c r="N2" s="256"/>
+      <c r="M2" s="255"/>
+      <c r="N2" s="255"/>
     </row>
     <row r="3" spans="1:19" ht="76.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="205">
@@ -8106,10 +8115,10 @@
       <c r="B3" s="206" t="s">
         <v>255</v>
       </c>
-      <c r="C3" s="298">
+      <c r="C3" s="297">
         <v>2019</v>
       </c>
-      <c r="D3" s="299" t="s">
+      <c r="D3" s="298" t="s">
         <v>256</v>
       </c>
       <c r="E3" s="208" t="s">
@@ -8136,10 +8145,10 @@
       <c r="B4" s="215" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="300">
+      <c r="C4" s="299">
         <v>2012</v>
       </c>
-      <c r="D4" s="301" t="s">
+      <c r="D4" s="300" t="s">
         <v>180</v>
       </c>
       <c r="E4" s="216" t="s">
@@ -8149,7 +8158,7 @@
         <v>28</v>
       </c>
       <c r="G4" s="218"/>
-      <c r="H4" s="295"/>
+      <c r="H4" s="294"/>
       <c r="I4" s="213"/>
       <c r="J4" s="213"/>
       <c r="K4" s="213"/>
@@ -8175,7 +8184,7 @@
         <v>28</v>
       </c>
       <c r="G5" s="218"/>
-      <c r="H5" s="295"/>
+      <c r="H5" s="294"/>
       <c r="I5" s="213"/>
       <c r="J5" s="213"/>
       <c r="K5" s="213"/>
@@ -8188,10 +8197,10 @@
       <c r="B6" s="215" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="300">
+      <c r="C6" s="299">
         <v>2020</v>
       </c>
-      <c r="D6" s="302" t="s">
+      <c r="D6" s="301" t="s">
         <v>236</v>
       </c>
       <c r="E6" s="216" t="s">
@@ -8201,7 +8210,7 @@
         <v>28</v>
       </c>
       <c r="G6" s="218"/>
-      <c r="H6" s="294" t="s">
+      <c r="H6" s="293" t="s">
         <v>261</v>
       </c>
       <c r="I6" s="213"/>
@@ -8216,10 +8225,10 @@
       <c r="B7" s="219" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="303">
+      <c r="C7" s="302">
         <v>2012</v>
       </c>
-      <c r="D7" s="304" t="s">
+      <c r="D7" s="303" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="216" t="s">
@@ -8231,7 +8240,7 @@
       <c r="G7" s="206" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="296"/>
+      <c r="H7" s="295"/>
       <c r="I7" s="137"/>
       <c r="J7" s="221"/>
       <c r="K7" s="213"/>
@@ -8241,13 +8250,13 @@
       <c r="A8" s="205">
         <v>6</v>
       </c>
-      <c r="B8" s="351" t="s">
+      <c r="B8" s="350" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="351">
+      <c r="C8" s="350">
         <v>2020</v>
       </c>
-      <c r="D8" s="352" t="s">
+      <c r="D8" s="351" t="s">
         <v>346</v>
       </c>
       <c r="E8" s="216" t="s">
@@ -8260,7 +8269,7 @@
       <c r="H8" s="106" t="s">
         <v>325</v>
       </c>
-      <c r="I8" s="312" t="s">
+      <c r="I8" s="311" t="s">
         <v>347</v>
       </c>
       <c r="J8" s="221"/>
@@ -8274,22 +8283,22 @@
       <c r="B9" s="222" t="s">
         <v>168</v>
       </c>
-      <c r="C9" s="305">
+      <c r="C9" s="304">
         <v>2011</v>
       </c>
-      <c r="D9" s="306" t="s">
+      <c r="D9" s="305" t="s">
         <v>18</v>
       </c>
       <c r="E9" s="223" t="s">
         <v>73</v>
       </c>
       <c r="F9" s="222" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G9" s="218" t="s">
         <v>77</v>
       </c>
-      <c r="H9" s="353" t="s">
+      <c r="H9" s="352" t="s">
         <v>260</v>
       </c>
       <c r="I9" s="106"/>
@@ -8304,10 +8313,10 @@
       <c r="B10" s="231" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="298">
+      <c r="C10" s="297">
         <v>2018</v>
       </c>
-      <c r="D10" s="308" t="s">
+      <c r="D10" s="307" t="s">
         <v>60</v>
       </c>
       <c r="E10" s="208" t="s">
@@ -8341,10 +8350,10 @@
       <c r="B11" s="231" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="298">
+      <c r="C11" s="297">
         <v>2018</v>
       </c>
-      <c r="D11" s="308" t="s">
+      <c r="D11" s="307" t="s">
         <v>91</v>
       </c>
       <c r="E11" s="208" t="s">
@@ -8356,7 +8365,7 @@
       <c r="G11" s="233" t="s">
         <v>93</v>
       </c>
-      <c r="H11" s="338" t="s">
+      <c r="H11" s="337" t="s">
         <v>320</v>
       </c>
       <c r="I11" s="137"/>
@@ -8378,10 +8387,10 @@
       <c r="B12" s="231" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="298">
+      <c r="C12" s="297">
         <v>2019</v>
       </c>
-      <c r="D12" s="308" t="s">
+      <c r="D12" s="307" t="s">
         <v>129</v>
       </c>
       <c r="E12" s="208" t="s">
@@ -8413,10 +8422,10 @@
       <c r="B13" s="232" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="298">
+      <c r="C13" s="297">
         <v>2015</v>
       </c>
-      <c r="D13" s="308" t="s">
+      <c r="D13" s="307" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="236" t="s">
@@ -8450,11 +8459,11 @@
       <c r="B14" s="232" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="298">
+      <c r="C14" s="297">
         <v>2015</v>
       </c>
-      <c r="D14" s="350" t="s">
-        <v>348</v>
+      <c r="D14" s="349" t="s">
+        <v>352</v>
       </c>
       <c r="E14" s="236" t="s">
         <v>74</v>
@@ -8465,12 +8474,14 @@
       <c r="G14" s="218" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="340" t="s">
+      <c r="H14" s="364" t="s">
         <v>326</v>
       </c>
-      <c r="I14" s="238"/>
-      <c r="J14" s="239"/>
-      <c r="K14" s="291"/>
+      <c r="I14" s="365" t="s">
+        <v>353</v>
+      </c>
+      <c r="J14" s="238"/>
+      <c r="K14" s="290"/>
       <c r="L14" s="106"/>
       <c r="M14" s="99"/>
       <c r="N14" s="137"/>
@@ -8487,16 +8498,16 @@
       <c r="B15" s="232" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="298">
+      <c r="C15" s="297">
         <v>2017</v>
       </c>
-      <c r="D15" s="308" t="s">
+      <c r="D15" s="307" t="s">
         <v>36</v>
       </c>
       <c r="E15" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="354"/>
+      <c r="F15" s="353"/>
       <c r="G15" s="233" t="s">
         <v>82</v>
       </c>
@@ -8522,16 +8533,16 @@
       <c r="B16" s="232" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="298">
+      <c r="C16" s="297">
         <v>2017</v>
       </c>
-      <c r="D16" s="308" t="s">
+      <c r="D16" s="307" t="s">
         <v>38</v>
       </c>
       <c r="E16" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F16" s="240" t="s">
+      <c r="F16" s="239" t="s">
         <v>19</v>
       </c>
       <c r="G16" s="233" t="s">
@@ -8559,22 +8570,22 @@
       <c r="B17" s="232" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="298">
+      <c r="C17" s="297">
         <v>2017</v>
       </c>
-      <c r="D17" s="308" t="s">
+      <c r="D17" s="307" t="s">
         <v>40</v>
       </c>
       <c r="E17" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="241" t="s">
+      <c r="F17" s="240" t="s">
         <v>5</v>
       </c>
       <c r="G17" s="233" t="s">
         <v>79</v>
       </c>
-      <c r="H17" s="344" t="s">
+      <c r="H17" s="343" t="s">
         <v>341</v>
       </c>
       <c r="I17" s="106"/>
@@ -8594,13 +8605,13 @@
       <c r="A18" s="205">
         <v>16</v>
       </c>
-      <c r="B18" s="259" t="s">
+      <c r="B18" s="258" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="298">
+      <c r="C18" s="297">
         <v>2018</v>
       </c>
-      <c r="D18" s="308" t="s">
+      <c r="D18" s="307" t="s">
         <v>54</v>
       </c>
       <c r="E18" s="208" t="s">
@@ -8630,13 +8641,13 @@
       <c r="A19" s="205">
         <v>17</v>
       </c>
-      <c r="B19" s="242" t="s">
+      <c r="B19" s="241" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="309">
+      <c r="C19" s="308">
         <v>2006</v>
       </c>
-      <c r="D19" s="310" t="s">
+      <c r="D19" s="309" t="s">
         <v>16</v>
       </c>
       <c r="E19" s="216" t="s">
@@ -8646,7 +8657,7 @@
         <v>17</v>
       </c>
       <c r="G19" s="218"/>
-      <c r="H19" s="295" t="s">
+      <c r="H19" s="294" t="s">
         <v>259</v>
       </c>
       <c r="I19" s="213"/>
@@ -8669,16 +8680,16 @@
       <c r="B20" s="219" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="303">
+      <c r="C20" s="302">
         <v>2018</v>
       </c>
-      <c r="D20" s="307" t="s">
+      <c r="D20" s="306" t="s">
         <v>58</v>
       </c>
       <c r="E20" s="216" t="s">
         <v>74</v>
       </c>
-      <c r="F20" s="245" t="s">
+      <c r="F20" s="244" t="s">
         <v>199</v>
       </c>
       <c r="G20" s="206" t="s">
@@ -8707,10 +8718,10 @@
       <c r="B21" s="232" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="298">
+      <c r="C21" s="297">
         <v>2015</v>
       </c>
-      <c r="D21" s="308" t="s">
+      <c r="D21" s="307" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="236" t="s">
@@ -8745,26 +8756,26 @@
       <c r="B22" s="232" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="298">
+      <c r="C22" s="297">
         <v>2015</v>
       </c>
-      <c r="D22" s="308" t="s">
+      <c r="D22" s="307" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="356" t="s">
+      <c r="F22" s="355" t="s">
         <v>51</v>
       </c>
       <c r="G22" s="218" t="s">
         <v>86</v>
       </c>
-      <c r="H22" s="329" t="s">
+      <c r="H22" s="328" t="s">
         <v>331</v>
       </c>
-      <c r="I22" s="312" t="s">
-        <v>351</v>
+      <c r="I22" s="311" t="s">
+        <v>350</v>
       </c>
       <c r="J22" s="213"/>
       <c r="K22" s="213"/>
@@ -8785,22 +8796,22 @@
       <c r="B23" s="232" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="298">
+      <c r="C23" s="297">
         <v>2015</v>
       </c>
-      <c r="D23" s="308" t="s">
+      <c r="D23" s="307" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F23" s="245" t="s">
+      <c r="F23" s="244" t="s">
         <v>151</v>
       </c>
       <c r="G23" s="218" t="s">
         <v>85</v>
       </c>
-      <c r="H23" s="355" t="s">
+      <c r="H23" s="354" t="s">
         <v>342</v>
       </c>
       <c r="I23" s="148"/>
@@ -8823,10 +8834,10 @@
       <c r="B24" s="232" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="298">
+      <c r="C24" s="297">
         <v>2016</v>
       </c>
-      <c r="D24" s="308" t="s">
+      <c r="D24" s="307" t="s">
         <v>20</v>
       </c>
       <c r="E24" s="236" t="s">
@@ -8841,8 +8852,8 @@
       <c r="H24" s="106" t="s">
         <v>343</v>
       </c>
-      <c r="I24" s="312" t="s">
-        <v>350</v>
+      <c r="I24" s="311" t="s">
+        <v>349</v>
       </c>
       <c r="J24" s="137"/>
       <c r="K24" s="152"/>
@@ -8863,10 +8874,10 @@
       <c r="B25" s="232" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="298">
+      <c r="C25" s="297">
         <v>2018</v>
       </c>
-      <c r="D25" s="308" t="s">
+      <c r="D25" s="307" t="s">
         <v>61</v>
       </c>
       <c r="E25" s="208" t="s">
@@ -8878,16 +8889,18 @@
       <c r="G25" s="218" t="s">
         <v>94</v>
       </c>
-      <c r="H25" s="316" t="s">
+      <c r="H25" s="328" t="s">
         <v>330</v>
       </c>
-      <c r="I25" s="349"/>
+      <c r="I25" s="311" t="s">
+        <v>351</v>
+      </c>
       <c r="J25" s="106"/>
-      <c r="K25" s="249"/>
+      <c r="K25" s="248"/>
       <c r="L25" s="137"/>
       <c r="M25" s="137"/>
       <c r="N25" s="137"/>
-      <c r="O25" s="254"/>
+      <c r="O25" s="253"/>
       <c r="P25" s="106"/>
       <c r="Q25" s="137"/>
       <c r="R25" s="213"/>
@@ -8901,27 +8914,27 @@
       <c r="B26" s="207" t="s">
         <v>184</v>
       </c>
-      <c r="C26" s="250" t="s">
+      <c r="C26" s="249" t="s">
         <v>195</v>
       </c>
-      <c r="D26" s="257" t="s">
+      <c r="D26" s="256" t="s">
         <v>185</v>
       </c>
-      <c r="E26" s="323" t="s">
-        <v>74</v>
-      </c>
-      <c r="F26" s="324" t="s">
+      <c r="E26" s="322" t="s">
+        <v>74</v>
+      </c>
+      <c r="F26" s="323" t="s">
         <v>323</v>
       </c>
       <c r="G26" s="218"/>
-      <c r="H26" s="294" t="s">
+      <c r="H26" s="293" t="s">
         <v>282</v>
       </c>
-      <c r="I26" s="339" t="s">
+      <c r="I26" s="338" t="s">
         <v>324</v>
       </c>
       <c r="J26" s="106"/>
-      <c r="K26" s="249"/>
+      <c r="K26" s="248"/>
       <c r="L26" s="137"/>
       <c r="M26" s="137"/>
       <c r="N26" s="213"/>
@@ -8936,26 +8949,26 @@
       <c r="A27" s="205">
         <v>25</v>
       </c>
-      <c r="B27" s="336" t="s">
+      <c r="B27" s="335" t="s">
         <v>316</v>
       </c>
-      <c r="C27" s="322" t="s">
+      <c r="C27" s="321" t="s">
         <v>280</v>
       </c>
-      <c r="D27" s="327" t="s">
+      <c r="D27" s="326" t="s">
         <v>307</v>
       </c>
-      <c r="E27" s="328" t="s">
+      <c r="E27" s="327" t="s">
         <v>281</v>
       </c>
-      <c r="F27" s="300" t="s">
+      <c r="F27" s="299" t="s">
         <v>309</v>
       </c>
       <c r="G27" s="218"/>
       <c r="H27" s="137" t="s">
         <v>310</v>
       </c>
-      <c r="I27" s="339" t="s">
+      <c r="I27" s="338" t="s">
         <v>328</v>
       </c>
       <c r="J27" s="213"/>
@@ -8966,49 +8979,49 @@
       <c r="A28" s="205">
         <v>26</v>
       </c>
-      <c r="B28" s="336" t="s">
+      <c r="B28" s="335" t="s">
         <v>315</v>
       </c>
-      <c r="C28" s="250" t="s">
+      <c r="C28" s="249" t="s">
         <v>280</v>
       </c>
-      <c r="D28" s="327" t="s">
+      <c r="D28" s="326" t="s">
         <v>308</v>
       </c>
-      <c r="E28" s="328" t="s">
+      <c r="E28" s="327" t="s">
         <v>281</v>
       </c>
-      <c r="F28" s="300" t="s">
+      <c r="F28" s="299" t="s">
         <v>55</v>
       </c>
       <c r="G28" s="218"/>
       <c r="H28" s="105" t="s">
         <v>311</v>
       </c>
-      <c r="I28" s="248"/>
+      <c r="I28" s="247"/>
     </row>
     <row r="29" spans="1:20" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="205">
         <v>27</v>
       </c>
-      <c r="B29" s="321" t="s">
+      <c r="B29" s="320" t="s">
         <v>312</v>
       </c>
-      <c r="C29" s="335" t="s">
+      <c r="C29" s="334" t="s">
         <v>314</v>
       </c>
-      <c r="D29" s="333" t="s">
+      <c r="D29" s="332" t="s">
         <v>313</v>
       </c>
-      <c r="E29" s="337" t="s">
+      <c r="E29" s="336" t="s">
         <v>317</v>
       </c>
-      <c r="F29" s="334" t="s">
+      <c r="F29" s="333" t="s">
         <v>26</v>
       </c>
       <c r="G29" s="218"/>
-      <c r="H29" s="349"/>
-      <c r="I29" s="248"/>
+      <c r="H29" s="348"/>
+      <c r="I29" s="247"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9048,302 +9061,302 @@
     <col min="2" max="2" width="26.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="277" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="276" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E1" s="290" t="s">
+      <c r="E1" s="289" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="2" spans="2:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="268" t="s">
+      <c r="B2" s="267" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="269" t="s">
+      <c r="C2" s="268" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="270" t="s">
+      <c r="D2" s="269" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="276" t="s">
+      <c r="B3" s="275" t="s">
         <v>249</v>
       </c>
       <c r="C3" s="168" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="282" t="s">
+      <c r="D3" s="281" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="289"/>
+      <c r="E3" s="288"/>
     </row>
     <row r="4" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="271" t="s">
+      <c r="B4" s="270" t="s">
         <v>75</v>
       </c>
       <c r="C4" s="161" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="283" t="s">
+      <c r="D4" s="282" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="289"/>
+      <c r="E4" s="288"/>
     </row>
     <row r="5" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="272" t="s">
+      <c r="B5" s="271" t="s">
         <v>250</v>
       </c>
       <c r="C5" s="161" t="s">
         <v>73</v>
       </c>
-      <c r="D5" s="273" t="s">
+      <c r="D5" s="272" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="289"/>
+      <c r="E5" s="288"/>
     </row>
     <row r="6" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="278" t="s">
+      <c r="B6" s="277" t="s">
         <v>60</v>
       </c>
       <c r="C6" s="157" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="273" t="s">
+      <c r="D6" s="272" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="289"/>
+      <c r="E6" s="288"/>
     </row>
     <row r="7" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="278" t="s">
+      <c r="B7" s="277" t="s">
         <v>91</v>
       </c>
       <c r="C7" s="157" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="273" t="s">
+      <c r="D7" s="272" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="289"/>
+      <c r="E7" s="288"/>
     </row>
     <row r="8" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="278" t="s">
+      <c r="B8" s="277" t="s">
         <v>129</v>
       </c>
       <c r="C8" s="157" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="274" t="s">
+      <c r="D8" s="273" t="s">
         <v>110</v>
       </c>
-      <c r="E8" s="289"/>
+      <c r="E8" s="288"/>
     </row>
     <row r="9" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="278" t="s">
+      <c r="B9" s="277" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="184" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="273" t="s">
+      <c r="D9" s="272" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="289" t="s">
+      <c r="E9" s="288" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="278" t="s">
+      <c r="B10" s="277" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="184" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="273" t="s">
+      <c r="D10" s="272" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="289"/>
+      <c r="E10" s="288"/>
     </row>
     <row r="11" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="278" t="s">
+      <c r="B11" s="277" t="s">
         <v>36</v>
       </c>
       <c r="C11" s="184" t="s">
         <v>74</v>
       </c>
-      <c r="D11" s="273" t="s">
+      <c r="D11" s="272" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="289"/>
+      <c r="E11" s="288"/>
     </row>
     <row r="12" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="278" t="s">
+      <c r="B12" s="277" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="184" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="273" t="s">
+      <c r="D12" s="272" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="289"/>
+      <c r="E12" s="288"/>
     </row>
     <row r="13" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="278" t="s">
+      <c r="B13" s="277" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="184" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="274" t="s">
+      <c r="D13" s="273" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="289"/>
+      <c r="E13" s="288"/>
     </row>
     <row r="14" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="279" t="s">
+      <c r="B14" s="278" t="s">
         <v>251</v>
       </c>
       <c r="C14" s="161" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="284" t="s">
+      <c r="D14" s="283" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="289"/>
+      <c r="E14" s="288"/>
     </row>
     <row r="15" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="280" t="s">
+      <c r="B15" s="279" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="161" t="s">
         <v>74</v>
       </c>
-      <c r="D15" s="284" t="s">
+      <c r="D15" s="283" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="289"/>
+      <c r="E15" s="288"/>
     </row>
     <row r="16" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="281" t="s">
+      <c r="B16" s="280" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="161" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="284" t="s">
+      <c r="D16" s="283" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="289"/>
+      <c r="E16" s="288"/>
     </row>
     <row r="17" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="281" t="s">
+      <c r="B17" s="280" t="s">
         <v>58</v>
       </c>
       <c r="C17" s="161" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="285" t="s">
+      <c r="D17" s="284" t="s">
         <v>199</v>
       </c>
-      <c r="E17" s="289"/>
+      <c r="E17" s="288"/>
     </row>
     <row r="18" spans="2:5" ht="32.450000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="278" t="s">
+      <c r="B18" s="277" t="s">
         <v>2</v>
       </c>
       <c r="C18" s="184" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="286" t="s">
+      <c r="D18" s="285" t="s">
         <v>142</v>
       </c>
-      <c r="E18" s="289"/>
+      <c r="E18" s="288"/>
     </row>
     <row r="19" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="278" t="s">
+      <c r="B19" s="277" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="184" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="273" t="s">
+      <c r="D19" s="272" t="s">
         <v>110</v>
       </c>
-      <c r="E19" s="289"/>
+      <c r="E19" s="288"/>
     </row>
     <row r="20" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="278" t="s">
+      <c r="B20" s="277" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="184" t="s">
         <v>74</v>
       </c>
-      <c r="D20" s="287" t="s">
+      <c r="D20" s="286" t="s">
         <v>110</v>
       </c>
-      <c r="E20" s="289"/>
+      <c r="E20" s="288"/>
     </row>
     <row r="21" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="278" t="s">
+      <c r="B21" s="277" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="184" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="273" t="s">
+      <c r="D21" s="272" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="289"/>
+      <c r="E21" s="288"/>
     </row>
     <row r="22" spans="2:5" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="278" t="s">
+      <c r="B22" s="277" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="184" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="285" t="s">
+      <c r="D22" s="284" t="s">
         <v>151</v>
       </c>
-      <c r="E22" s="289"/>
+      <c r="E22" s="288"/>
     </row>
     <row r="23" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="278" t="s">
+      <c r="B23" s="277" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="184" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="273" t="s">
+      <c r="D23" s="272" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="289"/>
+      <c r="E23" s="288"/>
     </row>
     <row r="24" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="278" t="s">
+      <c r="B24" s="277" t="s">
         <v>61</v>
       </c>
       <c r="C24" s="157" t="s">
         <v>74</v>
       </c>
-      <c r="D24" s="273" t="s">
+      <c r="D24" s="272" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="289"/>
+      <c r="E24" s="288"/>
     </row>
     <row r="25" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="275" t="s">
+      <c r="B25" s="274" t="s">
         <v>185</v>
       </c>
       <c r="C25" s="157" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="288" t="s">
+      <c r="D25" s="287" t="s">
         <v>245</v>
       </c>
-      <c r="E25" s="289"/>
+      <c r="E25" s="288"/>
     </row>
     <row r="26" spans="2:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>

<commit_message>
CIERRE 12 MAY 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
+++ b/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="355">
   <si>
     <t xml:space="preserve">RELACION DE UNIDADES Y ASIGNACION </t>
   </si>
@@ -1137,6 +1137,9 @@
   </si>
   <si>
     <t>26-Abr-22  232,866  KM</t>
+  </si>
+  <si>
+    <t>13 MAYO-2022,.</t>
   </si>
 </sst>
 </file>
@@ -2830,6 +2833,12 @@
     <xf numFmtId="0" fontId="34" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2853,12 +2862,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3734,14 +3737,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="356" t="s">
+      <c r="B1" s="358" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="356"/>
-      <c r="D1" s="356"/>
-      <c r="E1" s="357"/>
-      <c r="F1" s="356"/>
-      <c r="G1" s="356"/>
+      <c r="C1" s="358"/>
+      <c r="D1" s="358"/>
+      <c r="E1" s="359"/>
+      <c r="F1" s="358"/>
+      <c r="G1" s="358"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -4102,10 +4105,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="358" t="s">
+      <c r="L12" s="360" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="359"/>
+      <c r="M12" s="361"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -5300,14 +5303,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="356" t="s">
+      <c r="B1" s="358" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="356"/>
-      <c r="D1" s="356"/>
-      <c r="E1" s="357"/>
-      <c r="F1" s="356"/>
-      <c r="G1" s="356"/>
+      <c r="C1" s="358"/>
+      <c r="D1" s="358"/>
+      <c r="E1" s="359"/>
+      <c r="F1" s="358"/>
+      <c r="G1" s="358"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -5646,10 +5649,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="358" t="s">
+      <c r="L12" s="360" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="359"/>
+      <c r="M12" s="361"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -6626,14 +6629,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="360" t="s">
+      <c r="B1" s="362" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="360"/>
-      <c r="D1" s="360"/>
-      <c r="E1" s="361"/>
-      <c r="F1" s="360"/>
-      <c r="G1" s="360"/>
+      <c r="C1" s="362"/>
+      <c r="D1" s="362"/>
+      <c r="E1" s="363"/>
+      <c r="F1" s="362"/>
+      <c r="G1" s="362"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
@@ -6964,8 +6967,8 @@
       <c r="H12" s="228"/>
       <c r="I12" s="137"/>
       <c r="J12" s="137"/>
-      <c r="K12" s="362"/>
-      <c r="L12" s="363"/>
+      <c r="K12" s="364"/>
+      <c r="L12" s="365"/>
       <c r="M12" s="213"/>
       <c r="N12" s="213"/>
       <c r="O12" s="213"/>
@@ -8033,8 +8036,8 @@
   </sheetPr>
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="C24" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -8061,14 +8064,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="360" t="s">
+      <c r="B1" s="362" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="360"/>
-      <c r="D1" s="360"/>
-      <c r="E1" s="361"/>
-      <c r="F1" s="360"/>
-      <c r="G1" s="360"/>
+      <c r="C1" s="362"/>
+      <c r="D1" s="362"/>
+      <c r="E1" s="363"/>
+      <c r="F1" s="362"/>
+      <c r="G1" s="362"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
@@ -8474,10 +8477,10 @@
       <c r="G14" s="218" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="364" t="s">
+      <c r="H14" s="356" t="s">
         <v>326</v>
       </c>
-      <c r="I14" s="365" t="s">
+      <c r="I14" s="357" t="s">
         <v>353</v>
       </c>
       <c r="J14" s="238"/>
@@ -8933,7 +8936,9 @@
       <c r="I26" s="338" t="s">
         <v>324</v>
       </c>
-      <c r="J26" s="106"/>
+      <c r="J26" s="343" t="s">
+        <v>354</v>
+      </c>
       <c r="K26" s="248"/>
       <c r="L26" s="137"/>
       <c r="M26" s="137"/>

</xml_diff>

<commit_message>
cierre 4 julio 2022
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
+++ b/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="368">
   <si>
     <t xml:space="preserve">RELACION DE UNIDADES Y ASIGNACION </t>
   </si>
@@ -1146,6 +1146,39 @@
   </si>
   <si>
     <t>SM-56393---SP-13163</t>
+  </si>
+  <si>
+    <t>28-Jun-22   170,444  KM</t>
+  </si>
+  <si>
+    <t>6-Jun-22    117,634   KM</t>
+  </si>
+  <si>
+    <t>8-Mar-22    143,786 KM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 MAR-2022    156,877  KM </t>
+  </si>
+  <si>
+    <t>SM 47367--SP-13263</t>
+  </si>
+  <si>
+    <t>SM 46572--SP-13221</t>
+  </si>
+  <si>
+    <t>SL 78535--SP-13267</t>
+  </si>
+  <si>
+    <t>7-Jun-22     276,616 KM</t>
+  </si>
+  <si>
+    <t>3-May-22     162,113 KM</t>
+  </si>
+  <si>
+    <t>8-MAR-2022  68,924 KM</t>
+  </si>
+  <si>
+    <t>21-Jun-22       296,521 KM</t>
   </si>
 </sst>
 </file>
@@ -1846,7 +1879,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="366">
+  <cellXfs count="367">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2833,9 +2866,6 @@
     <xf numFmtId="0" fontId="34" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="34" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2843,6 +2873,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3491,6 +3527,138 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Conector recto 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2847975" y="21516975"/>
+          <a:ext cx="1133475" cy="142875"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>361950</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Conector recto 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2781300" y="10896600"/>
+          <a:ext cx="1304925" cy="47625"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Conector recto 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2819400" y="12849225"/>
+          <a:ext cx="1133475" cy="66675"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3787,14 +3955,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="358" t="s">
+      <c r="B1" s="359" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="358"/>
-      <c r="D1" s="358"/>
-      <c r="E1" s="359"/>
-      <c r="F1" s="358"/>
-      <c r="G1" s="358"/>
+      <c r="C1" s="359"/>
+      <c r="D1" s="359"/>
+      <c r="E1" s="360"/>
+      <c r="F1" s="359"/>
+      <c r="G1" s="359"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -4155,10 +4323,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="360" t="s">
+      <c r="L12" s="361" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="361"/>
+      <c r="M12" s="362"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -5353,14 +5521,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="358" t="s">
+      <c r="B1" s="359" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="358"/>
-      <c r="D1" s="358"/>
-      <c r="E1" s="359"/>
-      <c r="F1" s="358"/>
-      <c r="G1" s="358"/>
+      <c r="C1" s="359"/>
+      <c r="D1" s="359"/>
+      <c r="E1" s="360"/>
+      <c r="F1" s="359"/>
+      <c r="G1" s="359"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -5699,10 +5867,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="360" t="s">
+      <c r="L12" s="361" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="361"/>
+      <c r="M12" s="362"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -6679,14 +6847,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="362" t="s">
+      <c r="B1" s="363" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="362"/>
-      <c r="D1" s="362"/>
-      <c r="E1" s="363"/>
-      <c r="F1" s="362"/>
-      <c r="G1" s="362"/>
+      <c r="C1" s="363"/>
+      <c r="D1" s="363"/>
+      <c r="E1" s="364"/>
+      <c r="F1" s="363"/>
+      <c r="G1" s="363"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
@@ -7017,8 +7185,8 @@
       <c r="H12" s="228"/>
       <c r="I12" s="137"/>
       <c r="J12" s="137"/>
-      <c r="K12" s="364"/>
-      <c r="L12" s="365"/>
+      <c r="K12" s="365"/>
+      <c r="L12" s="366"/>
       <c r="M12" s="213"/>
       <c r="N12" s="213"/>
       <c r="O12" s="213"/>
@@ -8086,8 +8254,8 @@
   </sheetPr>
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -8114,14 +8282,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="362" t="s">
+      <c r="B1" s="363" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="362"/>
-      <c r="D1" s="362"/>
-      <c r="E1" s="363"/>
-      <c r="F1" s="362"/>
-      <c r="G1" s="362"/>
+      <c r="C1" s="363"/>
+      <c r="D1" s="363"/>
+      <c r="E1" s="364"/>
+      <c r="F1" s="363"/>
+      <c r="G1" s="363"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
@@ -8384,10 +8552,12 @@
       <c r="H10" s="106" t="s">
         <v>337</v>
       </c>
-      <c r="I10" s="315" t="s">
+      <c r="I10" s="357" t="s">
         <v>355</v>
       </c>
-      <c r="J10" s="106"/>
+      <c r="J10" s="100" t="s">
+        <v>358</v>
+      </c>
       <c r="K10" s="106"/>
       <c r="L10" s="213"/>
       <c r="M10" s="212"/>
@@ -8420,10 +8590,12 @@
       <c r="G11" s="233" t="s">
         <v>93</v>
       </c>
-      <c r="H11" s="337" t="s">
+      <c r="H11" s="358" t="s">
         <v>320</v>
       </c>
-      <c r="I11" s="137"/>
+      <c r="I11" s="311" t="s">
+        <v>359</v>
+      </c>
       <c r="J11" s="106"/>
       <c r="K11" s="234"/>
       <c r="L11" s="106"/>
@@ -8480,8 +8652,8 @@
       <c r="C13" s="297">
         <v>2015</v>
       </c>
-      <c r="D13" s="307" t="s">
-        <v>12</v>
+      <c r="D13" s="301" t="s">
+        <v>362</v>
       </c>
       <c r="E13" s="236" t="s">
         <v>74</v>
@@ -8529,10 +8701,10 @@
       <c r="G14" s="218" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="356" t="s">
+      <c r="H14" s="355" t="s">
         <v>326</v>
       </c>
-      <c r="I14" s="357" t="s">
+      <c r="I14" s="356" t="s">
         <v>353</v>
       </c>
       <c r="J14" s="238"/>
@@ -8556,8 +8728,8 @@
       <c r="C15" s="297">
         <v>2017</v>
       </c>
-      <c r="D15" s="307" t="s">
-        <v>36</v>
+      <c r="D15" s="301" t="s">
+        <v>363</v>
       </c>
       <c r="E15" s="236" t="s">
         <v>74</v>
@@ -8566,10 +8738,12 @@
       <c r="G15" s="233" t="s">
         <v>82</v>
       </c>
-      <c r="H15" s="105" t="s">
+      <c r="H15" s="137" t="s">
         <v>333</v>
       </c>
-      <c r="I15" s="137"/>
+      <c r="I15" s="311" t="s">
+        <v>364</v>
+      </c>
       <c r="J15" s="137"/>
       <c r="K15" s="106"/>
       <c r="L15" s="137"/>
@@ -8603,10 +8777,12 @@
       <c r="G16" s="233" t="s">
         <v>83</v>
       </c>
-      <c r="H16" s="100" t="s">
+      <c r="H16" s="106" t="s">
         <v>329</v>
       </c>
-      <c r="I16" s="137"/>
+      <c r="I16" s="311" t="s">
+        <v>365</v>
+      </c>
       <c r="J16" s="99"/>
       <c r="K16" s="106"/>
       <c r="L16" s="137"/>
@@ -8640,8 +8816,8 @@
       <c r="G17" s="233" t="s">
         <v>79</v>
       </c>
-      <c r="H17" s="343" t="s">
-        <v>341</v>
+      <c r="H17" s="100" t="s">
+        <v>366</v>
       </c>
       <c r="I17" s="106"/>
       <c r="J17" s="106"/>
@@ -8750,7 +8926,7 @@
       <c r="G20" s="206" t="s">
         <v>95</v>
       </c>
-      <c r="H20" s="105" t="s">
+      <c r="H20" s="315" t="s">
         <v>338</v>
       </c>
       <c r="I20" s="137"/>
@@ -8788,7 +8964,7 @@
       <c r="G21" s="218" t="s">
         <v>70</v>
       </c>
-      <c r="H21" s="100" t="s">
+      <c r="H21" s="97" t="s">
         <v>334</v>
       </c>
       <c r="I21" s="137"/>
@@ -8820,7 +8996,7 @@
       <c r="E22" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="355" t="s">
+      <c r="F22" s="354" t="s">
         <v>51</v>
       </c>
       <c r="G22" s="218" t="s">
@@ -8866,8 +9042,8 @@
       <c r="G23" s="218" t="s">
         <v>85</v>
       </c>
-      <c r="H23" s="354" t="s">
-        <v>342</v>
+      <c r="H23" s="311" t="s">
+        <v>360</v>
       </c>
       <c r="I23" s="148"/>
       <c r="J23" s="137"/>
@@ -8892,8 +9068,8 @@
       <c r="C24" s="297">
         <v>2016</v>
       </c>
-      <c r="D24" s="307" t="s">
-        <v>20</v>
+      <c r="D24" s="301" t="s">
+        <v>361</v>
       </c>
       <c r="E24" s="236" t="s">
         <v>74</v>
@@ -8907,10 +9083,12 @@
       <c r="H24" s="106" t="s">
         <v>343</v>
       </c>
-      <c r="I24" s="311" t="s">
+      <c r="I24" s="293" t="s">
         <v>349</v>
       </c>
-      <c r="J24" s="137"/>
+      <c r="J24" s="311" t="s">
+        <v>367</v>
+      </c>
       <c r="K24" s="152"/>
       <c r="L24" s="106"/>
       <c r="M24" s="106"/>
@@ -8947,10 +9125,12 @@
       <c r="H25" s="328" t="s">
         <v>330</v>
       </c>
-      <c r="I25" s="311" t="s">
+      <c r="I25" s="293" t="s">
         <v>351</v>
       </c>
-      <c r="J25" s="106"/>
+      <c r="J25" s="311" t="s">
+        <v>357</v>
+      </c>
       <c r="K25" s="248"/>
       <c r="L25" s="137"/>
       <c r="M25" s="137"/>

</xml_diff>

<commit_message>
CIERRE 15 AGO 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
+++ b/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="370">
   <si>
     <t xml:space="preserve">RELACION DE UNIDADES Y ASIGNACION </t>
   </si>
@@ -1179,6 +1179,12 @@
   </si>
   <si>
     <t>21-Jun-22       296,521 KM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>28-Jul-22    232,099   KM</t>
   </si>
 </sst>
 </file>
@@ -8254,8 +8260,8 @@
   </sheetPr>
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -8593,10 +8599,12 @@
       <c r="H11" s="358" t="s">
         <v>320</v>
       </c>
-      <c r="I11" s="311" t="s">
+      <c r="I11" s="293" t="s">
         <v>359</v>
       </c>
-      <c r="J11" s="106"/>
+      <c r="J11" s="100" t="s">
+        <v>368</v>
+      </c>
       <c r="K11" s="234"/>
       <c r="L11" s="106"/>
       <c r="M11" s="106"/>
@@ -8664,10 +8672,12 @@
       <c r="G13" s="218" t="s">
         <v>84</v>
       </c>
-      <c r="H13" s="100" t="s">
+      <c r="H13" s="106" t="s">
         <v>339</v>
       </c>
-      <c r="I13" s="106"/>
+      <c r="I13" s="311" t="s">
+        <v>369</v>
+      </c>
       <c r="J13" s="137"/>
       <c r="K13" s="137"/>
       <c r="L13" s="106"/>

</xml_diff>

<commit_message>
CIERRE  5 SEPT 2022
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
+++ b/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
@@ -17,7 +17,7 @@
     <sheet name="A Ñ O      2 0 2 1      " sheetId="4" state="hidden" r:id="rId3"/>
     <sheet name="    A Ñ O       2 0 2 2       " sheetId="7" r:id="rId4"/>
     <sheet name="Hoja1" sheetId="5" r:id="rId5"/>
-    <sheet name="Hoja4" sheetId="6" r:id="rId6"/>
+    <sheet name="ASIGNACIONES DE CAMIONETAS 2022" sheetId="6" r:id="rId6"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="457">
   <si>
     <t xml:space="preserve">RELACION DE UNIDADES Y ASIGNACION </t>
   </si>
@@ -821,27 +821,12 @@
     <t>9 ENE-2021   48,264 KM</t>
   </si>
   <si>
-    <t>TALLER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KENWORTH   </t>
-  </si>
-  <si>
-    <t>58-AN-4L  Tracto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Kodiak    SL 53584</t>
-  </si>
-  <si>
     <t>19-Ene-2021   105,301  KM</t>
   </si>
   <si>
     <t>26-Ene-21  203,077 KM</t>
   </si>
   <si>
-    <t>SEMANA # 7</t>
-  </si>
-  <si>
     <t>RANGER ROVER</t>
   </si>
   <si>
@@ -1194,6 +1179,273 @@
   </si>
   <si>
     <t>3-AGO--22     12,985  KM</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>N°</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDAD </t>
+  </si>
+  <si>
+    <t>MODELO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLACAS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N° DE SERIE </t>
+  </si>
+  <si>
+    <t>ASIGNACION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAM </t>
+  </si>
+  <si>
+    <t>9BD265559J9096358</t>
+  </si>
+  <si>
+    <t>PABLO  OSIRIS</t>
+  </si>
+  <si>
+    <t>SP 13163</t>
+  </si>
+  <si>
+    <t>9BD265557J9102609</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAUL </t>
+  </si>
+  <si>
+    <t>SP 13215</t>
+  </si>
+  <si>
+    <t>9BD265557K9120898</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JESUS </t>
+  </si>
+  <si>
+    <t>3N6AD35C0JK886728</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRISTOBAL </t>
+  </si>
+  <si>
+    <t>3N6AD35C8GK832196</t>
+  </si>
+  <si>
+    <t>3N6DD25X1FK071438</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 SUR </t>
+  </si>
+  <si>
+    <t>3N6DD25X3FK071733</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIGUEL </t>
+  </si>
+  <si>
+    <t>3N6DD25X3FK071571</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALENTE </t>
+  </si>
+  <si>
+    <t>TOYOTA 1</t>
+  </si>
+  <si>
+    <t>SP 13165</t>
+  </si>
+  <si>
+    <t>MR0CX8CB5N0426604</t>
+  </si>
+  <si>
+    <t>TOYOTA 2</t>
+  </si>
+  <si>
+    <t>SP 13166</t>
+  </si>
+  <si>
+    <t>MR0CX8CB1N0426762</t>
+  </si>
+  <si>
+    <t>TOYOTA 3</t>
+  </si>
+  <si>
+    <t>SP 41023</t>
+  </si>
+  <si>
+    <t>MR0CX8CB0N0427790</t>
+  </si>
+  <si>
+    <t>SP 13221</t>
+  </si>
+  <si>
+    <t>1FDEF3G6XFEC48778</t>
+  </si>
+  <si>
+    <t>SN 81676</t>
+  </si>
+  <si>
+    <t>1FDEF3G65FEC06776</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GONZALO </t>
+  </si>
+  <si>
+    <t>1FDWF3G63HEB43877</t>
+  </si>
+  <si>
+    <t>FORD 4</t>
+  </si>
+  <si>
+    <t>SL78539</t>
+  </si>
+  <si>
+    <t>1FDWF3G67HEB43803</t>
+  </si>
+  <si>
+    <t>FORD 5</t>
+  </si>
+  <si>
+    <t>1FDWF3G67HEC27443</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TORNADO </t>
+  </si>
+  <si>
+    <t>SN 79093</t>
+  </si>
+  <si>
+    <t>LZWNNNGM7NC829681</t>
+  </si>
+  <si>
+    <t>SP 41040</t>
+  </si>
+  <si>
+    <t>3N6AD35A7NK819032</t>
+  </si>
+  <si>
+    <t>3GBM7H1C66M100053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KENWORTH </t>
+  </si>
+  <si>
+    <t>01AP3G</t>
+  </si>
+  <si>
+    <t>3BKHHM8XXBF377174</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> VERSA </t>
+  </si>
+  <si>
+    <t>TRA 959A</t>
+  </si>
+  <si>
+    <t>3N1CNBAE1LL845649</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVEO </t>
+  </si>
+  <si>
+    <t>TUK 059A</t>
+  </si>
+  <si>
+    <t>LSGHD52H4MD124508</t>
+  </si>
+  <si>
+    <t>TUK 062A</t>
+  </si>
+  <si>
+    <t>LSGHD52H5MD124498</t>
+  </si>
+  <si>
+    <t>ARDRIANA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWE 080A </t>
+  </si>
+  <si>
+    <t>LSGHD52H2ND018673</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MARCH </t>
+  </si>
+  <si>
+    <t>3N1CK3CD9JL250996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEOPOLDO        </t>
+  </si>
+  <si>
+    <t>58AN4L</t>
+  </si>
+  <si>
+    <t>3WKYD40X3MF517376</t>
+  </si>
+  <si>
+    <t>ARTURO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPERBUS </t>
+  </si>
+  <si>
+    <t>12UD6W</t>
+  </si>
+  <si>
+    <t>3PBB3Z621C1002716</t>
+  </si>
+  <si>
+    <t>CAJA UTILITY</t>
+  </si>
+  <si>
+    <t>74UD6V</t>
+  </si>
+  <si>
+    <t>1UYVS2535AM933905</t>
+  </si>
+  <si>
+    <t>1C4PJLAKXCW159476</t>
+  </si>
+  <si>
+    <t>TPM 596A</t>
+  </si>
+  <si>
+    <t>1GNSK8KC6LR116593</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRIS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JEEP SAHARA </t>
+  </si>
+  <si>
+    <t>1C4HJXEG4JW104892</t>
+  </si>
+  <si>
+    <t>RANGE ROVER</t>
+  </si>
+  <si>
+    <t>TRK 613A</t>
+  </si>
+  <si>
+    <t>SALYA2BX6KA791646</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BMW </t>
+  </si>
+  <si>
+    <t>TVJ 884C</t>
+  </si>
+  <si>
+    <t>XXX</t>
   </si>
 </sst>
 </file>
@@ -1204,7 +1456,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="[$-C0A]dd\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="44" x14ac:knownFonts="1">
+  <fonts count="50" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1503,20 +1755,68 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="24">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1651,8 +1951,16 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="darkVertical">
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkVertical"/>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1857,19 +2165,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -1905,11 +2200,109 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="369">
+  <cellXfs count="397">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2641,75 +3034,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2786,7 +3110,7 @@
     <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2802,10 +3126,10 @@
     <xf numFmtId="17" fontId="39" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2914,7 +3238,7 @@
     <xf numFmtId="16" fontId="12" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2940,6 +3264,155 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3698,6 +4171,118 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>238120</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3276601" cy="542925"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectángulo 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3B0F336-E664-40BC-90CE-6301DEEEE411}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1857370" y="0"/>
+          <a:ext cx="3276601" cy="542925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="3000" b="1" cap="none" spc="0">
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="12700" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>RELACION</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES" sz="3000" b="1" cap="none" spc="0" baseline="0">
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="12700" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> VEHICULOS 2022</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-ES" sz="3000" b="1" cap="none" spc="0">
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="12700" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -3991,14 +4576,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="361" t="s">
+      <c r="B1" s="338" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="361"/>
-      <c r="D1" s="361"/>
-      <c r="E1" s="362"/>
-      <c r="F1" s="361"/>
-      <c r="G1" s="361"/>
+      <c r="C1" s="338"/>
+      <c r="D1" s="338"/>
+      <c r="E1" s="339"/>
+      <c r="F1" s="338"/>
+      <c r="G1" s="338"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -4359,10 +4944,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="363" t="s">
+      <c r="L12" s="340" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="364"/>
+      <c r="M12" s="341"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -5557,14 +6142,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="361" t="s">
+      <c r="B1" s="338" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="361"/>
-      <c r="D1" s="361"/>
-      <c r="E1" s="362"/>
-      <c r="F1" s="361"/>
-      <c r="G1" s="361"/>
+      <c r="C1" s="338"/>
+      <c r="D1" s="338"/>
+      <c r="E1" s="339"/>
+      <c r="F1" s="338"/>
+      <c r="G1" s="338"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -5903,10 +6488,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="363" t="s">
+      <c r="L12" s="340" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="364"/>
+      <c r="M12" s="341"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -6883,14 +7468,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="365" t="s">
+      <c r="B1" s="342" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="365"/>
-      <c r="D1" s="365"/>
-      <c r="E1" s="366"/>
-      <c r="F1" s="365"/>
-      <c r="G1" s="365"/>
+      <c r="C1" s="342"/>
+      <c r="D1" s="342"/>
+      <c r="E1" s="343"/>
+      <c r="F1" s="342"/>
+      <c r="G1" s="342"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
@@ -6971,13 +7556,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="206" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C4" s="207">
         <v>2019</v>
       </c>
-      <c r="D4" s="314" t="s">
-        <v>256</v>
+      <c r="D4" s="291" t="s">
+        <v>251</v>
       </c>
       <c r="E4" s="208" t="s">
         <v>74</v>
@@ -6987,7 +7572,7 @@
       </c>
       <c r="G4" s="51"/>
       <c r="H4" s="100" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="I4" s="106"/>
       <c r="J4" s="106"/>
@@ -7114,7 +7699,7 @@
       <c r="C9" s="219">
         <v>2017</v>
       </c>
-      <c r="D9" s="313" t="s">
+      <c r="D9" s="290" t="s">
         <v>44</v>
       </c>
       <c r="E9" s="216" t="s">
@@ -7163,14 +7748,14 @@
       <c r="A11" s="205">
         <v>8</v>
       </c>
-      <c r="B11" s="350" t="s">
+      <c r="B11" s="327" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="350">
+      <c r="C11" s="327">
         <v>2020</v>
       </c>
-      <c r="D11" s="351" t="s">
-        <v>346</v>
+      <c r="D11" s="328" t="s">
+        <v>341</v>
       </c>
       <c r="E11" s="216" t="s">
         <v>73</v>
@@ -7180,10 +7765,10 @@
       </c>
       <c r="G11" s="224"/>
       <c r="H11" s="106" t="s">
-        <v>325</v>
-      </c>
-      <c r="I11" s="311" t="s">
-        <v>347</v>
+        <v>320</v>
+      </c>
+      <c r="I11" s="288" t="s">
+        <v>342</v>
       </c>
       <c r="J11" s="212"/>
       <c r="K11" s="212"/>
@@ -7221,8 +7806,8 @@
       <c r="H12" s="228"/>
       <c r="I12" s="137"/>
       <c r="J12" s="137"/>
-      <c r="K12" s="367"/>
-      <c r="L12" s="368"/>
+      <c r="K12" s="344"/>
+      <c r="L12" s="345"/>
       <c r="M12" s="213"/>
       <c r="N12" s="213"/>
       <c r="O12" s="213"/>
@@ -7252,7 +7837,7 @@
       </c>
       <c r="G13" s="218"/>
       <c r="H13" s="100" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="I13" s="137"/>
       <c r="J13" s="137"/>
@@ -7289,18 +7874,18 @@
         <v>94</v>
       </c>
       <c r="H14" s="137" t="s">
-        <v>270</v>
-      </c>
-      <c r="I14" s="293" t="s">
-        <v>293</v>
+        <v>265</v>
+      </c>
+      <c r="I14" s="270" t="s">
+        <v>288</v>
       </c>
       <c r="J14" s="106" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="K14" s="100" t="s">
-        <v>337</v>
-      </c>
-      <c r="L14" s="344"/>
+        <v>332</v>
+      </c>
+      <c r="L14" s="321"/>
       <c r="M14" s="212"/>
       <c r="N14" s="212"/>
       <c r="O14" s="212"/>
@@ -7332,18 +7917,18 @@
         <v>93</v>
       </c>
       <c r="H15" s="137" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="I15" s="137" t="s">
-        <v>285</v>
-      </c>
-      <c r="J15" s="293" t="s">
-        <v>294</v>
-      </c>
-      <c r="K15" s="337" t="s">
-        <v>320</v>
-      </c>
-      <c r="L15" s="343"/>
+        <v>280</v>
+      </c>
+      <c r="J15" s="270" t="s">
+        <v>289</v>
+      </c>
+      <c r="K15" s="314" t="s">
+        <v>315</v>
+      </c>
+      <c r="L15" s="320"/>
       <c r="M15" s="106"/>
       <c r="N15" s="106"/>
       <c r="O15" s="212"/>
@@ -7373,15 +7958,15 @@
       </c>
       <c r="G16" s="233"/>
       <c r="H16" s="106" t="s">
-        <v>273</v>
-      </c>
-      <c r="I16" s="293" t="s">
-        <v>301</v>
+        <v>268</v>
+      </c>
+      <c r="I16" s="270" t="s">
+        <v>296</v>
       </c>
       <c r="J16" s="105" t="s">
-        <v>336</v>
-      </c>
-      <c r="K16" s="344"/>
+        <v>331</v>
+      </c>
+      <c r="K16" s="321"/>
       <c r="L16" s="212"/>
       <c r="M16" s="212"/>
       <c r="N16" s="212"/>
@@ -7414,19 +7999,19 @@
         <v>84</v>
       </c>
       <c r="H17" s="137" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="I17" s="106" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="J17" s="106" t="s">
-        <v>291</v>
-      </c>
-      <c r="K17" s="328" t="s">
-        <v>322</v>
+        <v>286</v>
+      </c>
+      <c r="K17" s="305" t="s">
+        <v>317</v>
       </c>
       <c r="L17" s="100" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="M17" s="137"/>
       <c r="N17" s="237"/>
@@ -7446,8 +8031,8 @@
       <c r="C18" s="232">
         <v>2015</v>
       </c>
-      <c r="D18" s="349" t="s">
-        <v>344</v>
+      <c r="D18" s="326" t="s">
+        <v>339</v>
       </c>
       <c r="E18" s="236" t="s">
         <v>74</v>
@@ -7459,15 +8044,15 @@
         <v>71</v>
       </c>
       <c r="H18" s="106" t="s">
-        <v>274</v>
-      </c>
-      <c r="I18" s="340" t="s">
-        <v>327</v>
-      </c>
-      <c r="J18" s="339" t="s">
-        <v>326</v>
-      </c>
-      <c r="K18" s="345"/>
+        <v>269</v>
+      </c>
+      <c r="I18" s="317" t="s">
+        <v>322</v>
+      </c>
+      <c r="J18" s="316" t="s">
+        <v>321</v>
+      </c>
+      <c r="K18" s="322"/>
       <c r="L18" s="106"/>
       <c r="M18" s="99"/>
       <c r="N18" s="137"/>
@@ -7499,23 +8084,23 @@
       <c r="G19" s="233" t="s">
         <v>82</v>
       </c>
-      <c r="H19" s="293" t="s">
-        <v>257</v>
-      </c>
-      <c r="I19" s="328" t="s">
-        <v>267</v>
-      </c>
-      <c r="J19" s="328" t="s">
-        <v>288</v>
+      <c r="H19" s="270" t="s">
+        <v>252</v>
+      </c>
+      <c r="I19" s="305" t="s">
+        <v>262</v>
+      </c>
+      <c r="J19" s="305" t="s">
+        <v>283</v>
       </c>
       <c r="K19" s="106" t="s">
-        <v>290</v>
-      </c>
-      <c r="L19" s="328" t="s">
-        <v>318</v>
+        <v>285</v>
+      </c>
+      <c r="L19" s="305" t="s">
+        <v>313</v>
       </c>
       <c r="M19" s="105" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="N19" s="137"/>
       <c r="O19" s="106"/>
@@ -7546,19 +8131,19 @@
       <c r="G20" s="233" t="s">
         <v>83</v>
       </c>
-      <c r="H20" s="328" t="s">
-        <v>275</v>
-      </c>
-      <c r="I20" s="328" t="s">
-        <v>283</v>
-      </c>
-      <c r="J20" s="341" t="s">
-        <v>300</v>
+      <c r="H20" s="305" t="s">
+        <v>270</v>
+      </c>
+      <c r="I20" s="305" t="s">
+        <v>278</v>
+      </c>
+      <c r="J20" s="318" t="s">
+        <v>295</v>
       </c>
       <c r="K20" s="100" t="s">
-        <v>329</v>
-      </c>
-      <c r="L20" s="346"/>
+        <v>324</v>
+      </c>
+      <c r="L20" s="323"/>
       <c r="M20" s="213"/>
       <c r="N20" s="213"/>
       <c r="O20" s="137"/>
@@ -7589,14 +8174,14 @@
       <c r="G21" s="233" t="s">
         <v>79</v>
       </c>
-      <c r="H21" s="328" t="s">
-        <v>266</v>
-      </c>
-      <c r="I21" s="311" t="s">
-        <v>303</v>
+      <c r="H21" s="305" t="s">
+        <v>261</v>
+      </c>
+      <c r="I21" s="288" t="s">
+        <v>298</v>
       </c>
       <c r="J21" s="100" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="K21" s="213"/>
       <c r="L21" s="213"/>
@@ -7619,7 +8204,7 @@
       <c r="C22" s="232">
         <v>2018</v>
       </c>
-      <c r="D22" s="312" t="s">
+      <c r="D22" s="289" t="s">
         <v>54</v>
       </c>
       <c r="E22" s="208" t="s">
@@ -7629,11 +8214,11 @@
         <v>27</v>
       </c>
       <c r="G22" s="224"/>
-      <c r="H22" s="328" t="s">
-        <v>264</v>
+      <c r="H22" s="305" t="s">
+        <v>259</v>
       </c>
       <c r="I22" s="105" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="J22" s="137"/>
       <c r="K22" s="213"/>
@@ -7703,8 +8288,8 @@
       <c r="G24" s="243" t="s">
         <v>80</v>
       </c>
-      <c r="H24" s="317" t="s">
-        <v>279</v>
+      <c r="H24" s="294" t="s">
+        <v>274</v>
       </c>
       <c r="I24" s="137"/>
       <c r="J24" s="137"/>
@@ -7741,8 +8326,8 @@
       <c r="G25" s="206" t="s">
         <v>78</v>
       </c>
-      <c r="H25" s="316" t="s">
-        <v>278</v>
+      <c r="H25" s="293" t="s">
+        <v>273</v>
       </c>
       <c r="I25" s="137"/>
       <c r="J25" s="137"/>
@@ -7767,7 +8352,7 @@
       <c r="C26" s="219">
         <v>2018</v>
       </c>
-      <c r="D26" s="313" t="s">
+      <c r="D26" s="290" t="s">
         <v>58</v>
       </c>
       <c r="E26" s="216" t="s">
@@ -7782,13 +8367,13 @@
       <c r="H26" s="106" t="s">
         <v>247</v>
       </c>
-      <c r="I26" s="293" t="s">
-        <v>299</v>
+      <c r="I26" s="270" t="s">
+        <v>294</v>
       </c>
       <c r="J26" s="105" t="s">
-        <v>338</v>
-      </c>
-      <c r="K26" s="344"/>
+        <v>333</v>
+      </c>
+      <c r="K26" s="321"/>
       <c r="L26" s="213"/>
       <c r="M26" s="213"/>
       <c r="N26" s="213"/>
@@ -7822,13 +8407,13 @@
         <v>69</v>
       </c>
       <c r="H27" s="106" t="s">
-        <v>271</v>
-      </c>
-      <c r="I27" s="331" t="s">
-        <v>306</v>
-      </c>
-      <c r="J27" s="347" t="s">
-        <v>340</v>
+        <v>266</v>
+      </c>
+      <c r="I27" s="308" t="s">
+        <v>301</v>
+      </c>
+      <c r="J27" s="324" t="s">
+        <v>335</v>
       </c>
       <c r="K27" s="221"/>
       <c r="L27" s="137"/>
@@ -7863,16 +8448,16 @@
       <c r="G28" s="218" t="s">
         <v>70</v>
       </c>
-      <c r="H28" s="293" t="s">
-        <v>263</v>
+      <c r="H28" s="270" t="s">
+        <v>258</v>
       </c>
       <c r="I28" s="137" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="J28" s="100" t="s">
-        <v>334</v>
-      </c>
-      <c r="K28" s="346"/>
+        <v>329</v>
+      </c>
+      <c r="K28" s="323"/>
       <c r="L28" s="106"/>
       <c r="M28" s="137"/>
       <c r="N28" s="137"/>
@@ -7906,15 +8491,15 @@
         <v>86</v>
       </c>
       <c r="H29" s="137" t="s">
-        <v>262</v>
-      </c>
-      <c r="I29" s="293" t="s">
-        <v>296</v>
+        <v>257</v>
+      </c>
+      <c r="I29" s="270" t="s">
+        <v>291</v>
       </c>
       <c r="J29" s="105" t="s">
-        <v>331</v>
-      </c>
-      <c r="K29" s="344"/>
+        <v>326</v>
+      </c>
+      <c r="K29" s="321"/>
       <c r="L29" s="137"/>
       <c r="M29" s="137"/>
       <c r="N29" s="99"/>
@@ -7948,25 +8533,25 @@
         <v>67</v>
       </c>
       <c r="H30" s="137" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="I30" s="152" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="J30" s="137" t="s">
-        <v>287</v>
-      </c>
-      <c r="K30" s="328" t="s">
-        <v>297</v>
-      </c>
-      <c r="L30" s="293" t="s">
-        <v>321</v>
+        <v>282</v>
+      </c>
+      <c r="K30" s="305" t="s">
+        <v>292</v>
+      </c>
+      <c r="L30" s="270" t="s">
+        <v>316</v>
       </c>
       <c r="M30" s="137" t="s">
-        <v>332</v>
-      </c>
-      <c r="N30" s="347" t="s">
-        <v>335</v>
+        <v>327</v>
+      </c>
+      <c r="N30" s="324" t="s">
+        <v>330</v>
       </c>
       <c r="O30" s="137"/>
       <c r="P30" s="213"/>
@@ -8000,11 +8585,11 @@
       <c r="H31" s="106" t="s">
         <v>246</v>
       </c>
-      <c r="I31" s="329" t="s">
-        <v>298</v>
-      </c>
-      <c r="J31" s="348" t="s">
-        <v>342</v>
+      <c r="I31" s="306" t="s">
+        <v>293</v>
+      </c>
+      <c r="J31" s="325" t="s">
+        <v>337</v>
       </c>
       <c r="K31" s="152"/>
       <c r="L31" s="106"/>
@@ -8040,22 +8625,22 @@
         <v>81</v>
       </c>
       <c r="H32" s="106" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="I32" s="106" t="s">
-        <v>268</v>
-      </c>
-      <c r="J32" s="328" t="s">
-        <v>284</v>
-      </c>
-      <c r="K32" s="330" t="s">
-        <v>292</v>
+        <v>263</v>
+      </c>
+      <c r="J32" s="305" t="s">
+        <v>279</v>
+      </c>
+      <c r="K32" s="307" t="s">
+        <v>287</v>
       </c>
       <c r="L32" s="106" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="M32" s="100" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="N32" s="106"/>
       <c r="O32" s="137"/>
@@ -8088,21 +8673,21 @@
         <v>94</v>
       </c>
       <c r="H33" s="137" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="I33" s="247" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="J33" s="106" t="s">
-        <v>289</v>
-      </c>
-      <c r="K33" s="342" t="s">
-        <v>305</v>
-      </c>
-      <c r="L33" s="315" t="s">
-        <v>330</v>
-      </c>
-      <c r="M33" s="348"/>
+        <v>284</v>
+      </c>
+      <c r="K33" s="319" t="s">
+        <v>300</v>
+      </c>
+      <c r="L33" s="292" t="s">
+        <v>325</v>
+      </c>
+      <c r="M33" s="325"/>
       <c r="N33" s="137"/>
       <c r="O33" s="253"/>
       <c r="P33" s="106"/>
@@ -8124,18 +8709,18 @@
       <c r="D34" s="256" t="s">
         <v>185</v>
       </c>
-      <c r="E34" s="322" t="s">
+      <c r="E34" s="299" t="s">
         <v>74</v>
       </c>
-      <c r="F34" s="323" t="s">
-        <v>323</v>
+      <c r="F34" s="300" t="s">
+        <v>318</v>
       </c>
       <c r="G34" s="218"/>
-      <c r="H34" s="293" t="s">
-        <v>282</v>
-      </c>
-      <c r="I34" s="338" t="s">
-        <v>324</v>
+      <c r="H34" s="270" t="s">
+        <v>277</v>
+      </c>
+      <c r="I34" s="315" t="s">
+        <v>319</v>
       </c>
       <c r="J34" s="106"/>
       <c r="K34" s="248"/>
@@ -8153,117 +8738,117 @@
       <c r="A35" s="205">
         <v>30</v>
       </c>
-      <c r="B35" s="335" t="s">
-        <v>316</v>
-      </c>
-      <c r="C35" s="321" t="s">
-        <v>280</v>
-      </c>
-      <c r="D35" s="326" t="s">
-        <v>307</v>
-      </c>
-      <c r="E35" s="327" t="s">
-        <v>281</v>
-      </c>
-      <c r="F35" s="299" t="s">
-        <v>309</v>
+      <c r="B35" s="312" t="s">
+        <v>311</v>
+      </c>
+      <c r="C35" s="298" t="s">
+        <v>275</v>
+      </c>
+      <c r="D35" s="303" t="s">
+        <v>302</v>
+      </c>
+      <c r="E35" s="304" t="s">
+        <v>276</v>
+      </c>
+      <c r="F35" s="276" t="s">
+        <v>304</v>
       </c>
       <c r="G35" s="218"/>
       <c r="H35" s="137" t="s">
-        <v>310</v>
-      </c>
-      <c r="I35" s="338" t="s">
-        <v>328</v>
+        <v>305</v>
+      </c>
+      <c r="I35" s="315" t="s">
+        <v>323</v>
       </c>
       <c r="J35" s="106"/>
       <c r="K35" s="248"/>
       <c r="L35" s="137"/>
-      <c r="M35" s="318"/>
-      <c r="N35" s="319"/>
-      <c r="O35" s="319"/>
-      <c r="P35" s="319"/>
-      <c r="Q35" s="319"/>
-      <c r="R35" s="319"/>
-      <c r="S35" s="319"/>
+      <c r="M35" s="295"/>
+      <c r="N35" s="296"/>
+      <c r="O35" s="296"/>
+      <c r="P35" s="296"/>
+      <c r="Q35" s="296"/>
+      <c r="R35" s="296"/>
+      <c r="S35" s="296"/>
       <c r="T35" s="214"/>
     </row>
     <row r="36" spans="1:20" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="205">
         <v>31</v>
       </c>
-      <c r="B36" s="335" t="s">
-        <v>315</v>
+      <c r="B36" s="312" t="s">
+        <v>310</v>
       </c>
       <c r="C36" s="249" t="s">
-        <v>280</v>
-      </c>
-      <c r="D36" s="326" t="s">
-        <v>308</v>
-      </c>
-      <c r="E36" s="327" t="s">
-        <v>281</v>
-      </c>
-      <c r="F36" s="299" t="s">
+        <v>275</v>
+      </c>
+      <c r="D36" s="303" t="s">
+        <v>303</v>
+      </c>
+      <c r="E36" s="304" t="s">
+        <v>276</v>
+      </c>
+      <c r="F36" s="276" t="s">
         <v>55</v>
       </c>
       <c r="G36" s="218"/>
       <c r="H36" s="105" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="I36" s="247"/>
       <c r="J36" s="106"/>
       <c r="K36" s="248"/>
       <c r="L36" s="137"/>
-      <c r="M36" s="318"/>
-      <c r="N36" s="319"/>
-      <c r="O36" s="319"/>
-      <c r="P36" s="319"/>
-      <c r="Q36" s="319"/>
-      <c r="R36" s="319"/>
-      <c r="S36" s="319"/>
+      <c r="M36" s="295"/>
+      <c r="N36" s="296"/>
+      <c r="O36" s="296"/>
+      <c r="P36" s="296"/>
+      <c r="Q36" s="296"/>
+      <c r="R36" s="296"/>
+      <c r="S36" s="296"/>
       <c r="T36" s="214"/>
     </row>
     <row r="37" spans="1:20" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="205">
         <v>32</v>
       </c>
-      <c r="B37" s="320" t="s">
+      <c r="B37" s="297" t="s">
+        <v>307</v>
+      </c>
+      <c r="C37" s="311" t="s">
+        <v>309</v>
+      </c>
+      <c r="D37" s="309" t="s">
+        <v>308</v>
+      </c>
+      <c r="E37" s="313" t="s">
         <v>312</v>
       </c>
-      <c r="C37" s="334" t="s">
-        <v>314</v>
-      </c>
-      <c r="D37" s="332" t="s">
-        <v>313</v>
-      </c>
-      <c r="E37" s="336" t="s">
-        <v>317</v>
-      </c>
-      <c r="F37" s="333" t="s">
+      <c r="F37" s="310" t="s">
         <v>26</v>
       </c>
       <c r="G37" s="218"/>
-      <c r="H37" s="348"/>
+      <c r="H37" s="325"/>
       <c r="I37" s="247"/>
       <c r="J37" s="106"/>
       <c r="K37" s="248"/>
       <c r="L37" s="137"/>
-      <c r="M37" s="318"/>
-      <c r="N37" s="319"/>
-      <c r="O37" s="319"/>
-      <c r="P37" s="319"/>
-      <c r="Q37" s="319"/>
-      <c r="R37" s="319"/>
-      <c r="S37" s="319"/>
+      <c r="M37" s="295"/>
+      <c r="N37" s="296"/>
+      <c r="O37" s="296"/>
+      <c r="P37" s="296"/>
+      <c r="Q37" s="296"/>
+      <c r="R37" s="296"/>
+      <c r="S37" s="296"/>
       <c r="T37" s="214"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A38" s="205"/>
       <c r="B38" s="250"/>
       <c r="C38" s="250"/>
-      <c r="D38" s="324"/>
+      <c r="D38" s="301"/>
       <c r="E38" s="251"/>
-      <c r="F38" s="325"/>
+      <c r="F38" s="302"/>
       <c r="G38" s="252"/>
       <c r="H38" s="212"/>
       <c r="I38" s="212"/>
@@ -8291,7 +8876,7 @@
   <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C26" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -8299,11 +8884,11 @@
     <col min="1" max="1" width="5.5703125" style="198" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" style="199" customWidth="1"/>
     <col min="3" max="3" width="15" style="214" customWidth="1"/>
-    <col min="4" max="4" width="16" style="310" customWidth="1"/>
+    <col min="4" max="4" width="16" style="287" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" style="199" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.85546875" style="199" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" style="199" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" style="291" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" style="268" customWidth="1"/>
     <col min="9" max="9" width="21.85546875" style="214" customWidth="1"/>
     <col min="10" max="10" width="23.28515625" style="214" customWidth="1"/>
     <col min="11" max="11" width="18.28515625" style="214" customWidth="1"/>
@@ -8318,24 +8903,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="365" t="s">
+      <c r="B1" s="342" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="365"/>
-      <c r="D1" s="365"/>
-      <c r="E1" s="366"/>
-      <c r="F1" s="365"/>
-      <c r="G1" s="365"/>
+      <c r="C1" s="342"/>
+      <c r="D1" s="342"/>
+      <c r="E1" s="343"/>
+      <c r="F1" s="342"/>
+      <c r="G1" s="342"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
       <c r="B2" s="201" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="292" t="s">
+      <c r="C2" s="269" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="296" t="s">
+      <c r="D2" s="273" t="s">
         <v>49</v>
       </c>
       <c r="E2" s="202" t="s">
@@ -8370,13 +8955,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="206" t="s">
-        <v>255</v>
-      </c>
-      <c r="C3" s="297">
+        <v>250</v>
+      </c>
+      <c r="C3" s="274">
         <v>2019</v>
       </c>
-      <c r="D3" s="298" t="s">
-        <v>256</v>
+      <c r="D3" s="275" t="s">
+        <v>251</v>
       </c>
       <c r="E3" s="208" t="s">
         <v>74</v>
@@ -8386,7 +8971,7 @@
       </c>
       <c r="G3" s="51"/>
       <c r="H3" s="100" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="I3" s="106"/>
       <c r="J3" s="106"/>
@@ -8402,10 +8987,10 @@
       <c r="B4" s="215" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="299">
+      <c r="C4" s="276">
         <v>2012</v>
       </c>
-      <c r="D4" s="300" t="s">
+      <c r="D4" s="277" t="s">
         <v>180</v>
       </c>
       <c r="E4" s="216" t="s">
@@ -8415,7 +9000,7 @@
         <v>28</v>
       </c>
       <c r="G4" s="218"/>
-      <c r="H4" s="294"/>
+      <c r="H4" s="271"/>
       <c r="I4" s="213"/>
       <c r="J4" s="213"/>
       <c r="K4" s="213"/>
@@ -8441,7 +9026,7 @@
         <v>28</v>
       </c>
       <c r="G5" s="218"/>
-      <c r="H5" s="294"/>
+      <c r="H5" s="271"/>
       <c r="I5" s="213"/>
       <c r="J5" s="213"/>
       <c r="K5" s="213"/>
@@ -8454,10 +9039,10 @@
       <c r="B6" s="215" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="299">
+      <c r="C6" s="276">
         <v>2020</v>
       </c>
-      <c r="D6" s="301" t="s">
+      <c r="D6" s="278" t="s">
         <v>236</v>
       </c>
       <c r="E6" s="216" t="s">
@@ -8467,8 +9052,8 @@
         <v>28</v>
       </c>
       <c r="G6" s="218"/>
-      <c r="H6" s="293" t="s">
-        <v>261</v>
+      <c r="H6" s="270" t="s">
+        <v>256</v>
       </c>
       <c r="I6" s="213"/>
       <c r="J6" s="213"/>
@@ -8482,10 +9067,10 @@
       <c r="B7" s="219" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="302">
+      <c r="C7" s="279">
         <v>2012</v>
       </c>
-      <c r="D7" s="303" t="s">
+      <c r="D7" s="280" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="216" t="s">
@@ -8497,7 +9082,7 @@
       <c r="G7" s="206" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="295"/>
+      <c r="H7" s="272"/>
       <c r="I7" s="137"/>
       <c r="J7" s="221"/>
       <c r="K7" s="213"/>
@@ -8507,14 +9092,14 @@
       <c r="A8" s="205">
         <v>6</v>
       </c>
-      <c r="B8" s="350" t="s">
+      <c r="B8" s="327" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="350">
+      <c r="C8" s="327">
         <v>2020</v>
       </c>
-      <c r="D8" s="351" t="s">
-        <v>346</v>
+      <c r="D8" s="328" t="s">
+        <v>341</v>
       </c>
       <c r="E8" s="216" t="s">
         <v>73</v>
@@ -8524,10 +9109,10 @@
       </c>
       <c r="G8" s="224"/>
       <c r="H8" s="106" t="s">
-        <v>325</v>
-      </c>
-      <c r="I8" s="311" t="s">
-        <v>347</v>
+        <v>320</v>
+      </c>
+      <c r="I8" s="288" t="s">
+        <v>342</v>
       </c>
       <c r="J8" s="221"/>
       <c r="K8" s="213"/>
@@ -8540,23 +9125,23 @@
       <c r="B9" s="222" t="s">
         <v>168</v>
       </c>
-      <c r="C9" s="304">
+      <c r="C9" s="281">
         <v>2011</v>
       </c>
-      <c r="D9" s="305" t="s">
+      <c r="D9" s="282" t="s">
         <v>18</v>
       </c>
       <c r="E9" s="223" t="s">
         <v>73</v>
       </c>
       <c r="F9" s="222" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="G9" s="218" t="s">
         <v>77</v>
       </c>
-      <c r="H9" s="352" t="s">
-        <v>260</v>
+      <c r="H9" s="329" t="s">
+        <v>255</v>
       </c>
       <c r="I9" s="106"/>
       <c r="J9" s="106"/>
@@ -8570,10 +9155,10 @@
       <c r="B10" s="231" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="297">
+      <c r="C10" s="274">
         <v>2018</v>
       </c>
-      <c r="D10" s="307" t="s">
+      <c r="D10" s="284" t="s">
         <v>60</v>
       </c>
       <c r="E10" s="208" t="s">
@@ -8586,13 +9171,13 @@
         <v>94</v>
       </c>
       <c r="H10" s="106" t="s">
-        <v>337</v>
-      </c>
-      <c r="I10" s="357" t="s">
-        <v>355</v>
+        <v>332</v>
+      </c>
+      <c r="I10" s="334" t="s">
+        <v>350</v>
       </c>
       <c r="J10" s="100" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K10" s="106"/>
       <c r="L10" s="213"/>
@@ -8611,11 +9196,11 @@
       <c r="B11" s="231" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="297">
+      <c r="C11" s="274">
         <v>2018</v>
       </c>
-      <c r="D11" s="301" t="s">
-        <v>356</v>
+      <c r="D11" s="278" t="s">
+        <v>351</v>
       </c>
       <c r="E11" s="208" t="s">
         <v>74</v>
@@ -8626,14 +9211,14 @@
       <c r="G11" s="233" t="s">
         <v>93</v>
       </c>
-      <c r="H11" s="358" t="s">
-        <v>320</v>
-      </c>
-      <c r="I11" s="293" t="s">
-        <v>359</v>
+      <c r="H11" s="335" t="s">
+        <v>315</v>
+      </c>
+      <c r="I11" s="270" t="s">
+        <v>354</v>
       </c>
       <c r="J11" s="100" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="K11" s="234"/>
       <c r="L11" s="106"/>
@@ -8652,10 +9237,10 @@
       <c r="B12" s="231" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="297">
+      <c r="C12" s="274">
         <v>2019</v>
       </c>
-      <c r="D12" s="307" t="s">
+      <c r="D12" s="284" t="s">
         <v>129</v>
       </c>
       <c r="E12" s="208" t="s">
@@ -8666,7 +9251,7 @@
       </c>
       <c r="G12" s="233"/>
       <c r="H12" s="100" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="I12" s="137"/>
       <c r="J12" s="137"/>
@@ -8687,11 +9272,11 @@
       <c r="B13" s="232" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="297">
+      <c r="C13" s="274">
         <v>2015</v>
       </c>
-      <c r="D13" s="301" t="s">
-        <v>362</v>
+      <c r="D13" s="278" t="s">
+        <v>357</v>
       </c>
       <c r="E13" s="236" t="s">
         <v>74</v>
@@ -8703,10 +9288,10 @@
         <v>84</v>
       </c>
       <c r="H13" s="106" t="s">
-        <v>339</v>
-      </c>
-      <c r="I13" s="311" t="s">
-        <v>369</v>
+        <v>334</v>
+      </c>
+      <c r="I13" s="288" t="s">
+        <v>364</v>
       </c>
       <c r="J13" s="137"/>
       <c r="K13" s="137"/>
@@ -8726,11 +9311,11 @@
       <c r="B14" s="232" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="297">
+      <c r="C14" s="274">
         <v>2015</v>
       </c>
-      <c r="D14" s="349" t="s">
-        <v>352</v>
+      <c r="D14" s="326" t="s">
+        <v>347</v>
       </c>
       <c r="E14" s="236" t="s">
         <v>74</v>
@@ -8741,14 +9326,14 @@
       <c r="G14" s="218" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="355" t="s">
-        <v>326</v>
-      </c>
-      <c r="I14" s="356" t="s">
-        <v>353</v>
+      <c r="H14" s="332" t="s">
+        <v>321</v>
+      </c>
+      <c r="I14" s="333" t="s">
+        <v>348</v>
       </c>
       <c r="J14" s="238"/>
-      <c r="K14" s="290"/>
+      <c r="K14" s="267"/>
       <c r="L14" s="106"/>
       <c r="M14" s="99"/>
       <c r="N14" s="137"/>
@@ -8765,24 +9350,24 @@
       <c r="B15" s="232" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="297">
+      <c r="C15" s="274">
         <v>2017</v>
       </c>
-      <c r="D15" s="301" t="s">
-        <v>363</v>
+      <c r="D15" s="278" t="s">
+        <v>358</v>
       </c>
       <c r="E15" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="353"/>
+      <c r="F15" s="330"/>
       <c r="G15" s="233" t="s">
         <v>82</v>
       </c>
       <c r="H15" s="137" t="s">
-        <v>333</v>
-      </c>
-      <c r="I15" s="311" t="s">
-        <v>364</v>
+        <v>328</v>
+      </c>
+      <c r="I15" s="288" t="s">
+        <v>359</v>
       </c>
       <c r="J15" s="137"/>
       <c r="K15" s="106"/>
@@ -8802,10 +9387,10 @@
       <c r="B16" s="232" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="297">
+      <c r="C16" s="274">
         <v>2017</v>
       </c>
-      <c r="D16" s="307" t="s">
+      <c r="D16" s="284" t="s">
         <v>38</v>
       </c>
       <c r="E16" s="236" t="s">
@@ -8818,10 +9403,10 @@
         <v>83</v>
       </c>
       <c r="H16" s="106" t="s">
-        <v>329</v>
-      </c>
-      <c r="I16" s="311" t="s">
-        <v>365</v>
+        <v>324</v>
+      </c>
+      <c r="I16" s="288" t="s">
+        <v>360</v>
       </c>
       <c r="J16" s="99"/>
       <c r="K16" s="106"/>
@@ -8841,10 +9426,10 @@
       <c r="B17" s="232" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="297">
+      <c r="C17" s="274">
         <v>2017</v>
       </c>
-      <c r="D17" s="307" t="s">
+      <c r="D17" s="284" t="s">
         <v>40</v>
       </c>
       <c r="E17" s="236" t="s">
@@ -8857,7 +9442,7 @@
         <v>79</v>
       </c>
       <c r="H17" s="100" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="I17" s="106"/>
       <c r="J17" s="106"/>
@@ -8879,10 +9464,10 @@
       <c r="B18" s="258" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="297">
+      <c r="C18" s="274">
         <v>2018</v>
       </c>
-      <c r="D18" s="307" t="s">
+      <c r="D18" s="284" t="s">
         <v>54</v>
       </c>
       <c r="E18" s="208" t="s">
@@ -8893,10 +9478,10 @@
       </c>
       <c r="G18" s="224"/>
       <c r="H18" s="137" t="s">
-        <v>302</v>
-      </c>
-      <c r="I18" s="315" t="s">
-        <v>371</v>
+        <v>297</v>
+      </c>
+      <c r="I18" s="292" t="s">
+        <v>366</v>
       </c>
       <c r="J18" s="137"/>
       <c r="K18" s="213"/>
@@ -8917,10 +9502,10 @@
       <c r="B19" s="241" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="308">
+      <c r="C19" s="285">
         <v>2006</v>
       </c>
-      <c r="D19" s="309" t="s">
+      <c r="D19" s="286" t="s">
         <v>16</v>
       </c>
       <c r="E19" s="216" t="s">
@@ -8930,8 +9515,8 @@
         <v>17</v>
       </c>
       <c r="G19" s="218"/>
-      <c r="H19" s="294" t="s">
-        <v>259</v>
+      <c r="H19" s="271" t="s">
+        <v>254</v>
       </c>
       <c r="I19" s="213"/>
       <c r="J19" s="213"/>
@@ -8953,10 +9538,10 @@
       <c r="B20" s="219" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="302">
+      <c r="C20" s="279">
         <v>2018</v>
       </c>
-      <c r="D20" s="306" t="s">
+      <c r="D20" s="283" t="s">
         <v>58</v>
       </c>
       <c r="E20" s="216" t="s">
@@ -8968,8 +9553,8 @@
       <c r="G20" s="206" t="s">
         <v>95</v>
       </c>
-      <c r="H20" s="315" t="s">
-        <v>338</v>
+      <c r="H20" s="292" t="s">
+        <v>333</v>
       </c>
       <c r="I20" s="137"/>
       <c r="J20" s="137"/>
@@ -8991,10 +9576,10 @@
       <c r="B21" s="232" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="297">
+      <c r="C21" s="274">
         <v>2015</v>
       </c>
-      <c r="D21" s="307" t="s">
+      <c r="D21" s="284" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="236" t="s">
@@ -9007,7 +9592,7 @@
         <v>70</v>
       </c>
       <c r="H21" s="97" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="I21" s="137"/>
       <c r="J21" s="137"/>
@@ -9029,26 +9614,26 @@
       <c r="B22" s="232" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="297">
+      <c r="C22" s="274">
         <v>2015</v>
       </c>
-      <c r="D22" s="307" t="s">
+      <c r="D22" s="284" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="354" t="s">
+      <c r="F22" s="331" t="s">
         <v>51</v>
       </c>
       <c r="G22" s="218" t="s">
         <v>86</v>
       </c>
-      <c r="H22" s="328" t="s">
-        <v>331</v>
-      </c>
-      <c r="I22" s="311" t="s">
-        <v>350</v>
+      <c r="H22" s="305" t="s">
+        <v>326</v>
+      </c>
+      <c r="I22" s="288" t="s">
+        <v>345</v>
       </c>
       <c r="J22" s="213"/>
       <c r="K22" s="213"/>
@@ -9069,10 +9654,10 @@
       <c r="B23" s="232" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="297">
+      <c r="C23" s="274">
         <v>2015</v>
       </c>
-      <c r="D23" s="307" t="s">
+      <c r="D23" s="284" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="236" t="s">
@@ -9084,8 +9669,8 @@
       <c r="G23" s="218" t="s">
         <v>85</v>
       </c>
-      <c r="H23" s="311" t="s">
-        <v>360</v>
+      <c r="H23" s="288" t="s">
+        <v>355</v>
       </c>
       <c r="I23" s="148"/>
       <c r="J23" s="137"/>
@@ -9107,11 +9692,11 @@
       <c r="B24" s="232" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="297">
+      <c r="C24" s="274">
         <v>2016</v>
       </c>
-      <c r="D24" s="301" t="s">
-        <v>361</v>
+      <c r="D24" s="278" t="s">
+        <v>356</v>
       </c>
       <c r="E24" s="236" t="s">
         <v>74</v>
@@ -9123,13 +9708,13 @@
         <v>81</v>
       </c>
       <c r="H24" s="106" t="s">
-        <v>343</v>
-      </c>
-      <c r="I24" s="293" t="s">
-        <v>349</v>
-      </c>
-      <c r="J24" s="311" t="s">
-        <v>367</v>
+        <v>338</v>
+      </c>
+      <c r="I24" s="270" t="s">
+        <v>344</v>
+      </c>
+      <c r="J24" s="288" t="s">
+        <v>362</v>
       </c>
       <c r="K24" s="152"/>
       <c r="L24" s="106"/>
@@ -9149,10 +9734,10 @@
       <c r="B25" s="232" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="297">
+      <c r="C25" s="274">
         <v>2018</v>
       </c>
-      <c r="D25" s="307" t="s">
+      <c r="D25" s="284" t="s">
         <v>61</v>
       </c>
       <c r="E25" s="208" t="s">
@@ -9164,14 +9749,14 @@
       <c r="G25" s="218" t="s">
         <v>94</v>
       </c>
-      <c r="H25" s="328" t="s">
-        <v>330</v>
-      </c>
-      <c r="I25" s="293" t="s">
-        <v>351</v>
-      </c>
-      <c r="J25" s="311" t="s">
-        <v>357</v>
+      <c r="H25" s="305" t="s">
+        <v>325</v>
+      </c>
+      <c r="I25" s="270" t="s">
+        <v>346</v>
+      </c>
+      <c r="J25" s="288" t="s">
+        <v>352</v>
       </c>
       <c r="K25" s="248"/>
       <c r="L25" s="137"/>
@@ -9197,24 +9782,24 @@
       <c r="D26" s="256" t="s">
         <v>185</v>
       </c>
-      <c r="E26" s="322" t="s">
+      <c r="E26" s="299" t="s">
         <v>74</v>
       </c>
-      <c r="F26" s="323" t="s">
-        <v>323</v>
+      <c r="F26" s="300" t="s">
+        <v>318</v>
       </c>
       <c r="G26" s="218"/>
-      <c r="H26" s="293" t="s">
-        <v>282</v>
+      <c r="H26" s="270" t="s">
+        <v>277</v>
       </c>
       <c r="I26" s="247" t="s">
-        <v>324</v>
-      </c>
-      <c r="J26" s="293" t="s">
-        <v>354</v>
-      </c>
-      <c r="K26" s="359" t="s">
-        <v>370</v>
+        <v>319</v>
+      </c>
+      <c r="J26" s="270" t="s">
+        <v>349</v>
+      </c>
+      <c r="K26" s="336" t="s">
+        <v>365</v>
       </c>
       <c r="L26" s="137"/>
       <c r="M26" s="137"/>
@@ -9230,27 +9815,27 @@
       <c r="A27" s="205">
         <v>25</v>
       </c>
-      <c r="B27" s="335" t="s">
-        <v>316</v>
-      </c>
-      <c r="C27" s="321" t="s">
-        <v>280</v>
-      </c>
-      <c r="D27" s="326" t="s">
-        <v>307</v>
-      </c>
-      <c r="E27" s="327" t="s">
-        <v>281</v>
-      </c>
-      <c r="F27" s="299" t="s">
-        <v>309</v>
+      <c r="B27" s="312" t="s">
+        <v>311</v>
+      </c>
+      <c r="C27" s="298" t="s">
+        <v>275</v>
+      </c>
+      <c r="D27" s="303" t="s">
+        <v>302</v>
+      </c>
+      <c r="E27" s="304" t="s">
+        <v>276</v>
+      </c>
+      <c r="F27" s="276" t="s">
+        <v>304</v>
       </c>
       <c r="G27" s="218"/>
       <c r="H27" s="137" t="s">
-        <v>310</v>
-      </c>
-      <c r="I27" s="338" t="s">
-        <v>328</v>
+        <v>305</v>
+      </c>
+      <c r="I27" s="315" t="s">
+        <v>323</v>
       </c>
       <c r="J27" s="213"/>
       <c r="K27" s="213"/>
@@ -9260,24 +9845,24 @@
       <c r="A28" s="205">
         <v>26</v>
       </c>
-      <c r="B28" s="335" t="s">
-        <v>315</v>
+      <c r="B28" s="312" t="s">
+        <v>310</v>
       </c>
       <c r="C28" s="249" t="s">
-        <v>280</v>
-      </c>
-      <c r="D28" s="326" t="s">
-        <v>308</v>
-      </c>
-      <c r="E28" s="327" t="s">
-        <v>281</v>
-      </c>
-      <c r="F28" s="299" t="s">
+        <v>275</v>
+      </c>
+      <c r="D28" s="303" t="s">
+        <v>303</v>
+      </c>
+      <c r="E28" s="304" t="s">
+        <v>276</v>
+      </c>
+      <c r="F28" s="276" t="s">
         <v>55</v>
       </c>
       <c r="G28" s="218"/>
       <c r="H28" s="137" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="I28" s="247"/>
     </row>
@@ -9285,24 +9870,24 @@
       <c r="A29" s="205">
         <v>27</v>
       </c>
-      <c r="B29" s="320" t="s">
+      <c r="B29" s="297" t="s">
+        <v>307</v>
+      </c>
+      <c r="C29" s="311" t="s">
+        <v>309</v>
+      </c>
+      <c r="D29" s="309" t="s">
+        <v>308</v>
+      </c>
+      <c r="E29" s="313" t="s">
         <v>312</v>
       </c>
-      <c r="C29" s="334" t="s">
-        <v>314</v>
-      </c>
-      <c r="D29" s="332" t="s">
-        <v>313</v>
-      </c>
-      <c r="E29" s="336" t="s">
-        <v>317</v>
-      </c>
-      <c r="F29" s="333" t="s">
+      <c r="F29" s="310" t="s">
         <v>26</v>
       </c>
       <c r="G29" s="218"/>
-      <c r="H29" s="315" t="s">
-        <v>372</v>
+      <c r="H29" s="292" t="s">
+        <v>367</v>
       </c>
       <c r="I29" s="247"/>
     </row>
@@ -9333,318 +9918,1682 @@
   <sheetPr>
     <tabColor rgb="FF00FF00"/>
   </sheetPr>
-  <dimension ref="B1:E26"/>
+  <dimension ref="A1:L157"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="276" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" style="393" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="394" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="395"/>
+    <col min="4" max="4" width="15.85546875" style="396" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" style="396" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" style="395" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E1" s="289" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="2" spans="2:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="267" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="268" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="269" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="275" t="s">
-        <v>249</v>
-      </c>
-      <c r="C3" s="168" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" s="281" t="s">
+    <row r="1" spans="1:6" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="346" t="s">
+        <v>368</v>
+      </c>
+      <c r="B1" s="347"/>
+      <c r="C1" s="347"/>
+      <c r="D1" s="347"/>
+      <c r="E1" s="347"/>
+      <c r="F1" s="347"/>
+    </row>
+    <row r="2" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="348" t="s">
+        <v>369</v>
+      </c>
+      <c r="B2" s="349" t="s">
+        <v>370</v>
+      </c>
+      <c r="C2" s="349" t="s">
+        <v>371</v>
+      </c>
+      <c r="D2" s="350" t="s">
+        <v>372</v>
+      </c>
+      <c r="E2" s="350" t="s">
+        <v>373</v>
+      </c>
+      <c r="F2" s="351" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="352">
+        <v>1</v>
+      </c>
+      <c r="B3" s="353" t="s">
+        <v>375</v>
+      </c>
+      <c r="C3" s="353">
+        <v>2018</v>
+      </c>
+      <c r="D3" s="354" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="355" t="s">
+        <v>376</v>
+      </c>
+      <c r="F3" s="353" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="356">
+        <v>2</v>
+      </c>
+      <c r="B4" s="357" t="s">
+        <v>375</v>
+      </c>
+      <c r="C4" s="357">
+        <v>2018</v>
+      </c>
+      <c r="D4" s="358" t="s">
+        <v>378</v>
+      </c>
+      <c r="E4" s="359" t="s">
+        <v>379</v>
+      </c>
+      <c r="F4" s="357" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="356">
+        <v>3</v>
+      </c>
+      <c r="B5" s="357" t="s">
+        <v>375</v>
+      </c>
+      <c r="C5" s="357">
+        <v>2019</v>
+      </c>
+      <c r="D5" s="358" t="s">
+        <v>381</v>
+      </c>
+      <c r="E5" s="359" t="s">
+        <v>382</v>
+      </c>
+      <c r="F5" s="357" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="356">
+        <v>4</v>
+      </c>
+      <c r="B6" s="357" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="357">
+        <v>2018</v>
+      </c>
+      <c r="D6" s="360" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="359" t="s">
+        <v>384</v>
+      </c>
+      <c r="F6" s="357" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="356">
+        <v>5</v>
+      </c>
+      <c r="B7" s="357" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="357">
+        <v>2016</v>
+      </c>
+      <c r="D7" s="360" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="359" t="s">
+        <v>386</v>
+      </c>
+      <c r="F7" s="357" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="288"/>
-    </row>
-    <row r="4" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="270" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="161" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="282" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4" s="288"/>
-    </row>
-    <row r="5" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="271" t="s">
-        <v>250</v>
-      </c>
-      <c r="C5" s="161" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="272" t="s">
+    </row>
+    <row r="8" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="356">
+        <v>7</v>
+      </c>
+      <c r="B8" s="357" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="357">
+        <v>2015</v>
+      </c>
+      <c r="D8" s="360" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="361" t="s">
+        <v>387</v>
+      </c>
+      <c r="F8" s="357" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="356">
+        <v>8</v>
+      </c>
+      <c r="B9" s="357" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="353">
+        <v>2015</v>
+      </c>
+      <c r="D9" s="360" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="361" t="s">
+        <v>389</v>
+      </c>
+      <c r="F9" s="357" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="356">
+        <v>9</v>
+      </c>
+      <c r="B10" s="357" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="357">
+        <v>2015</v>
+      </c>
+      <c r="D10" s="360" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="362" t="s">
+        <v>391</v>
+      </c>
+      <c r="F10" s="357" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="356"/>
+      <c r="B11" s="363" t="s">
+        <v>393</v>
+      </c>
+      <c r="C11" s="363">
+        <v>2022</v>
+      </c>
+      <c r="D11" s="358" t="s">
+        <v>394</v>
+      </c>
+      <c r="E11" s="362" t="s">
+        <v>395</v>
+      </c>
+      <c r="F11" s="357"/>
+    </row>
+    <row r="12" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="356"/>
+      <c r="B12" s="363" t="s">
+        <v>396</v>
+      </c>
+      <c r="C12" s="363">
+        <v>2022</v>
+      </c>
+      <c r="D12" s="358" t="s">
+        <v>397</v>
+      </c>
+      <c r="E12" s="362" t="s">
+        <v>398</v>
+      </c>
+      <c r="F12" s="357"/>
+    </row>
+    <row r="13" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="356"/>
+      <c r="B13" s="363" t="s">
+        <v>399</v>
+      </c>
+      <c r="C13" s="363">
+        <v>2022</v>
+      </c>
+      <c r="D13" s="358" t="s">
+        <v>400</v>
+      </c>
+      <c r="E13" s="364" t="s">
+        <v>401</v>
+      </c>
+      <c r="F13" s="357"/>
+    </row>
+    <row r="14" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="356">
+        <v>10</v>
+      </c>
+      <c r="B14" s="360" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="360">
+        <v>2015</v>
+      </c>
+      <c r="D14" s="365" t="s">
+        <v>402</v>
+      </c>
+      <c r="E14" s="359" t="s">
+        <v>403</v>
+      </c>
+      <c r="F14" s="360" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="356">
+        <v>11</v>
+      </c>
+      <c r="B15" s="360" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="360">
+        <v>2015</v>
+      </c>
+      <c r="D15" s="360" t="s">
+        <v>404</v>
+      </c>
+      <c r="E15" s="359" t="s">
+        <v>405</v>
+      </c>
+      <c r="F15" s="357" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="356">
+        <v>12</v>
+      </c>
+      <c r="B16" s="357" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="357">
+        <v>2017</v>
+      </c>
+      <c r="D16" s="360" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="366" t="s">
+        <v>407</v>
+      </c>
+      <c r="F16" s="357" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="356">
+        <v>13</v>
+      </c>
+      <c r="B17" s="357" t="s">
+        <v>408</v>
+      </c>
+      <c r="C17" s="357">
+        <v>2017</v>
+      </c>
+      <c r="D17" s="360" t="s">
+        <v>409</v>
+      </c>
+      <c r="E17" s="366" t="s">
+        <v>410</v>
+      </c>
+      <c r="F17" s="357" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="356">
+        <v>14</v>
+      </c>
+      <c r="B18" s="357" t="s">
+        <v>411</v>
+      </c>
+      <c r="C18" s="357">
+        <v>2017</v>
+      </c>
+      <c r="D18" s="360" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="362" t="s">
+        <v>412</v>
+      </c>
+      <c r="F18" s="357" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="356"/>
+      <c r="B19" s="357" t="s">
+        <v>413</v>
+      </c>
+      <c r="C19" s="357">
+        <v>2022</v>
+      </c>
+      <c r="D19" s="360" t="s">
+        <v>414</v>
+      </c>
+      <c r="E19" s="362" t="s">
+        <v>415</v>
+      </c>
+      <c r="F19" s="357"/>
+    </row>
+    <row r="20" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="356"/>
+      <c r="B20" s="357" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="357">
+        <v>2022</v>
+      </c>
+      <c r="D20" s="360" t="s">
+        <v>416</v>
+      </c>
+      <c r="E20" s="362" t="s">
+        <v>417</v>
+      </c>
+      <c r="F20" s="357"/>
+    </row>
+    <row r="21" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="356">
+        <v>15</v>
+      </c>
+      <c r="B21" s="357" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="357">
+        <v>2006</v>
+      </c>
+      <c r="D21" s="360" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="362" t="s">
+        <v>418</v>
+      </c>
+      <c r="F21" s="357" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="367">
+        <v>16</v>
+      </c>
+      <c r="B22" s="357" t="s">
+        <v>419</v>
+      </c>
+      <c r="C22" s="357">
+        <v>2011</v>
+      </c>
+      <c r="D22" s="360" t="s">
+        <v>420</v>
+      </c>
+      <c r="E22" s="366" t="s">
+        <v>421</v>
+      </c>
+      <c r="F22" s="357" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="288"/>
-    </row>
-    <row r="6" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="277" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="157" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" s="272" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="288"/>
-    </row>
-    <row r="7" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="277" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="157" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="272" t="s">
-        <v>92</v>
-      </c>
-      <c r="E7" s="288"/>
-    </row>
-    <row r="8" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="277" t="s">
-        <v>129</v>
-      </c>
-      <c r="C8" s="157" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="273" t="s">
-        <v>110</v>
-      </c>
-      <c r="E8" s="288"/>
-    </row>
-    <row r="9" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="277" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="184" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" s="272" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="288" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="277" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="184" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="272" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="288"/>
-    </row>
-    <row r="11" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="277" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="184" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="272" t="s">
+    </row>
+    <row r="23" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="367">
+        <v>17</v>
+      </c>
+      <c r="B23" s="357" t="s">
+        <v>422</v>
+      </c>
+      <c r="C23" s="357">
+        <v>2020</v>
+      </c>
+      <c r="D23" s="360" t="s">
+        <v>423</v>
+      </c>
+      <c r="E23" s="366" t="s">
+        <v>424</v>
+      </c>
+      <c r="F23" s="357" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="373" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="368">
+        <v>18</v>
+      </c>
+      <c r="B24" s="369" t="s">
+        <v>425</v>
+      </c>
+      <c r="C24" s="369">
+        <v>2021</v>
+      </c>
+      <c r="D24" s="369" t="s">
+        <v>426</v>
+      </c>
+      <c r="E24" s="370" t="s">
+        <v>427</v>
+      </c>
+      <c r="F24" s="360" t="s">
+        <v>380</v>
+      </c>
+      <c r="G24" s="371"/>
+      <c r="H24" s="372"/>
+      <c r="I24" s="372"/>
+      <c r="J24" s="372"/>
+      <c r="K24" s="372"/>
+      <c r="L24" s="372"/>
+    </row>
+    <row r="25" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="356">
+        <v>19</v>
+      </c>
+      <c r="B25" s="369" t="s">
+        <v>425</v>
+      </c>
+      <c r="C25" s="369">
+        <v>2021</v>
+      </c>
+      <c r="D25" s="369" t="s">
+        <v>428</v>
+      </c>
+      <c r="E25" s="370" t="s">
+        <v>429</v>
+      </c>
+      <c r="F25" s="357" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="356">
+        <v>20</v>
+      </c>
+      <c r="B26" s="369" t="s">
+        <v>425</v>
+      </c>
+      <c r="C26" s="369">
+        <v>2022</v>
+      </c>
+      <c r="D26" s="369" t="s">
+        <v>431</v>
+      </c>
+      <c r="E26" s="374" t="s">
+        <v>432</v>
+      </c>
+      <c r="F26" s="357" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="356">
         <v>21</v>
       </c>
-      <c r="E11" s="288"/>
-    </row>
-    <row r="12" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="277" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="184" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="272" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="288"/>
-    </row>
-    <row r="13" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="277" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="184" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" s="273" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="288"/>
-    </row>
-    <row r="14" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="278" t="s">
-        <v>251</v>
-      </c>
-      <c r="C14" s="161" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="283" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="288"/>
-    </row>
-    <row r="15" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="279" t="s">
+      <c r="B27" s="369" t="s">
+        <v>433</v>
+      </c>
+      <c r="C27" s="369">
+        <v>2018</v>
+      </c>
+      <c r="D27" s="369" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="366" t="s">
+        <v>434</v>
+      </c>
+      <c r="F27" s="357" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="375"/>
+      <c r="B28" s="376"/>
+      <c r="C28" s="376"/>
+      <c r="D28" s="376"/>
+      <c r="E28" s="376"/>
+      <c r="F28" s="377"/>
+    </row>
+    <row r="29" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="356">
         <v>23</v>
       </c>
-      <c r="C15" s="161" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" s="283" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="288"/>
-    </row>
-    <row r="16" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="280" t="s">
+      <c r="B29" s="369" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="369">
+        <v>2021</v>
+      </c>
+      <c r="D29" s="369" t="s">
+        <v>436</v>
+      </c>
+      <c r="E29" s="364" t="s">
+        <v>437</v>
+      </c>
+      <c r="F29" s="357" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="356">
+        <v>24</v>
+      </c>
+      <c r="B30" s="369" t="s">
+        <v>439</v>
+      </c>
+      <c r="C30" s="369">
+        <v>2012</v>
+      </c>
+      <c r="D30" s="369" t="s">
+        <v>440</v>
+      </c>
+      <c r="E30" s="378" t="s">
+        <v>441</v>
+      </c>
+      <c r="F30" s="357" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="356">
         <v>25</v>
       </c>
-      <c r="C16" s="161" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="283" t="s">
+      <c r="B31" s="369" t="s">
+        <v>442</v>
+      </c>
+      <c r="C31" s="369">
+        <v>2010</v>
+      </c>
+      <c r="D31" s="369" t="s">
+        <v>443</v>
+      </c>
+      <c r="E31" s="366" t="s">
+        <v>444</v>
+      </c>
+      <c r="F31" s="357" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="379"/>
+      <c r="B32" s="376"/>
+      <c r="C32" s="376"/>
+      <c r="D32" s="376"/>
+      <c r="E32" s="376"/>
+      <c r="F32" s="380"/>
+    </row>
+    <row r="33" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="356">
         <v>26</v>
       </c>
-      <c r="E16" s="288"/>
-    </row>
-    <row r="17" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="280" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="161" t="s">
-        <v>74</v>
-      </c>
-      <c r="D17" s="284" t="s">
-        <v>199</v>
-      </c>
-      <c r="E17" s="288"/>
-    </row>
-    <row r="18" spans="2:5" ht="32.450000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="277" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="184" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="285" t="s">
-        <v>142</v>
-      </c>
-      <c r="E18" s="288"/>
-    </row>
-    <row r="19" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="277" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="184" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="272" t="s">
-        <v>110</v>
-      </c>
-      <c r="E19" s="288"/>
-    </row>
-    <row r="20" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="277" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="184" t="s">
-        <v>74</v>
-      </c>
-      <c r="D20" s="286" t="s">
-        <v>110</v>
-      </c>
-      <c r="E20" s="288"/>
-    </row>
-    <row r="21" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="277" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="184" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21" s="272" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="288"/>
-    </row>
-    <row r="22" spans="2:5" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="277" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="184" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="284" t="s">
-        <v>151</v>
-      </c>
-      <c r="E22" s="288"/>
-    </row>
-    <row r="23" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="277" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="184" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" s="272" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="288"/>
-    </row>
-    <row r="24" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="277" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="157" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="272" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="288"/>
-    </row>
-    <row r="25" spans="2:5" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="274" t="s">
-        <v>185</v>
-      </c>
-      <c r="C25" s="157" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="287" t="s">
-        <v>245</v>
-      </c>
-      <c r="E25" s="288"/>
-    </row>
-    <row r="26" spans="2:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="B33" s="369" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="369">
+        <v>2012</v>
+      </c>
+      <c r="D33" s="369" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" s="366" t="s">
+        <v>445</v>
+      </c>
+      <c r="F33" s="357" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="356">
+        <v>27</v>
+      </c>
+      <c r="B34" s="381" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="369">
+        <v>2020</v>
+      </c>
+      <c r="D34" s="369" t="s">
+        <v>446</v>
+      </c>
+      <c r="E34" s="361" t="s">
+        <v>447</v>
+      </c>
+      <c r="F34" s="357" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="356">
+        <v>28</v>
+      </c>
+      <c r="B35" s="381" t="s">
+        <v>449</v>
+      </c>
+      <c r="C35" s="357">
+        <v>2018</v>
+      </c>
+      <c r="D35" s="360" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35" s="359" t="s">
+        <v>450</v>
+      </c>
+      <c r="F35" s="357" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="382">
+        <v>29</v>
+      </c>
+      <c r="B36" s="383" t="s">
+        <v>451</v>
+      </c>
+      <c r="C36" s="384">
+        <v>2019</v>
+      </c>
+      <c r="D36" s="385" t="s">
+        <v>452</v>
+      </c>
+      <c r="E36" s="386" t="s">
+        <v>453</v>
+      </c>
+      <c r="F36" s="387" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="382">
+        <v>30</v>
+      </c>
+      <c r="B37" s="381" t="s">
+        <v>454</v>
+      </c>
+      <c r="C37" s="357">
+        <v>2019</v>
+      </c>
+      <c r="D37" s="388" t="s">
+        <v>455</v>
+      </c>
+      <c r="E37" s="388" t="s">
+        <v>456</v>
+      </c>
+      <c r="F37" s="389" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38"/>
+      <c r="B38" s="390"/>
+      <c r="C38" s="391"/>
+      <c r="D38" s="392"/>
+      <c r="E38" s="391"/>
+      <c r="F38" s="391"/>
+    </row>
+    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39"/>
+      <c r="B39" s="390"/>
+      <c r="C39" s="391"/>
+      <c r="D39" s="392"/>
+      <c r="E39" s="391"/>
+      <c r="F39" s="391"/>
+    </row>
+    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40"/>
+      <c r="B40" s="390"/>
+      <c r="C40" s="391"/>
+      <c r="D40" s="392"/>
+      <c r="E40" s="391"/>
+      <c r="F40" s="391"/>
+    </row>
+    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41"/>
+      <c r="B41" s="390"/>
+      <c r="C41" s="391"/>
+      <c r="D41" s="392"/>
+      <c r="E41" s="391"/>
+      <c r="F41" s="391"/>
+    </row>
+    <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42"/>
+      <c r="B42" s="390"/>
+      <c r="C42" s="391"/>
+      <c r="D42" s="392"/>
+      <c r="E42" s="391"/>
+      <c r="F42" s="391"/>
+    </row>
+    <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43"/>
+      <c r="B43" s="390"/>
+      <c r="C43" s="391"/>
+      <c r="D43" s="392"/>
+      <c r="E43" s="391"/>
+      <c r="F43" s="391"/>
+    </row>
+    <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44"/>
+      <c r="B44" s="390"/>
+      <c r="C44" s="391"/>
+      <c r="D44" s="392"/>
+      <c r="E44" s="391"/>
+      <c r="F44" s="391"/>
+    </row>
+    <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45"/>
+      <c r="B45" s="390"/>
+      <c r="C45" s="391"/>
+      <c r="D45" s="392"/>
+      <c r="E45" s="391"/>
+      <c r="F45" s="391"/>
+    </row>
+    <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46"/>
+      <c r="B46" s="390"/>
+      <c r="C46" s="391"/>
+      <c r="D46" s="392"/>
+      <c r="E46" s="391"/>
+      <c r="F46" s="391"/>
+    </row>
+    <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47"/>
+      <c r="B47" s="390"/>
+      <c r="C47" s="391"/>
+      <c r="D47" s="392"/>
+      <c r="E47" s="391"/>
+      <c r="F47" s="391"/>
+    </row>
+    <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48"/>
+      <c r="B48" s="390"/>
+      <c r="C48" s="391"/>
+      <c r="D48" s="392"/>
+      <c r="E48" s="391"/>
+      <c r="F48" s="391"/>
+    </row>
+    <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49"/>
+      <c r="B49" s="390"/>
+      <c r="C49" s="391"/>
+      <c r="D49" s="392"/>
+      <c r="E49" s="391"/>
+      <c r="F49" s="391"/>
+    </row>
+    <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50"/>
+      <c r="B50" s="390"/>
+      <c r="C50" s="391"/>
+      <c r="D50" s="392"/>
+      <c r="E50" s="391"/>
+      <c r="F50" s="391"/>
+    </row>
+    <row r="51" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51"/>
+      <c r="B51" s="390"/>
+      <c r="C51" s="391"/>
+      <c r="D51" s="392"/>
+      <c r="E51" s="391"/>
+      <c r="F51" s="391"/>
+    </row>
+    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52"/>
+      <c r="B52" s="390"/>
+      <c r="C52" s="391"/>
+      <c r="D52" s="392"/>
+      <c r="E52" s="391"/>
+      <c r="F52" s="391"/>
+    </row>
+    <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53"/>
+      <c r="B53" s="390"/>
+      <c r="C53" s="391"/>
+      <c r="D53" s="392"/>
+      <c r="E53" s="391"/>
+      <c r="F53" s="391"/>
+    </row>
+    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54"/>
+      <c r="B54" s="390"/>
+      <c r="C54" s="391"/>
+      <c r="D54" s="392"/>
+      <c r="E54" s="391"/>
+      <c r="F54" s="391"/>
+    </row>
+    <row r="55" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55"/>
+      <c r="B55" s="390"/>
+      <c r="C55" s="391"/>
+      <c r="D55" s="392"/>
+      <c r="E55" s="391"/>
+      <c r="F55" s="391"/>
+    </row>
+    <row r="56" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56"/>
+      <c r="B56" s="390"/>
+      <c r="C56" s="391"/>
+      <c r="D56" s="392"/>
+      <c r="E56" s="391"/>
+      <c r="F56" s="391"/>
+    </row>
+    <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57"/>
+      <c r="B57" s="390"/>
+      <c r="C57" s="391"/>
+      <c r="D57" s="392"/>
+      <c r="E57" s="391"/>
+      <c r="F57" s="391"/>
+    </row>
+    <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58"/>
+      <c r="B58" s="390"/>
+      <c r="C58" s="391"/>
+      <c r="D58" s="392"/>
+      <c r="E58" s="391"/>
+      <c r="F58" s="391"/>
+    </row>
+    <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59"/>
+      <c r="B59" s="390"/>
+      <c r="C59" s="391"/>
+      <c r="D59" s="392"/>
+      <c r="E59" s="391"/>
+      <c r="F59" s="391"/>
+    </row>
+    <row r="60" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60"/>
+      <c r="B60" s="390"/>
+      <c r="C60" s="391"/>
+      <c r="D60" s="392"/>
+      <c r="E60" s="391"/>
+      <c r="F60" s="391"/>
+    </row>
+    <row r="61" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61"/>
+      <c r="B61" s="390"/>
+      <c r="C61" s="391"/>
+      <c r="D61" s="392"/>
+      <c r="E61" s="391"/>
+      <c r="F61" s="391"/>
+    </row>
+    <row r="62" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62"/>
+      <c r="B62" s="390"/>
+      <c r="C62" s="391"/>
+      <c r="D62" s="392"/>
+      <c r="E62" s="391"/>
+      <c r="F62" s="391"/>
+    </row>
+    <row r="63" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63"/>
+      <c r="B63" s="390"/>
+      <c r="C63" s="391"/>
+      <c r="D63" s="392"/>
+      <c r="E63" s="391"/>
+      <c r="F63" s="391"/>
+    </row>
+    <row r="64" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64"/>
+      <c r="B64" s="390"/>
+      <c r="C64" s="391"/>
+      <c r="D64" s="392"/>
+      <c r="E64" s="391"/>
+      <c r="F64" s="391"/>
+    </row>
+    <row r="65" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65"/>
+      <c r="B65" s="390"/>
+      <c r="C65" s="391"/>
+      <c r="D65" s="392"/>
+      <c r="E65" s="391"/>
+      <c r="F65" s="391"/>
+    </row>
+    <row r="66" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66"/>
+      <c r="B66" s="390"/>
+      <c r="C66" s="391"/>
+      <c r="D66" s="392"/>
+      <c r="E66" s="391"/>
+      <c r="F66" s="391"/>
+    </row>
+    <row r="67" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67"/>
+      <c r="B67" s="390"/>
+      <c r="C67" s="391"/>
+      <c r="D67" s="392"/>
+      <c r="E67" s="391"/>
+      <c r="F67" s="391"/>
+    </row>
+    <row r="68" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68"/>
+      <c r="B68" s="390"/>
+      <c r="C68" s="391"/>
+      <c r="D68" s="392"/>
+      <c r="E68" s="391"/>
+      <c r="F68" s="391"/>
+    </row>
+    <row r="69" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A69"/>
+      <c r="B69" s="390"/>
+      <c r="C69" s="391"/>
+      <c r="D69" s="392"/>
+      <c r="E69" s="391"/>
+      <c r="F69" s="391"/>
+    </row>
+    <row r="70" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70"/>
+      <c r="B70" s="390"/>
+      <c r="C70" s="391"/>
+      <c r="D70" s="392"/>
+      <c r="E70" s="391"/>
+      <c r="F70" s="391"/>
+    </row>
+    <row r="71" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A71"/>
+      <c r="B71" s="390"/>
+      <c r="C71" s="391"/>
+      <c r="D71" s="392"/>
+      <c r="E71" s="391"/>
+      <c r="F71" s="391"/>
+    </row>
+    <row r="72" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72"/>
+      <c r="B72" s="390"/>
+      <c r="C72" s="391"/>
+      <c r="D72" s="392"/>
+      <c r="E72" s="391"/>
+      <c r="F72" s="391"/>
+    </row>
+    <row r="73" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73"/>
+      <c r="B73" s="390"/>
+      <c r="C73" s="391"/>
+      <c r="D73" s="392"/>
+      <c r="E73" s="391"/>
+      <c r="F73" s="391"/>
+    </row>
+    <row r="74" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A74"/>
+      <c r="B74" s="390"/>
+      <c r="C74" s="391"/>
+      <c r="D74" s="392"/>
+      <c r="E74" s="391"/>
+      <c r="F74" s="391"/>
+    </row>
+    <row r="75" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A75"/>
+      <c r="B75" s="390"/>
+      <c r="C75" s="391"/>
+      <c r="D75" s="392"/>
+      <c r="E75" s="391"/>
+      <c r="F75" s="391"/>
+    </row>
+    <row r="76" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A76"/>
+      <c r="B76" s="390"/>
+      <c r="C76" s="391"/>
+      <c r="D76" s="392"/>
+      <c r="E76" s="391"/>
+      <c r="F76" s="391"/>
+    </row>
+    <row r="77" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A77"/>
+      <c r="B77" s="390"/>
+      <c r="C77" s="391"/>
+      <c r="D77" s="392"/>
+      <c r="E77" s="391"/>
+      <c r="F77" s="391"/>
+    </row>
+    <row r="78" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A78"/>
+      <c r="B78" s="390"/>
+      <c r="C78" s="391"/>
+      <c r="D78" s="392"/>
+      <c r="E78" s="391"/>
+      <c r="F78" s="391"/>
+    </row>
+    <row r="79" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A79"/>
+      <c r="B79" s="390"/>
+      <c r="C79" s="391"/>
+      <c r="D79" s="392"/>
+      <c r="E79" s="391"/>
+      <c r="F79" s="391"/>
+    </row>
+    <row r="80" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A80"/>
+      <c r="B80" s="390"/>
+      <c r="C80" s="391"/>
+      <c r="D80" s="392"/>
+      <c r="E80" s="391"/>
+      <c r="F80" s="391"/>
+    </row>
+    <row r="81" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A81"/>
+      <c r="B81" s="390"/>
+      <c r="C81" s="391"/>
+      <c r="D81" s="392"/>
+      <c r="E81" s="391"/>
+      <c r="F81" s="391"/>
+    </row>
+    <row r="82" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A82"/>
+      <c r="B82" s="390"/>
+      <c r="C82" s="391"/>
+      <c r="D82" s="392"/>
+      <c r="E82" s="391"/>
+      <c r="F82" s="391"/>
+    </row>
+    <row r="83" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A83"/>
+      <c r="B83" s="390"/>
+      <c r="C83" s="391"/>
+      <c r="D83" s="392"/>
+      <c r="E83" s="391"/>
+      <c r="F83" s="391"/>
+    </row>
+    <row r="84" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A84"/>
+      <c r="B84" s="390"/>
+      <c r="C84" s="391"/>
+      <c r="D84" s="392"/>
+      <c r="E84" s="391"/>
+      <c r="F84" s="391"/>
+    </row>
+    <row r="85" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A85"/>
+      <c r="B85" s="390"/>
+      <c r="C85" s="391"/>
+      <c r="D85" s="392"/>
+      <c r="E85" s="391"/>
+      <c r="F85" s="391"/>
+    </row>
+    <row r="86" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A86"/>
+      <c r="B86" s="390"/>
+      <c r="C86" s="391"/>
+      <c r="D86" s="392"/>
+      <c r="E86" s="391"/>
+      <c r="F86" s="391"/>
+    </row>
+    <row r="87" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A87"/>
+      <c r="B87" s="390"/>
+      <c r="C87" s="391"/>
+      <c r="D87" s="392"/>
+      <c r="E87" s="391"/>
+      <c r="F87" s="391"/>
+    </row>
+    <row r="88" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A88"/>
+      <c r="B88" s="390"/>
+      <c r="C88" s="391"/>
+      <c r="D88" s="392"/>
+      <c r="E88" s="391"/>
+      <c r="F88" s="391"/>
+    </row>
+    <row r="89" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A89"/>
+      <c r="B89" s="390"/>
+      <c r="C89" s="391"/>
+      <c r="D89" s="392"/>
+      <c r="E89" s="391"/>
+      <c r="F89" s="391"/>
+    </row>
+    <row r="90" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A90"/>
+      <c r="B90" s="390"/>
+      <c r="C90" s="391"/>
+      <c r="D90" s="392"/>
+      <c r="E90" s="391"/>
+      <c r="F90" s="391"/>
+    </row>
+    <row r="91" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A91"/>
+      <c r="B91" s="390"/>
+      <c r="C91" s="391"/>
+      <c r="D91" s="392"/>
+      <c r="E91" s="391"/>
+      <c r="F91" s="391"/>
+    </row>
+    <row r="92" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A92"/>
+      <c r="B92" s="390"/>
+      <c r="C92" s="391"/>
+      <c r="D92" s="392"/>
+      <c r="E92" s="391"/>
+      <c r="F92" s="391"/>
+    </row>
+    <row r="93" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A93"/>
+      <c r="B93" s="390"/>
+      <c r="C93" s="391"/>
+      <c r="D93" s="392"/>
+      <c r="E93" s="391"/>
+      <c r="F93" s="391"/>
+    </row>
+    <row r="94" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A94"/>
+      <c r="B94" s="390"/>
+      <c r="C94" s="391"/>
+      <c r="D94" s="392"/>
+      <c r="E94" s="391"/>
+      <c r="F94" s="391"/>
+    </row>
+    <row r="95" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A95"/>
+      <c r="B95" s="390"/>
+      <c r="C95" s="391"/>
+      <c r="D95" s="392"/>
+      <c r="E95" s="391"/>
+      <c r="F95" s="391"/>
+    </row>
+    <row r="96" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A96"/>
+      <c r="B96" s="390"/>
+      <c r="C96" s="391"/>
+      <c r="D96" s="392"/>
+      <c r="E96" s="391"/>
+      <c r="F96" s="391"/>
+    </row>
+    <row r="97" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A97"/>
+      <c r="B97" s="390"/>
+      <c r="C97" s="391"/>
+      <c r="D97" s="392"/>
+      <c r="E97" s="391"/>
+      <c r="F97" s="391"/>
+    </row>
+    <row r="98" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A98"/>
+      <c r="B98" s="390"/>
+      <c r="C98" s="391"/>
+      <c r="D98" s="392"/>
+      <c r="E98" s="391"/>
+      <c r="F98" s="391"/>
+    </row>
+    <row r="99" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A99"/>
+      <c r="B99" s="390"/>
+      <c r="C99" s="391"/>
+      <c r="D99" s="392"/>
+      <c r="E99" s="391"/>
+      <c r="F99" s="391"/>
+    </row>
+    <row r="100" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A100"/>
+      <c r="B100" s="390"/>
+      <c r="C100" s="391"/>
+      <c r="D100" s="392"/>
+      <c r="E100" s="391"/>
+      <c r="F100" s="391"/>
+    </row>
+    <row r="101" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A101"/>
+      <c r="B101" s="390"/>
+      <c r="C101" s="391"/>
+      <c r="D101" s="392"/>
+      <c r="E101" s="391"/>
+      <c r="F101" s="391"/>
+    </row>
+    <row r="102" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A102"/>
+      <c r="B102" s="390"/>
+      <c r="C102" s="391"/>
+      <c r="D102" s="392"/>
+      <c r="E102" s="391"/>
+      <c r="F102" s="391"/>
+    </row>
+    <row r="103" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A103"/>
+      <c r="B103" s="390"/>
+      <c r="C103" s="391"/>
+      <c r="D103" s="392"/>
+      <c r="E103" s="391"/>
+      <c r="F103" s="391"/>
+    </row>
+    <row r="104" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A104"/>
+      <c r="B104" s="390"/>
+      <c r="C104" s="391"/>
+      <c r="D104" s="392"/>
+      <c r="E104" s="391"/>
+      <c r="F104" s="391"/>
+    </row>
+    <row r="105" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A105"/>
+      <c r="B105" s="390"/>
+      <c r="C105" s="391"/>
+      <c r="D105" s="392"/>
+      <c r="E105" s="391"/>
+      <c r="F105" s="391"/>
+    </row>
+    <row r="106" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A106"/>
+      <c r="B106" s="390"/>
+      <c r="C106" s="391"/>
+      <c r="D106" s="392"/>
+      <c r="E106" s="391"/>
+      <c r="F106" s="391"/>
+    </row>
+    <row r="107" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A107"/>
+      <c r="B107" s="390"/>
+      <c r="C107" s="391"/>
+      <c r="D107" s="392"/>
+      <c r="E107" s="391"/>
+      <c r="F107" s="391"/>
+    </row>
+    <row r="108" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A108"/>
+      <c r="B108" s="390"/>
+      <c r="C108" s="391"/>
+      <c r="D108" s="392"/>
+      <c r="E108" s="391"/>
+      <c r="F108" s="391"/>
+    </row>
+    <row r="109" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A109"/>
+      <c r="B109" s="390"/>
+      <c r="C109" s="391"/>
+      <c r="D109" s="392"/>
+      <c r="E109" s="391"/>
+      <c r="F109" s="391"/>
+    </row>
+    <row r="110" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A110"/>
+      <c r="B110" s="390"/>
+      <c r="C110" s="391"/>
+      <c r="D110" s="392"/>
+      <c r="E110" s="391"/>
+      <c r="F110" s="391"/>
+    </row>
+    <row r="111" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A111"/>
+      <c r="B111" s="390"/>
+      <c r="C111" s="391"/>
+      <c r="D111" s="392"/>
+      <c r="E111" s="391"/>
+      <c r="F111" s="391"/>
+    </row>
+    <row r="112" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A112"/>
+      <c r="B112" s="390"/>
+      <c r="C112" s="391"/>
+      <c r="D112" s="392"/>
+      <c r="E112" s="391"/>
+      <c r="F112" s="391"/>
+    </row>
+    <row r="113" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A113"/>
+      <c r="B113" s="390"/>
+      <c r="C113" s="391"/>
+      <c r="D113" s="392"/>
+      <c r="E113" s="391"/>
+      <c r="F113" s="391"/>
+    </row>
+    <row r="114" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A114"/>
+      <c r="B114" s="390"/>
+      <c r="C114" s="391"/>
+      <c r="D114" s="392"/>
+      <c r="E114" s="391"/>
+      <c r="F114" s="391"/>
+    </row>
+    <row r="115" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A115"/>
+      <c r="B115" s="390"/>
+      <c r="C115" s="391"/>
+      <c r="D115" s="392"/>
+      <c r="E115" s="391"/>
+      <c r="F115" s="391"/>
+    </row>
+    <row r="116" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A116"/>
+      <c r="B116" s="390"/>
+      <c r="C116" s="391"/>
+      <c r="D116" s="392"/>
+      <c r="E116" s="391"/>
+      <c r="F116" s="391"/>
+    </row>
+    <row r="117" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A117"/>
+      <c r="B117" s="390"/>
+      <c r="C117" s="391"/>
+      <c r="D117" s="392"/>
+      <c r="E117" s="391"/>
+      <c r="F117" s="391"/>
+    </row>
+    <row r="118" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A118"/>
+      <c r="B118" s="390"/>
+      <c r="C118" s="391"/>
+      <c r="D118" s="392"/>
+      <c r="E118" s="391"/>
+      <c r="F118" s="391"/>
+    </row>
+    <row r="119" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A119"/>
+      <c r="B119" s="390"/>
+      <c r="C119" s="391"/>
+      <c r="D119" s="392"/>
+      <c r="E119" s="391"/>
+      <c r="F119" s="391"/>
+    </row>
+    <row r="120" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A120"/>
+      <c r="B120" s="390"/>
+      <c r="C120" s="391"/>
+      <c r="D120" s="392"/>
+      <c r="E120" s="391"/>
+      <c r="F120" s="391"/>
+    </row>
+    <row r="121" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A121"/>
+      <c r="B121" s="390"/>
+      <c r="C121" s="391"/>
+      <c r="D121" s="392"/>
+      <c r="E121" s="391"/>
+      <c r="F121" s="391"/>
+    </row>
+    <row r="122" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A122"/>
+      <c r="B122" s="390"/>
+      <c r="C122" s="391"/>
+      <c r="D122" s="392"/>
+      <c r="E122" s="391"/>
+      <c r="F122" s="391"/>
+    </row>
+    <row r="123" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A123"/>
+      <c r="B123" s="390"/>
+      <c r="C123" s="391"/>
+      <c r="D123" s="392"/>
+      <c r="E123" s="391"/>
+      <c r="F123" s="391"/>
+    </row>
+    <row r="124" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A124"/>
+      <c r="B124" s="390"/>
+      <c r="C124" s="391"/>
+      <c r="D124" s="392"/>
+      <c r="E124" s="391"/>
+      <c r="F124" s="391"/>
+    </row>
+    <row r="125" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A125"/>
+      <c r="B125" s="390"/>
+      <c r="C125" s="391"/>
+      <c r="D125" s="392"/>
+      <c r="E125" s="391"/>
+      <c r="F125" s="391"/>
+    </row>
+    <row r="126" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A126"/>
+      <c r="B126" s="390"/>
+      <c r="C126" s="391"/>
+      <c r="D126" s="392"/>
+      <c r="E126" s="391"/>
+      <c r="F126" s="391"/>
+    </row>
+    <row r="127" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A127"/>
+      <c r="B127" s="390"/>
+      <c r="C127" s="391"/>
+      <c r="D127" s="392"/>
+      <c r="E127" s="391"/>
+      <c r="F127" s="391"/>
+    </row>
+    <row r="128" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A128"/>
+      <c r="B128" s="390"/>
+      <c r="C128" s="391"/>
+      <c r="D128" s="392"/>
+      <c r="E128" s="391"/>
+      <c r="F128" s="391"/>
+    </row>
+    <row r="129" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A129"/>
+      <c r="B129" s="390"/>
+      <c r="C129" s="391"/>
+      <c r="D129" s="392"/>
+      <c r="E129" s="391"/>
+      <c r="F129" s="391"/>
+    </row>
+    <row r="130" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A130"/>
+      <c r="B130" s="390"/>
+      <c r="C130" s="391"/>
+      <c r="D130" s="392"/>
+      <c r="E130" s="391"/>
+      <c r="F130" s="391"/>
+    </row>
+    <row r="131" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A131"/>
+      <c r="B131" s="390"/>
+      <c r="C131" s="391"/>
+      <c r="D131" s="392"/>
+      <c r="E131" s="391"/>
+      <c r="F131" s="391"/>
+    </row>
+    <row r="132" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A132"/>
+      <c r="B132" s="390"/>
+      <c r="C132" s="391"/>
+      <c r="D132" s="392"/>
+      <c r="E132" s="391"/>
+      <c r="F132" s="391"/>
+    </row>
+    <row r="133" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A133"/>
+      <c r="B133" s="390"/>
+      <c r="C133" s="391"/>
+      <c r="D133" s="392"/>
+      <c r="E133" s="391"/>
+      <c r="F133" s="391"/>
+    </row>
+    <row r="134" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A134"/>
+      <c r="B134" s="390"/>
+      <c r="C134" s="391"/>
+      <c r="D134" s="392"/>
+      <c r="E134" s="391"/>
+      <c r="F134" s="391"/>
+    </row>
+    <row r="135" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A135"/>
+      <c r="B135" s="390"/>
+      <c r="C135" s="391"/>
+      <c r="D135" s="392"/>
+      <c r="E135" s="391"/>
+      <c r="F135" s="391"/>
+    </row>
+    <row r="136" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A136"/>
+      <c r="B136" s="390"/>
+      <c r="C136" s="391"/>
+      <c r="D136" s="392"/>
+      <c r="E136" s="391"/>
+      <c r="F136" s="391"/>
+    </row>
+    <row r="137" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A137"/>
+      <c r="B137" s="390"/>
+      <c r="C137" s="391"/>
+      <c r="D137" s="392"/>
+      <c r="E137" s="391"/>
+      <c r="F137" s="391"/>
+    </row>
+    <row r="138" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A138"/>
+      <c r="B138" s="390"/>
+      <c r="C138" s="391"/>
+      <c r="D138" s="392"/>
+      <c r="E138" s="391"/>
+      <c r="F138" s="391"/>
+    </row>
+    <row r="139" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A139"/>
+      <c r="B139" s="390"/>
+      <c r="C139" s="391"/>
+      <c r="D139" s="392"/>
+      <c r="E139" s="391"/>
+      <c r="F139" s="391"/>
+    </row>
+    <row r="140" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A140"/>
+      <c r="B140" s="390"/>
+      <c r="C140" s="391"/>
+      <c r="D140" s="392"/>
+      <c r="E140" s="391"/>
+      <c r="F140" s="391"/>
+    </row>
+    <row r="141" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A141"/>
+      <c r="B141" s="390"/>
+      <c r="C141" s="391"/>
+      <c r="D141" s="392"/>
+      <c r="E141" s="391"/>
+      <c r="F141" s="391"/>
+    </row>
+    <row r="142" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A142"/>
+      <c r="B142" s="390"/>
+      <c r="C142" s="391"/>
+      <c r="D142" s="392"/>
+      <c r="E142" s="391"/>
+      <c r="F142" s="391"/>
+    </row>
+    <row r="143" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A143"/>
+      <c r="B143" s="390"/>
+      <c r="C143" s="391"/>
+      <c r="D143" s="392"/>
+      <c r="E143" s="391"/>
+      <c r="F143" s="391"/>
+    </row>
+    <row r="144" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A144"/>
+      <c r="B144" s="390"/>
+      <c r="C144" s="391"/>
+      <c r="D144" s="392"/>
+      <c r="E144" s="391"/>
+      <c r="F144" s="391"/>
+    </row>
+    <row r="145" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A145"/>
+      <c r="B145" s="390"/>
+      <c r="C145" s="391"/>
+      <c r="D145" s="392"/>
+      <c r="E145" s="391"/>
+      <c r="F145" s="391"/>
+    </row>
+    <row r="146" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A146"/>
+      <c r="B146" s="390"/>
+      <c r="C146" s="391"/>
+      <c r="D146" s="392"/>
+      <c r="E146" s="391"/>
+      <c r="F146" s="391"/>
+    </row>
+    <row r="147" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A147"/>
+      <c r="B147" s="390"/>
+      <c r="C147" s="391"/>
+      <c r="D147" s="392"/>
+      <c r="E147" s="391"/>
+      <c r="F147" s="391"/>
+    </row>
+    <row r="148" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A148"/>
+      <c r="B148" s="390"/>
+      <c r="C148" s="391"/>
+      <c r="D148" s="392"/>
+      <c r="E148" s="391"/>
+      <c r="F148" s="391"/>
+    </row>
+    <row r="149" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A149"/>
+      <c r="B149" s="390"/>
+      <c r="C149" s="391"/>
+      <c r="D149" s="392"/>
+      <c r="E149" s="391"/>
+      <c r="F149" s="391"/>
+    </row>
+    <row r="150" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A150"/>
+      <c r="B150" s="390"/>
+      <c r="C150" s="391"/>
+      <c r="D150" s="392"/>
+      <c r="E150" s="391"/>
+      <c r="F150" s="391"/>
+    </row>
+    <row r="151" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A151"/>
+      <c r="B151" s="390"/>
+      <c r="C151" s="391"/>
+      <c r="D151" s="392"/>
+      <c r="E151" s="391"/>
+      <c r="F151" s="391"/>
+    </row>
+    <row r="152" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A152"/>
+      <c r="B152" s="390"/>
+      <c r="C152" s="391"/>
+      <c r="D152" s="392"/>
+      <c r="E152" s="391"/>
+      <c r="F152" s="391"/>
+    </row>
+    <row r="153" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A153"/>
+      <c r="B153" s="390"/>
+      <c r="C153" s="391"/>
+      <c r="D153" s="392"/>
+      <c r="E153" s="391"/>
+      <c r="F153" s="391"/>
+    </row>
+    <row r="154" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A154"/>
+      <c r="B154" s="390"/>
+      <c r="C154" s="391"/>
+      <c r="D154" s="392"/>
+      <c r="E154" s="391"/>
+      <c r="F154" s="391"/>
+    </row>
+    <row r="155" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A155"/>
+      <c r="B155" s="390"/>
+      <c r="C155" s="391"/>
+      <c r="D155" s="392"/>
+      <c r="E155" s="391"/>
+      <c r="F155" s="391"/>
+    </row>
+    <row r="156" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A156"/>
+      <c r="B156" s="390"/>
+      <c r="C156" s="391"/>
+      <c r="D156" s="392"/>
+      <c r="E156" s="391"/>
+      <c r="F156" s="391"/>
+    </row>
+    <row r="157" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A157"/>
+      <c r="B157" s="390"/>
+      <c r="C157" s="391"/>
+      <c r="D157" s="392"/>
+      <c r="E157" s="391"/>
+      <c r="F157" s="391"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G24:L24"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -9663,7 +11612,7 @@
   <sheetData>
     <row r="3" spans="3:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:3" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="360" t="s">
+      <c r="C4" s="337" t="s">
         <v>185</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cierre 19 sept 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
+++ b/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="472">
   <si>
     <t xml:space="preserve">RELACION DE UNIDADES Y ASIGNACION </t>
   </si>
@@ -1446,6 +1446,51 @@
   </si>
   <si>
     <t>XXX</t>
+  </si>
+  <si>
+    <t>SM 55463--SP--16664</t>
+  </si>
+  <si>
+    <t>6-Sept-22  128,536  KM</t>
+  </si>
+  <si>
+    <t>SM 39220--SP-16650</t>
+  </si>
+  <si>
+    <t>SM 39222--SP-16662</t>
+  </si>
+  <si>
+    <t>SM 51619--SP-16649</t>
+  </si>
+  <si>
+    <t>TRA-959-A--UJW-329A</t>
+  </si>
+  <si>
+    <t>SP-41040</t>
+  </si>
+  <si>
+    <t>TOYOTA  1</t>
+  </si>
+  <si>
+    <t>TOYOTA  2</t>
+  </si>
+  <si>
+    <t>TOYOTA  3</t>
+  </si>
+  <si>
+    <t>SP-13165</t>
+  </si>
+  <si>
+    <t>SP-13166</t>
+  </si>
+  <si>
+    <t>SP-41023</t>
+  </si>
+  <si>
+    <t>7-SEPT-2022   209,113 KM</t>
+  </si>
+  <si>
+    <t>6-Sept-22      245,739 KM</t>
   </si>
 </sst>
 </file>
@@ -1816,7 +1861,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="26">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1958,6 +2003,12 @@
     </fill>
     <fill>
       <patternFill patternType="darkVertical"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="27">
@@ -2302,7 +2353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="397">
+  <cellXfs count="400">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2953,9 +3004,6 @@
     <xf numFmtId="17" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3226,9 +3274,6 @@
     <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3241,34 +3286,7 @@
     <xf numFmtId="0" fontId="34" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3336,12 +3354,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -3413,6 +3425,54 @@
     </xf>
     <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3422,16 +3482,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCCFF"/>
+      <color rgb="FF00FF00"/>
       <color rgb="FF00FFFF"/>
       <color rgb="FF9966FF"/>
       <color rgb="FFCC6600"/>
       <color rgb="FFFF9900"/>
       <color rgb="FF9999FF"/>
-      <color rgb="FF00FF00"/>
       <color rgb="FFFF00FF"/>
       <color rgb="FF3399FF"/>
       <color rgb="FF99CCFF"/>
-      <color rgb="FF0000FF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -4168,6 +4228,226 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>895350</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>476250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Conector recto 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2714625" y="7953375"/>
+          <a:ext cx="1352550" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>885825</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Conector recto 7"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2705100" y="19640550"/>
+          <a:ext cx="1400175" cy="57150"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>790575</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>409575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Conector recto 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2609850" y="20621625"/>
+          <a:ext cx="1514475" cy="85725"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>857250</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>361950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Conector recto 12"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2676525" y="22602825"/>
+          <a:ext cx="1438275" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>885825</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Conector recto 14"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2705100" y="23545800"/>
+          <a:ext cx="1400175" cy="38100"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4576,14 +4856,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="338" t="s">
+      <c r="B1" s="384" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="338"/>
-      <c r="D1" s="338"/>
-      <c r="E1" s="339"/>
-      <c r="F1" s="338"/>
-      <c r="G1" s="338"/>
+      <c r="C1" s="384"/>
+      <c r="D1" s="384"/>
+      <c r="E1" s="385"/>
+      <c r="F1" s="384"/>
+      <c r="G1" s="384"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -4944,10 +5224,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="340" t="s">
+      <c r="L12" s="386" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="341"/>
+      <c r="M12" s="387"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -6142,14 +6422,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="338" t="s">
+      <c r="B1" s="384" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="338"/>
-      <c r="D1" s="338"/>
-      <c r="E1" s="339"/>
-      <c r="F1" s="338"/>
-      <c r="G1" s="338"/>
+      <c r="C1" s="384"/>
+      <c r="D1" s="384"/>
+      <c r="E1" s="385"/>
+      <c r="F1" s="384"/>
+      <c r="G1" s="384"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -6488,10 +6768,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="340" t="s">
+      <c r="L12" s="386" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="341"/>
+      <c r="M12" s="387"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -7449,7 +7729,7 @@
     <col min="1" max="1" width="5.5703125" style="198" customWidth="1"/>
     <col min="2" max="2" width="22.140625" style="199" customWidth="1"/>
     <col min="3" max="3" width="15" style="199" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" style="266" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="265" customWidth="1"/>
     <col min="5" max="5" width="18.140625" style="199" customWidth="1"/>
     <col min="6" max="6" width="22.85546875" style="199" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" style="199" hidden="1" customWidth="1"/>
@@ -7468,14 +7748,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="342" t="s">
+      <c r="B1" s="388" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="342"/>
-      <c r="D1" s="342"/>
-      <c r="E1" s="343"/>
-      <c r="F1" s="342"/>
-      <c r="G1" s="342"/>
+      <c r="C1" s="388"/>
+      <c r="D1" s="388"/>
+      <c r="E1" s="389"/>
+      <c r="F1" s="388"/>
+      <c r="G1" s="388"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
@@ -7509,11 +7789,11 @@
       <c r="K2" s="204" t="s">
         <v>64</v>
       </c>
-      <c r="L2" s="254" t="s">
+      <c r="L2" s="253" t="s">
         <v>64</v>
       </c>
-      <c r="M2" s="255"/>
-      <c r="N2" s="255"/>
+      <c r="M2" s="254"/>
+      <c r="N2" s="254"/>
     </row>
     <row r="3" spans="1:19" ht="71.25" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="205">
@@ -7525,7 +7805,7 @@
       <c r="C3" s="207">
         <v>2015</v>
       </c>
-      <c r="D3" s="256" t="s">
+      <c r="D3" s="255" t="s">
         <v>32</v>
       </c>
       <c r="E3" s="208" t="s">
@@ -7561,7 +7841,7 @@
       <c r="C4" s="207">
         <v>2019</v>
       </c>
-      <c r="D4" s="291" t="s">
+      <c r="D4" s="290" t="s">
         <v>251</v>
       </c>
       <c r="E4" s="208" t="s">
@@ -7591,7 +7871,7 @@
       <c r="C5" s="215">
         <v>2012</v>
       </c>
-      <c r="D5" s="257" t="s">
+      <c r="D5" s="256" t="s">
         <v>180</v>
       </c>
       <c r="E5" s="216" t="s">
@@ -7643,7 +7923,7 @@
       <c r="C7" s="220">
         <v>2012</v>
       </c>
-      <c r="D7" s="258" t="s">
+      <c r="D7" s="257" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="216" t="s">
@@ -7671,7 +7951,7 @@
       <c r="C8" s="222">
         <v>2011</v>
       </c>
-      <c r="D8" s="259" t="s">
+      <c r="D8" s="258" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="223" t="s">
@@ -7699,7 +7979,7 @@
       <c r="C9" s="219">
         <v>2017</v>
       </c>
-      <c r="D9" s="290" t="s">
+      <c r="D9" s="289" t="s">
         <v>44</v>
       </c>
       <c r="E9" s="216" t="s">
@@ -7726,7 +8006,7 @@
       <c r="C10" s="226">
         <v>2010</v>
       </c>
-      <c r="D10" s="260" t="s">
+      <c r="D10" s="259" t="s">
         <v>75</v>
       </c>
       <c r="E10" s="216" t="s">
@@ -7748,13 +8028,13 @@
       <c r="A11" s="205">
         <v>8</v>
       </c>
-      <c r="B11" s="327" t="s">
+      <c r="B11" s="326" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="327">
+      <c r="C11" s="326">
         <v>2020</v>
       </c>
-      <c r="D11" s="328" t="s">
+      <c r="D11" s="327" t="s">
         <v>341</v>
       </c>
       <c r="E11" s="216" t="s">
@@ -7767,7 +8047,7 @@
       <c r="H11" s="106" t="s">
         <v>320</v>
       </c>
-      <c r="I11" s="288" t="s">
+      <c r="I11" s="287" t="s">
         <v>342</v>
       </c>
       <c r="J11" s="212"/>
@@ -7791,7 +8071,7 @@
       <c r="C12" s="215">
         <v>2018</v>
       </c>
-      <c r="D12" s="262" t="s">
+      <c r="D12" s="261" t="s">
         <v>56</v>
       </c>
       <c r="E12" s="216" t="s">
@@ -7806,8 +8086,8 @@
       <c r="H12" s="228"/>
       <c r="I12" s="137"/>
       <c r="J12" s="137"/>
-      <c r="K12" s="344"/>
-      <c r="L12" s="345"/>
+      <c r="K12" s="390"/>
+      <c r="L12" s="391"/>
       <c r="M12" s="213"/>
       <c r="N12" s="213"/>
       <c r="O12" s="213"/>
@@ -7826,7 +8106,7 @@
       <c r="C13" s="215">
         <v>2020</v>
       </c>
-      <c r="D13" s="262" t="s">
+      <c r="D13" s="261" t="s">
         <v>236</v>
       </c>
       <c r="E13" s="216" t="s">
@@ -7861,7 +8141,7 @@
       <c r="C14" s="232">
         <v>2018</v>
       </c>
-      <c r="D14" s="263" t="s">
+      <c r="D14" s="262" t="s">
         <v>60</v>
       </c>
       <c r="E14" s="208" t="s">
@@ -7876,7 +8156,7 @@
       <c r="H14" s="137" t="s">
         <v>265</v>
       </c>
-      <c r="I14" s="270" t="s">
+      <c r="I14" s="269" t="s">
         <v>288</v>
       </c>
       <c r="J14" s="106" t="s">
@@ -7885,7 +8165,7 @@
       <c r="K14" s="100" t="s">
         <v>332</v>
       </c>
-      <c r="L14" s="321"/>
+      <c r="L14" s="320"/>
       <c r="M14" s="212"/>
       <c r="N14" s="212"/>
       <c r="O14" s="212"/>
@@ -7904,7 +8184,7 @@
       <c r="C15" s="232">
         <v>2018</v>
       </c>
-      <c r="D15" s="263" t="s">
+      <c r="D15" s="262" t="s">
         <v>91</v>
       </c>
       <c r="E15" s="208" t="s">
@@ -7922,13 +8202,13 @@
       <c r="I15" s="137" t="s">
         <v>280</v>
       </c>
-      <c r="J15" s="270" t="s">
+      <c r="J15" s="269" t="s">
         <v>289</v>
       </c>
-      <c r="K15" s="314" t="s">
+      <c r="K15" s="313" t="s">
         <v>315</v>
       </c>
-      <c r="L15" s="320"/>
+      <c r="L15" s="319"/>
       <c r="M15" s="106"/>
       <c r="N15" s="106"/>
       <c r="O15" s="212"/>
@@ -7947,7 +8227,7 @@
       <c r="C16" s="232">
         <v>2019</v>
       </c>
-      <c r="D16" s="263" t="s">
+      <c r="D16" s="262" t="s">
         <v>129</v>
       </c>
       <c r="E16" s="208" t="s">
@@ -7960,13 +8240,13 @@
       <c r="H16" s="106" t="s">
         <v>268</v>
       </c>
-      <c r="I16" s="270" t="s">
+      <c r="I16" s="269" t="s">
         <v>296</v>
       </c>
       <c r="J16" s="105" t="s">
         <v>331</v>
       </c>
-      <c r="K16" s="321"/>
+      <c r="K16" s="320"/>
       <c r="L16" s="212"/>
       <c r="M16" s="212"/>
       <c r="N16" s="212"/>
@@ -7986,7 +8266,7 @@
       <c r="C17" s="232">
         <v>2015</v>
       </c>
-      <c r="D17" s="263" t="s">
+      <c r="D17" s="262" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="236" t="s">
@@ -8007,7 +8287,7 @@
       <c r="J17" s="106" t="s">
         <v>286</v>
       </c>
-      <c r="K17" s="305" t="s">
+      <c r="K17" s="304" t="s">
         <v>317</v>
       </c>
       <c r="L17" s="100" t="s">
@@ -8031,7 +8311,7 @@
       <c r="C18" s="232">
         <v>2015</v>
       </c>
-      <c r="D18" s="326" t="s">
+      <c r="D18" s="325" t="s">
         <v>339</v>
       </c>
       <c r="E18" s="236" t="s">
@@ -8046,13 +8326,13 @@
       <c r="H18" s="106" t="s">
         <v>269</v>
       </c>
-      <c r="I18" s="317" t="s">
+      <c r="I18" s="316" t="s">
         <v>322</v>
       </c>
-      <c r="J18" s="316" t="s">
+      <c r="J18" s="315" t="s">
         <v>321</v>
       </c>
-      <c r="K18" s="322"/>
+      <c r="K18" s="321"/>
       <c r="L18" s="106"/>
       <c r="M18" s="99"/>
       <c r="N18" s="137"/>
@@ -8072,7 +8352,7 @@
       <c r="C19" s="232">
         <v>2017</v>
       </c>
-      <c r="D19" s="263" t="s">
+      <c r="D19" s="262" t="s">
         <v>36</v>
       </c>
       <c r="E19" s="236" t="s">
@@ -8084,19 +8364,19 @@
       <c r="G19" s="233" t="s">
         <v>82</v>
       </c>
-      <c r="H19" s="270" t="s">
+      <c r="H19" s="269" t="s">
         <v>252</v>
       </c>
-      <c r="I19" s="305" t="s">
+      <c r="I19" s="304" t="s">
         <v>262</v>
       </c>
-      <c r="J19" s="305" t="s">
+      <c r="J19" s="304" t="s">
         <v>283</v>
       </c>
       <c r="K19" s="106" t="s">
         <v>285</v>
       </c>
-      <c r="L19" s="305" t="s">
+      <c r="L19" s="304" t="s">
         <v>313</v>
       </c>
       <c r="M19" s="105" t="s">
@@ -8119,31 +8399,31 @@
       <c r="C20" s="232">
         <v>2017</v>
       </c>
-      <c r="D20" s="263" t="s">
+      <c r="D20" s="262" t="s">
         <v>38</v>
       </c>
       <c r="E20" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F20" s="239" t="s">
+      <c r="F20" s="238" t="s">
         <v>19</v>
       </c>
       <c r="G20" s="233" t="s">
         <v>83</v>
       </c>
-      <c r="H20" s="305" t="s">
+      <c r="H20" s="304" t="s">
         <v>270</v>
       </c>
-      <c r="I20" s="305" t="s">
+      <c r="I20" s="304" t="s">
         <v>278</v>
       </c>
-      <c r="J20" s="318" t="s">
+      <c r="J20" s="317" t="s">
         <v>295</v>
       </c>
       <c r="K20" s="100" t="s">
         <v>324</v>
       </c>
-      <c r="L20" s="323"/>
+      <c r="L20" s="322"/>
       <c r="M20" s="213"/>
       <c r="N20" s="213"/>
       <c r="O20" s="137"/>
@@ -8162,22 +8442,22 @@
       <c r="C21" s="232">
         <v>2017</v>
       </c>
-      <c r="D21" s="263" t="s">
+      <c r="D21" s="262" t="s">
         <v>40</v>
       </c>
       <c r="E21" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F21" s="240" t="s">
+      <c r="F21" s="239" t="s">
         <v>5</v>
       </c>
       <c r="G21" s="233" t="s">
         <v>79</v>
       </c>
-      <c r="H21" s="305" t="s">
+      <c r="H21" s="304" t="s">
         <v>261</v>
       </c>
-      <c r="I21" s="288" t="s">
+      <c r="I21" s="287" t="s">
         <v>298</v>
       </c>
       <c r="J21" s="100" t="s">
@@ -8198,13 +8478,13 @@
       <c r="A22" s="205">
         <v>19</v>
       </c>
-      <c r="B22" s="258" t="s">
+      <c r="B22" s="257" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="232">
         <v>2018</v>
       </c>
-      <c r="D22" s="289" t="s">
+      <c r="D22" s="288" t="s">
         <v>54</v>
       </c>
       <c r="E22" s="208" t="s">
@@ -8214,7 +8494,7 @@
         <v>27</v>
       </c>
       <c r="G22" s="224"/>
-      <c r="H22" s="305" t="s">
+      <c r="H22" s="304" t="s">
         <v>259</v>
       </c>
       <c r="I22" s="105" t="s">
@@ -8236,13 +8516,13 @@
       <c r="A23" s="205">
         <v>20</v>
       </c>
-      <c r="B23" s="241" t="s">
+      <c r="B23" s="240" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="241">
+      <c r="C23" s="240">
         <v>2006</v>
       </c>
-      <c r="D23" s="264" t="s">
+      <c r="D23" s="263" t="s">
         <v>16</v>
       </c>
       <c r="E23" s="216" t="s">
@@ -8270,13 +8550,13 @@
       <c r="A24" s="205">
         <v>21</v>
       </c>
-      <c r="B24" s="242" t="s">
+      <c r="B24" s="241" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="242">
+      <c r="C24" s="241">
         <v>2016</v>
       </c>
-      <c r="D24" s="265" t="s">
+      <c r="D24" s="264" t="s">
         <v>23</v>
       </c>
       <c r="E24" s="216" t="s">
@@ -8285,10 +8565,10 @@
       <c r="F24" s="209" t="s">
         <v>55</v>
       </c>
-      <c r="G24" s="243" t="s">
+      <c r="G24" s="242" t="s">
         <v>80</v>
       </c>
-      <c r="H24" s="294" t="s">
+      <c r="H24" s="293" t="s">
         <v>274</v>
       </c>
       <c r="I24" s="137"/>
@@ -8314,7 +8594,7 @@
       <c r="C25" s="219">
         <v>2017</v>
       </c>
-      <c r="D25" s="261" t="s">
+      <c r="D25" s="260" t="s">
         <v>25</v>
       </c>
       <c r="E25" s="216" t="s">
@@ -8326,7 +8606,7 @@
       <c r="G25" s="206" t="s">
         <v>78</v>
       </c>
-      <c r="H25" s="293" t="s">
+      <c r="H25" s="292" t="s">
         <v>273</v>
       </c>
       <c r="I25" s="137"/>
@@ -8352,13 +8632,13 @@
       <c r="C26" s="219">
         <v>2018</v>
       </c>
-      <c r="D26" s="290" t="s">
+      <c r="D26" s="289" t="s">
         <v>58</v>
       </c>
       <c r="E26" s="216" t="s">
         <v>74</v>
       </c>
-      <c r="F26" s="244" t="s">
+      <c r="F26" s="243" t="s">
         <v>199</v>
       </c>
       <c r="G26" s="206" t="s">
@@ -8367,13 +8647,13 @@
       <c r="H26" s="106" t="s">
         <v>247</v>
       </c>
-      <c r="I26" s="270" t="s">
+      <c r="I26" s="269" t="s">
         <v>294</v>
       </c>
       <c r="J26" s="105" t="s">
         <v>333</v>
       </c>
-      <c r="K26" s="321"/>
+      <c r="K26" s="320"/>
       <c r="L26" s="213"/>
       <c r="M26" s="213"/>
       <c r="N26" s="213"/>
@@ -8394,13 +8674,13 @@
       <c r="C27" s="232">
         <v>2015</v>
       </c>
-      <c r="D27" s="263" t="s">
+      <c r="D27" s="262" t="s">
         <v>2</v>
       </c>
       <c r="E27" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F27" s="245" t="s">
+      <c r="F27" s="244" t="s">
         <v>142</v>
       </c>
       <c r="G27" s="218" t="s">
@@ -8409,10 +8689,10 @@
       <c r="H27" s="106" t="s">
         <v>266</v>
       </c>
-      <c r="I27" s="308" t="s">
+      <c r="I27" s="307" t="s">
         <v>301</v>
       </c>
-      <c r="J27" s="324" t="s">
+      <c r="J27" s="323" t="s">
         <v>335</v>
       </c>
       <c r="K27" s="221"/>
@@ -8436,7 +8716,7 @@
       <c r="C28" s="232">
         <v>2015</v>
       </c>
-      <c r="D28" s="263" t="s">
+      <c r="D28" s="262" t="s">
         <v>3</v>
       </c>
       <c r="E28" s="236" t="s">
@@ -8448,7 +8728,7 @@
       <c r="G28" s="218" t="s">
         <v>70</v>
       </c>
-      <c r="H28" s="270" t="s">
+      <c r="H28" s="269" t="s">
         <v>258</v>
       </c>
       <c r="I28" s="137" t="s">
@@ -8457,7 +8737,7 @@
       <c r="J28" s="100" t="s">
         <v>329</v>
       </c>
-      <c r="K28" s="323"/>
+      <c r="K28" s="322"/>
       <c r="L28" s="106"/>
       <c r="M28" s="137"/>
       <c r="N28" s="137"/>
@@ -8478,13 +8758,13 @@
       <c r="C29" s="232">
         <v>2015</v>
       </c>
-      <c r="D29" s="263" t="s">
+      <c r="D29" s="262" t="s">
         <v>4</v>
       </c>
       <c r="E29" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F29" s="246" t="s">
+      <c r="F29" s="245" t="s">
         <v>110</v>
       </c>
       <c r="G29" s="218" t="s">
@@ -8493,13 +8773,13 @@
       <c r="H29" s="137" t="s">
         <v>257</v>
       </c>
-      <c r="I29" s="270" t="s">
+      <c r="I29" s="269" t="s">
         <v>291</v>
       </c>
       <c r="J29" s="105" t="s">
         <v>326</v>
       </c>
-      <c r="K29" s="321"/>
+      <c r="K29" s="320"/>
       <c r="L29" s="137"/>
       <c r="M29" s="137"/>
       <c r="N29" s="99"/>
@@ -8520,7 +8800,7 @@
       <c r="C30" s="232">
         <v>2015</v>
       </c>
-      <c r="D30" s="263" t="s">
+      <c r="D30" s="262" t="s">
         <v>6</v>
       </c>
       <c r="E30" s="236" t="s">
@@ -8541,16 +8821,16 @@
       <c r="J30" s="137" t="s">
         <v>282</v>
       </c>
-      <c r="K30" s="305" t="s">
+      <c r="K30" s="304" t="s">
         <v>292</v>
       </c>
-      <c r="L30" s="270" t="s">
+      <c r="L30" s="269" t="s">
         <v>316</v>
       </c>
       <c r="M30" s="137" t="s">
         <v>327</v>
       </c>
-      <c r="N30" s="324" t="s">
+      <c r="N30" s="323" t="s">
         <v>330</v>
       </c>
       <c r="O30" s="137"/>
@@ -8570,13 +8850,13 @@
       <c r="C31" s="232">
         <v>2015</v>
       </c>
-      <c r="D31" s="263" t="s">
+      <c r="D31" s="262" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="244" t="s">
+      <c r="F31" s="243" t="s">
         <v>151</v>
       </c>
       <c r="G31" s="218" t="s">
@@ -8585,10 +8865,10 @@
       <c r="H31" s="106" t="s">
         <v>246</v>
       </c>
-      <c r="I31" s="306" t="s">
+      <c r="I31" s="305" t="s">
         <v>293</v>
       </c>
-      <c r="J31" s="325" t="s">
+      <c r="J31" s="324" t="s">
         <v>337</v>
       </c>
       <c r="K31" s="152"/>
@@ -8612,7 +8892,7 @@
       <c r="C32" s="232">
         <v>2016</v>
       </c>
-      <c r="D32" s="263" t="s">
+      <c r="D32" s="262" t="s">
         <v>20</v>
       </c>
       <c r="E32" s="236" t="s">
@@ -8630,10 +8910,10 @@
       <c r="I32" s="106" t="s">
         <v>263</v>
       </c>
-      <c r="J32" s="305" t="s">
+      <c r="J32" s="304" t="s">
         <v>279</v>
       </c>
-      <c r="K32" s="307" t="s">
+      <c r="K32" s="306" t="s">
         <v>287</v>
       </c>
       <c r="L32" s="106" t="s">
@@ -8660,7 +8940,7 @@
       <c r="C33" s="232">
         <v>2018</v>
       </c>
-      <c r="D33" s="263" t="s">
+      <c r="D33" s="262" t="s">
         <v>61</v>
       </c>
       <c r="E33" s="208" t="s">
@@ -8675,21 +8955,21 @@
       <c r="H33" s="137" t="s">
         <v>264</v>
       </c>
-      <c r="I33" s="247" t="s">
+      <c r="I33" s="246" t="s">
         <v>281</v>
       </c>
       <c r="J33" s="106" t="s">
         <v>284</v>
       </c>
-      <c r="K33" s="319" t="s">
+      <c r="K33" s="318" t="s">
         <v>300</v>
       </c>
-      <c r="L33" s="292" t="s">
+      <c r="L33" s="291" t="s">
         <v>325</v>
       </c>
-      <c r="M33" s="325"/>
+      <c r="M33" s="324"/>
       <c r="N33" s="137"/>
-      <c r="O33" s="253"/>
+      <c r="O33" s="252"/>
       <c r="P33" s="106"/>
       <c r="Q33" s="137"/>
       <c r="R33" s="213"/>
@@ -8703,27 +8983,27 @@
       <c r="B34" s="207" t="s">
         <v>184</v>
       </c>
-      <c r="C34" s="249" t="s">
+      <c r="C34" s="248" t="s">
         <v>195</v>
       </c>
-      <c r="D34" s="256" t="s">
+      <c r="D34" s="255" t="s">
         <v>185</v>
       </c>
-      <c r="E34" s="299" t="s">
+      <c r="E34" s="298" t="s">
         <v>74</v>
       </c>
-      <c r="F34" s="300" t="s">
+      <c r="F34" s="299" t="s">
         <v>318</v>
       </c>
       <c r="G34" s="218"/>
-      <c r="H34" s="270" t="s">
+      <c r="H34" s="269" t="s">
         <v>277</v>
       </c>
-      <c r="I34" s="315" t="s">
+      <c r="I34" s="314" t="s">
         <v>319</v>
       </c>
       <c r="J34" s="106"/>
-      <c r="K34" s="248"/>
+      <c r="K34" s="247"/>
       <c r="L34" s="137"/>
       <c r="M34" s="137"/>
       <c r="N34" s="213"/>
@@ -8738,118 +9018,118 @@
       <c r="A35" s="205">
         <v>30</v>
       </c>
-      <c r="B35" s="312" t="s">
+      <c r="B35" s="311" t="s">
         <v>311</v>
       </c>
-      <c r="C35" s="298" t="s">
+      <c r="C35" s="297" t="s">
         <v>275</v>
       </c>
-      <c r="D35" s="303" t="s">
+      <c r="D35" s="302" t="s">
         <v>302</v>
       </c>
-      <c r="E35" s="304" t="s">
+      <c r="E35" s="303" t="s">
         <v>276</v>
       </c>
-      <c r="F35" s="276" t="s">
+      <c r="F35" s="275" t="s">
         <v>304</v>
       </c>
       <c r="G35" s="218"/>
       <c r="H35" s="137" t="s">
         <v>305</v>
       </c>
-      <c r="I35" s="315" t="s">
+      <c r="I35" s="314" t="s">
         <v>323</v>
       </c>
       <c r="J35" s="106"/>
-      <c r="K35" s="248"/>
+      <c r="K35" s="247"/>
       <c r="L35" s="137"/>
-      <c r="M35" s="295"/>
-      <c r="N35" s="296"/>
-      <c r="O35" s="296"/>
-      <c r="P35" s="296"/>
-      <c r="Q35" s="296"/>
-      <c r="R35" s="296"/>
-      <c r="S35" s="296"/>
+      <c r="M35" s="294"/>
+      <c r="N35" s="295"/>
+      <c r="O35" s="295"/>
+      <c r="P35" s="295"/>
+      <c r="Q35" s="295"/>
+      <c r="R35" s="295"/>
+      <c r="S35" s="295"/>
       <c r="T35" s="214"/>
     </row>
     <row r="36" spans="1:20" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="205">
         <v>31</v>
       </c>
-      <c r="B36" s="312" t="s">
+      <c r="B36" s="311" t="s">
         <v>310</v>
       </c>
-      <c r="C36" s="249" t="s">
+      <c r="C36" s="248" t="s">
         <v>275</v>
       </c>
-      <c r="D36" s="303" t="s">
+      <c r="D36" s="302" t="s">
         <v>303</v>
       </c>
-      <c r="E36" s="304" t="s">
+      <c r="E36" s="303" t="s">
         <v>276</v>
       </c>
-      <c r="F36" s="276" t="s">
+      <c r="F36" s="275" t="s">
         <v>55</v>
       </c>
       <c r="G36" s="218"/>
       <c r="H36" s="105" t="s">
         <v>306</v>
       </c>
-      <c r="I36" s="247"/>
+      <c r="I36" s="246"/>
       <c r="J36" s="106"/>
-      <c r="K36" s="248"/>
+      <c r="K36" s="247"/>
       <c r="L36" s="137"/>
-      <c r="M36" s="295"/>
-      <c r="N36" s="296"/>
-      <c r="O36" s="296"/>
-      <c r="P36" s="296"/>
-      <c r="Q36" s="296"/>
-      <c r="R36" s="296"/>
-      <c r="S36" s="296"/>
+      <c r="M36" s="294"/>
+      <c r="N36" s="295"/>
+      <c r="O36" s="295"/>
+      <c r="P36" s="295"/>
+      <c r="Q36" s="295"/>
+      <c r="R36" s="295"/>
+      <c r="S36" s="295"/>
       <c r="T36" s="214"/>
     </row>
     <row r="37" spans="1:20" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="205">
         <v>32</v>
       </c>
-      <c r="B37" s="297" t="s">
+      <c r="B37" s="296" t="s">
         <v>307</v>
       </c>
-      <c r="C37" s="311" t="s">
+      <c r="C37" s="310" t="s">
         <v>309</v>
       </c>
-      <c r="D37" s="309" t="s">
+      <c r="D37" s="308" t="s">
         <v>308</v>
       </c>
-      <c r="E37" s="313" t="s">
+      <c r="E37" s="312" t="s">
         <v>312</v>
       </c>
-      <c r="F37" s="310" t="s">
+      <c r="F37" s="309" t="s">
         <v>26</v>
       </c>
       <c r="G37" s="218"/>
-      <c r="H37" s="325"/>
-      <c r="I37" s="247"/>
+      <c r="H37" s="324"/>
+      <c r="I37" s="246"/>
       <c r="J37" s="106"/>
-      <c r="K37" s="248"/>
+      <c r="K37" s="247"/>
       <c r="L37" s="137"/>
-      <c r="M37" s="295"/>
-      <c r="N37" s="296"/>
-      <c r="O37" s="296"/>
-      <c r="P37" s="296"/>
-      <c r="Q37" s="296"/>
-      <c r="R37" s="296"/>
-      <c r="S37" s="296"/>
+      <c r="M37" s="294"/>
+      <c r="N37" s="295"/>
+      <c r="O37" s="295"/>
+      <c r="P37" s="295"/>
+      <c r="Q37" s="295"/>
+      <c r="R37" s="295"/>
+      <c r="S37" s="295"/>
       <c r="T37" s="214"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A38" s="205"/>
-      <c r="B38" s="250"/>
-      <c r="C38" s="250"/>
-      <c r="D38" s="301"/>
-      <c r="E38" s="251"/>
-      <c r="F38" s="302"/>
-      <c r="G38" s="252"/>
+      <c r="B38" s="249"/>
+      <c r="C38" s="249"/>
+      <c r="D38" s="300"/>
+      <c r="E38" s="250"/>
+      <c r="F38" s="301"/>
+      <c r="G38" s="251"/>
       <c r="H38" s="212"/>
       <c r="I38" s="212"/>
       <c r="J38" s="212"/>
@@ -8873,10 +9153,10 @@
   <sheetPr>
     <tabColor rgb="FFCC6600"/>
   </sheetPr>
-  <dimension ref="A1:T29"/>
+  <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C26" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -8884,14 +9164,14 @@
     <col min="1" max="1" width="5.5703125" style="198" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" style="199" customWidth="1"/>
     <col min="3" max="3" width="15" style="214" customWidth="1"/>
-    <col min="4" max="4" width="16" style="287" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="286" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" style="199" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.85546875" style="199" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" style="199" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" style="268" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" style="267" customWidth="1"/>
     <col min="9" max="9" width="21.85546875" style="214" customWidth="1"/>
     <col min="10" max="10" width="23.28515625" style="214" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" style="214" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="214" customWidth="1"/>
     <col min="12" max="12" width="20" style="214" customWidth="1"/>
     <col min="13" max="13" width="17.85546875" style="199" customWidth="1"/>
     <col min="14" max="14" width="18.85546875" style="199" customWidth="1"/>
@@ -8903,24 +9183,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="342" t="s">
+      <c r="B1" s="388" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="342"/>
-      <c r="D1" s="342"/>
-      <c r="E1" s="343"/>
-      <c r="F1" s="342"/>
-      <c r="G1" s="342"/>
+      <c r="C1" s="388"/>
+      <c r="D1" s="388"/>
+      <c r="E1" s="389"/>
+      <c r="F1" s="388"/>
+      <c r="G1" s="388"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
       <c r="B2" s="201" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="269" t="s">
+      <c r="C2" s="268" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="273" t="s">
+      <c r="D2" s="272" t="s">
         <v>49</v>
       </c>
       <c r="E2" s="202" t="s">
@@ -8944,11 +9224,11 @@
       <c r="K2" s="204" t="s">
         <v>64</v>
       </c>
-      <c r="L2" s="254" t="s">
+      <c r="L2" s="253" t="s">
         <v>64</v>
       </c>
-      <c r="M2" s="255"/>
-      <c r="N2" s="255"/>
+      <c r="M2" s="254"/>
+      <c r="N2" s="254"/>
     </row>
     <row r="3" spans="1:19" ht="76.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="205">
@@ -8957,10 +9237,10 @@
       <c r="B3" s="206" t="s">
         <v>250</v>
       </c>
-      <c r="C3" s="274">
+      <c r="C3" s="273">
         <v>2019</v>
       </c>
-      <c r="D3" s="275" t="s">
+      <c r="D3" s="274" t="s">
         <v>251</v>
       </c>
       <c r="E3" s="208" t="s">
@@ -8987,10 +9267,10 @@
       <c r="B4" s="215" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="276">
+      <c r="C4" s="275">
         <v>2012</v>
       </c>
-      <c r="D4" s="277" t="s">
+      <c r="D4" s="276" t="s">
         <v>180</v>
       </c>
       <c r="E4" s="216" t="s">
@@ -9000,7 +9280,7 @@
         <v>28</v>
       </c>
       <c r="G4" s="218"/>
-      <c r="H4" s="271"/>
+      <c r="H4" s="270"/>
       <c r="I4" s="213"/>
       <c r="J4" s="213"/>
       <c r="K4" s="213"/>
@@ -9026,7 +9306,7 @@
         <v>28</v>
       </c>
       <c r="G5" s="218"/>
-      <c r="H5" s="271"/>
+      <c r="H5" s="270"/>
       <c r="I5" s="213"/>
       <c r="J5" s="213"/>
       <c r="K5" s="213"/>
@@ -9039,10 +9319,10 @@
       <c r="B6" s="215" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="276">
+      <c r="C6" s="275">
         <v>2020</v>
       </c>
-      <c r="D6" s="278" t="s">
+      <c r="D6" s="277" t="s">
         <v>236</v>
       </c>
       <c r="E6" s="216" t="s">
@@ -9052,7 +9332,7 @@
         <v>28</v>
       </c>
       <c r="G6" s="218"/>
-      <c r="H6" s="270" t="s">
+      <c r="H6" s="269" t="s">
         <v>256</v>
       </c>
       <c r="I6" s="213"/>
@@ -9067,10 +9347,10 @@
       <c r="B7" s="219" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="279">
+      <c r="C7" s="278">
         <v>2012</v>
       </c>
-      <c r="D7" s="280" t="s">
+      <c r="D7" s="279" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="216" t="s">
@@ -9082,7 +9362,7 @@
       <c r="G7" s="206" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="272"/>
+      <c r="H7" s="271"/>
       <c r="I7" s="137"/>
       <c r="J7" s="221"/>
       <c r="K7" s="213"/>
@@ -9092,13 +9372,13 @@
       <c r="A8" s="205">
         <v>6</v>
       </c>
-      <c r="B8" s="327" t="s">
+      <c r="B8" s="326" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="327">
+      <c r="C8" s="326">
         <v>2020</v>
       </c>
-      <c r="D8" s="328" t="s">
+      <c r="D8" s="327" t="s">
         <v>341</v>
       </c>
       <c r="E8" s="216" t="s">
@@ -9111,7 +9391,7 @@
       <c r="H8" s="106" t="s">
         <v>320</v>
       </c>
-      <c r="I8" s="288" t="s">
+      <c r="I8" s="287" t="s">
         <v>342</v>
       </c>
       <c r="J8" s="221"/>
@@ -9125,10 +9405,10 @@
       <c r="B9" s="222" t="s">
         <v>168</v>
       </c>
-      <c r="C9" s="281">
+      <c r="C9" s="280">
         <v>2011</v>
       </c>
-      <c r="D9" s="282" t="s">
+      <c r="D9" s="281" t="s">
         <v>18</v>
       </c>
       <c r="E9" s="223" t="s">
@@ -9140,7 +9420,7 @@
       <c r="G9" s="218" t="s">
         <v>77</v>
       </c>
-      <c r="H9" s="329" t="s">
+      <c r="H9" s="328" t="s">
         <v>255</v>
       </c>
       <c r="I9" s="106"/>
@@ -9155,11 +9435,11 @@
       <c r="B10" s="231" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="274">
+      <c r="C10" s="273">
         <v>2018</v>
       </c>
-      <c r="D10" s="284" t="s">
-        <v>60</v>
+      <c r="D10" s="277" t="s">
+        <v>457</v>
       </c>
       <c r="E10" s="208" t="s">
         <v>74</v>
@@ -9173,13 +9453,15 @@
       <c r="H10" s="106" t="s">
         <v>332</v>
       </c>
-      <c r="I10" s="334" t="s">
+      <c r="I10" s="332" t="s">
         <v>350</v>
       </c>
-      <c r="J10" s="100" t="s">
+      <c r="J10" s="106" t="s">
         <v>353</v>
       </c>
-      <c r="K10" s="106"/>
+      <c r="K10" s="287" t="s">
+        <v>458</v>
+      </c>
       <c r="L10" s="213"/>
       <c r="M10" s="212"/>
       <c r="N10" s="212"/>
@@ -9196,10 +9478,10 @@
       <c r="B11" s="231" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="274">
+      <c r="C11" s="273">
         <v>2018</v>
       </c>
-      <c r="D11" s="278" t="s">
+      <c r="D11" s="277" t="s">
         <v>351</v>
       </c>
       <c r="E11" s="208" t="s">
@@ -9211,10 +9493,10 @@
       <c r="G11" s="233" t="s">
         <v>93</v>
       </c>
-      <c r="H11" s="335" t="s">
+      <c r="H11" s="333" t="s">
         <v>315</v>
       </c>
-      <c r="I11" s="270" t="s">
+      <c r="I11" s="269" t="s">
         <v>354</v>
       </c>
       <c r="J11" s="100" t="s">
@@ -9237,10 +9519,10 @@
       <c r="B12" s="231" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="274">
+      <c r="C12" s="273">
         <v>2019</v>
       </c>
-      <c r="D12" s="284" t="s">
+      <c r="D12" s="283" t="s">
         <v>129</v>
       </c>
       <c r="E12" s="208" t="s">
@@ -9272,10 +9554,10 @@
       <c r="B13" s="232" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="274">
+      <c r="C13" s="273">
         <v>2015</v>
       </c>
-      <c r="D13" s="278" t="s">
+      <c r="D13" s="277" t="s">
         <v>357</v>
       </c>
       <c r="E13" s="236" t="s">
@@ -9290,7 +9572,7 @@
       <c r="H13" s="106" t="s">
         <v>334</v>
       </c>
-      <c r="I13" s="288" t="s">
+      <c r="I13" s="287" t="s">
         <v>364</v>
       </c>
       <c r="J13" s="137"/>
@@ -9311,10 +9593,10 @@
       <c r="B14" s="232" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="274">
+      <c r="C14" s="273">
         <v>2015</v>
       </c>
-      <c r="D14" s="326" t="s">
+      <c r="D14" s="325" t="s">
         <v>347</v>
       </c>
       <c r="E14" s="236" t="s">
@@ -9326,14 +9608,16 @@
       <c r="G14" s="218" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="332" t="s">
+      <c r="H14" s="331" t="s">
         <v>321</v>
       </c>
-      <c r="I14" s="333" t="s">
+      <c r="I14" s="399" t="s">
         <v>348</v>
       </c>
-      <c r="J14" s="238"/>
-      <c r="K14" s="267"/>
+      <c r="J14" s="398" t="s">
+        <v>471</v>
+      </c>
+      <c r="K14" s="266"/>
       <c r="L14" s="106"/>
       <c r="M14" s="99"/>
       <c r="N14" s="137"/>
@@ -9350,23 +9634,23 @@
       <c r="B15" s="232" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="274">
+      <c r="C15" s="273">
         <v>2017</v>
       </c>
-      <c r="D15" s="278" t="s">
+      <c r="D15" s="277" t="s">
         <v>358</v>
       </c>
       <c r="E15" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="330"/>
+      <c r="F15" s="329"/>
       <c r="G15" s="233" t="s">
         <v>82</v>
       </c>
       <c r="H15" s="137" t="s">
         <v>328</v>
       </c>
-      <c r="I15" s="288" t="s">
+      <c r="I15" s="287" t="s">
         <v>359</v>
       </c>
       <c r="J15" s="137"/>
@@ -9387,16 +9671,16 @@
       <c r="B16" s="232" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="274">
+      <c r="C16" s="273">
         <v>2017</v>
       </c>
-      <c r="D16" s="284" t="s">
+      <c r="D16" s="283" t="s">
         <v>38</v>
       </c>
       <c r="E16" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F16" s="239" t="s">
+      <c r="F16" s="238" t="s">
         <v>19</v>
       </c>
       <c r="G16" s="233" t="s">
@@ -9405,7 +9689,7 @@
       <c r="H16" s="106" t="s">
         <v>324</v>
       </c>
-      <c r="I16" s="288" t="s">
+      <c r="I16" s="287" t="s">
         <v>360</v>
       </c>
       <c r="J16" s="99"/>
@@ -9426,16 +9710,16 @@
       <c r="B17" s="232" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="274">
+      <c r="C17" s="273">
         <v>2017</v>
       </c>
-      <c r="D17" s="284" t="s">
+      <c r="D17" s="283" t="s">
         <v>40</v>
       </c>
       <c r="E17" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="240" t="s">
+      <c r="F17" s="239" t="s">
         <v>5</v>
       </c>
       <c r="G17" s="233" t="s">
@@ -9461,13 +9745,13 @@
       <c r="A18" s="205">
         <v>16</v>
       </c>
-      <c r="B18" s="258" t="s">
+      <c r="B18" s="257" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="274">
+      <c r="C18" s="273">
         <v>2018</v>
       </c>
-      <c r="D18" s="284" t="s">
+      <c r="D18" s="283" t="s">
         <v>54</v>
       </c>
       <c r="E18" s="208" t="s">
@@ -9480,7 +9764,7 @@
       <c r="H18" s="137" t="s">
         <v>297</v>
       </c>
-      <c r="I18" s="292" t="s">
+      <c r="I18" s="291" t="s">
         <v>366</v>
       </c>
       <c r="J18" s="137"/>
@@ -9499,13 +9783,13 @@
       <c r="A19" s="205">
         <v>17</v>
       </c>
-      <c r="B19" s="241" t="s">
+      <c r="B19" s="240" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="285">
+      <c r="C19" s="284">
         <v>2006</v>
       </c>
-      <c r="D19" s="286" t="s">
+      <c r="D19" s="285" t="s">
         <v>16</v>
       </c>
       <c r="E19" s="216" t="s">
@@ -9515,7 +9799,7 @@
         <v>17</v>
       </c>
       <c r="G19" s="218"/>
-      <c r="H19" s="271" t="s">
+      <c r="H19" s="270" t="s">
         <v>254</v>
       </c>
       <c r="I19" s="213"/>
@@ -9538,22 +9822,22 @@
       <c r="B20" s="219" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="279">
+      <c r="C20" s="278">
         <v>2018</v>
       </c>
-      <c r="D20" s="283" t="s">
+      <c r="D20" s="282" t="s">
         <v>58</v>
       </c>
       <c r="E20" s="216" t="s">
         <v>74</v>
       </c>
-      <c r="F20" s="244" t="s">
+      <c r="F20" s="243" t="s">
         <v>199</v>
       </c>
       <c r="G20" s="206" t="s">
         <v>95</v>
       </c>
-      <c r="H20" s="292" t="s">
+      <c r="H20" s="291" t="s">
         <v>333</v>
       </c>
       <c r="I20" s="137"/>
@@ -9576,10 +9860,10 @@
       <c r="B21" s="232" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="274">
+      <c r="C21" s="273">
         <v>2015</v>
       </c>
-      <c r="D21" s="284" t="s">
+      <c r="D21" s="283" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="236" t="s">
@@ -9614,28 +9898,30 @@
       <c r="B22" s="232" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="274">
+      <c r="C22" s="273">
         <v>2015</v>
       </c>
-      <c r="D22" s="284" t="s">
-        <v>4</v>
+      <c r="D22" s="277" t="s">
+        <v>459</v>
       </c>
       <c r="E22" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="331" t="s">
+      <c r="F22" s="330" t="s">
         <v>51</v>
       </c>
       <c r="G22" s="218" t="s">
         <v>86</v>
       </c>
-      <c r="H22" s="305" t="s">
+      <c r="H22" s="304" t="s">
         <v>326</v>
       </c>
-      <c r="I22" s="288" t="s">
+      <c r="I22" s="269" t="s">
         <v>345</v>
       </c>
-      <c r="J22" s="213"/>
+      <c r="J22" s="287" t="s">
+        <v>470</v>
+      </c>
       <c r="K22" s="213"/>
       <c r="L22" s="137"/>
       <c r="M22" s="137"/>
@@ -9654,22 +9940,22 @@
       <c r="B23" s="232" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="274">
+      <c r="C23" s="273">
         <v>2015</v>
       </c>
-      <c r="D23" s="284" t="s">
-        <v>8</v>
+      <c r="D23" s="277" t="s">
+        <v>460</v>
       </c>
       <c r="E23" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F23" s="244" t="s">
+      <c r="F23" s="243" t="s">
         <v>151</v>
       </c>
       <c r="G23" s="218" t="s">
         <v>85</v>
       </c>
-      <c r="H23" s="288" t="s">
+      <c r="H23" s="287" t="s">
         <v>355</v>
       </c>
       <c r="I23" s="148"/>
@@ -9692,10 +9978,10 @@
       <c r="B24" s="232" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="274">
+      <c r="C24" s="273">
         <v>2016</v>
       </c>
-      <c r="D24" s="278" t="s">
+      <c r="D24" s="277" t="s">
         <v>356</v>
       </c>
       <c r="E24" s="236" t="s">
@@ -9710,10 +9996,10 @@
       <c r="H24" s="106" t="s">
         <v>338</v>
       </c>
-      <c r="I24" s="270" t="s">
+      <c r="I24" s="269" t="s">
         <v>344</v>
       </c>
-      <c r="J24" s="288" t="s">
+      <c r="J24" s="287" t="s">
         <v>362</v>
       </c>
       <c r="K24" s="152"/>
@@ -9734,11 +10020,11 @@
       <c r="B25" s="232" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="274">
+      <c r="C25" s="273">
         <v>2018</v>
       </c>
-      <c r="D25" s="284" t="s">
-        <v>61</v>
+      <c r="D25" s="277" t="s">
+        <v>461</v>
       </c>
       <c r="E25" s="208" t="s">
         <v>74</v>
@@ -9749,147 +10035,277 @@
       <c r="G25" s="218" t="s">
         <v>94</v>
       </c>
-      <c r="H25" s="305" t="s">
+      <c r="H25" s="304" t="s">
         <v>325</v>
       </c>
-      <c r="I25" s="270" t="s">
+      <c r="I25" s="269" t="s">
         <v>346</v>
       </c>
-      <c r="J25" s="288" t="s">
+      <c r="J25" s="287" t="s">
         <v>352</v>
       </c>
-      <c r="K25" s="248"/>
+      <c r="K25" s="247"/>
       <c r="L25" s="137"/>
       <c r="M25" s="137"/>
       <c r="N25" s="137"/>
-      <c r="O25" s="253"/>
+      <c r="O25" s="252"/>
       <c r="P25" s="106"/>
       <c r="Q25" s="137"/>
       <c r="R25" s="213"/>
       <c r="S25" s="213"/>
       <c r="T25" s="214"/>
     </row>
-    <row r="26" spans="1:20" ht="76.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" ht="76.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="205">
         <v>24</v>
       </c>
-      <c r="B26" s="207" t="s">
-        <v>184</v>
-      </c>
-      <c r="C26" s="249" t="s">
-        <v>195</v>
-      </c>
-      <c r="D26" s="256" t="s">
-        <v>185</v>
-      </c>
-      <c r="E26" s="299" t="s">
+      <c r="B26" s="232" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="273">
+        <v>2022</v>
+      </c>
+      <c r="D26" s="285" t="s">
+        <v>463</v>
+      </c>
+      <c r="E26" s="298" t="s">
         <v>74</v>
       </c>
-      <c r="F26" s="300" t="s">
-        <v>318</v>
+      <c r="F26" s="396" t="s">
+        <v>388</v>
       </c>
       <c r="G26" s="218"/>
-      <c r="H26" s="270" t="s">
-        <v>277</v>
-      </c>
-      <c r="I26" s="247" t="s">
-        <v>319</v>
-      </c>
-      <c r="J26" s="270" t="s">
-        <v>349</v>
-      </c>
-      <c r="K26" s="336" t="s">
-        <v>365</v>
-      </c>
+      <c r="H26" s="304"/>
+      <c r="I26" s="269"/>
+      <c r="J26" s="287"/>
+      <c r="K26" s="247"/>
       <c r="L26" s="137"/>
       <c r="M26" s="137"/>
-      <c r="N26" s="213"/>
-      <c r="O26" s="213"/>
-      <c r="P26" s="213"/>
-      <c r="Q26" s="213"/>
+      <c r="N26" s="137"/>
+      <c r="O26" s="252"/>
+      <c r="P26" s="106"/>
+      <c r="Q26" s="137"/>
       <c r="R26" s="213"/>
       <c r="S26" s="213"/>
       <c r="T26" s="214"/>
     </row>
-    <row r="27" spans="1:20" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" ht="76.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="205">
         <v>25</v>
       </c>
-      <c r="B27" s="312" t="s">
-        <v>311</v>
-      </c>
-      <c r="C27" s="298" t="s">
-        <v>275</v>
-      </c>
-      <c r="D27" s="303" t="s">
-        <v>302</v>
-      </c>
-      <c r="E27" s="304" t="s">
-        <v>276</v>
-      </c>
-      <c r="F27" s="276" t="s">
-        <v>304</v>
-      </c>
+      <c r="B27" s="232" t="s">
+        <v>464</v>
+      </c>
+      <c r="C27" s="273">
+        <v>2022</v>
+      </c>
+      <c r="D27" s="285" t="s">
+        <v>467</v>
+      </c>
+      <c r="E27" s="298" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" s="397"/>
       <c r="G27" s="218"/>
-      <c r="H27" s="137" t="s">
-        <v>305</v>
-      </c>
-      <c r="I27" s="315" t="s">
-        <v>323</v>
-      </c>
-      <c r="J27" s="213"/>
-      <c r="K27" s="213"/>
-      <c r="L27" s="213"/>
-    </row>
-    <row r="28" spans="1:20" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="H27" s="304"/>
+      <c r="I27" s="269"/>
+      <c r="J27" s="287"/>
+      <c r="K27" s="247"/>
+      <c r="L27" s="137"/>
+      <c r="M27" s="137"/>
+      <c r="N27" s="137"/>
+      <c r="O27" s="252"/>
+      <c r="P27" s="106"/>
+      <c r="Q27" s="137"/>
+      <c r="R27" s="213"/>
+      <c r="S27" s="213"/>
+      <c r="T27" s="214"/>
+    </row>
+    <row r="28" spans="1:20" ht="76.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="205">
         <v>26</v>
       </c>
-      <c r="B28" s="312" t="s">
-        <v>310</v>
-      </c>
-      <c r="C28" s="249" t="s">
-        <v>275</v>
-      </c>
-      <c r="D28" s="303" t="s">
-        <v>303</v>
-      </c>
-      <c r="E28" s="304" t="s">
-        <v>276</v>
-      </c>
-      <c r="F28" s="276" t="s">
-        <v>55</v>
-      </c>
+      <c r="B28" s="232" t="s">
+        <v>465</v>
+      </c>
+      <c r="C28" s="273">
+        <v>2022</v>
+      </c>
+      <c r="D28" s="285" t="s">
+        <v>468</v>
+      </c>
+      <c r="E28" s="298" t="s">
+        <v>74</v>
+      </c>
+      <c r="F28" s="397"/>
       <c r="G28" s="218"/>
-      <c r="H28" s="137" t="s">
-        <v>306</v>
-      </c>
-      <c r="I28" s="247"/>
-    </row>
-    <row r="29" spans="1:20" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H28" s="304"/>
+      <c r="I28" s="269"/>
+      <c r="J28" s="287"/>
+      <c r="K28" s="247"/>
+      <c r="L28" s="137"/>
+      <c r="M28" s="137"/>
+      <c r="N28" s="137"/>
+      <c r="O28" s="252"/>
+      <c r="P28" s="106"/>
+      <c r="Q28" s="137"/>
+      <c r="R28" s="213"/>
+      <c r="S28" s="213"/>
+      <c r="T28" s="214"/>
+    </row>
+    <row r="29" spans="1:20" ht="76.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="205">
         <v>27</v>
       </c>
-      <c r="B29" s="297" t="s">
+      <c r="B29" s="232" t="s">
+        <v>466</v>
+      </c>
+      <c r="C29" s="273">
+        <v>2022</v>
+      </c>
+      <c r="D29" s="285" t="s">
+        <v>469</v>
+      </c>
+      <c r="E29" s="298" t="s">
+        <v>74</v>
+      </c>
+      <c r="F29" s="397"/>
+      <c r="G29" s="218"/>
+      <c r="H29" s="304"/>
+      <c r="I29" s="269"/>
+      <c r="J29" s="287"/>
+      <c r="K29" s="247"/>
+      <c r="L29" s="137"/>
+      <c r="M29" s="137"/>
+      <c r="N29" s="137"/>
+      <c r="O29" s="252"/>
+      <c r="P29" s="106"/>
+      <c r="Q29" s="137"/>
+      <c r="R29" s="213"/>
+      <c r="S29" s="213"/>
+      <c r="T29" s="214"/>
+    </row>
+    <row r="30" spans="1:20" ht="76.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="205">
+        <v>28</v>
+      </c>
+      <c r="B30" s="207" t="s">
+        <v>184</v>
+      </c>
+      <c r="C30" s="248" t="s">
+        <v>195</v>
+      </c>
+      <c r="D30" s="395" t="s">
+        <v>462</v>
+      </c>
+      <c r="E30" s="298" t="s">
+        <v>74</v>
+      </c>
+      <c r="F30" s="299" t="s">
+        <v>318</v>
+      </c>
+      <c r="G30" s="218"/>
+      <c r="H30" s="269" t="s">
+        <v>277</v>
+      </c>
+      <c r="I30" s="246" t="s">
+        <v>319</v>
+      </c>
+      <c r="J30" s="269" t="s">
+        <v>349</v>
+      </c>
+      <c r="K30" s="334" t="s">
+        <v>365</v>
+      </c>
+      <c r="L30" s="137"/>
+      <c r="M30" s="137"/>
+      <c r="N30" s="213"/>
+      <c r="O30" s="213"/>
+      <c r="P30" s="213"/>
+      <c r="Q30" s="213"/>
+      <c r="R30" s="213"/>
+      <c r="S30" s="213"/>
+      <c r="T30" s="214"/>
+    </row>
+    <row r="31" spans="1:20" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A31" s="205">
+        <v>29</v>
+      </c>
+      <c r="B31" s="311" t="s">
+        <v>311</v>
+      </c>
+      <c r="C31" s="297" t="s">
+        <v>275</v>
+      </c>
+      <c r="D31" s="302" t="s">
+        <v>302</v>
+      </c>
+      <c r="E31" s="303" t="s">
+        <v>276</v>
+      </c>
+      <c r="F31" s="275" t="s">
+        <v>304</v>
+      </c>
+      <c r="G31" s="218"/>
+      <c r="H31" s="137" t="s">
+        <v>305</v>
+      </c>
+      <c r="I31" s="314" t="s">
+        <v>323</v>
+      </c>
+      <c r="J31" s="213"/>
+      <c r="K31" s="213"/>
+      <c r="L31" s="213"/>
+    </row>
+    <row r="32" spans="1:20" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A32" s="205">
+        <v>30</v>
+      </c>
+      <c r="B32" s="311" t="s">
+        <v>310</v>
+      </c>
+      <c r="C32" s="248" t="s">
+        <v>275</v>
+      </c>
+      <c r="D32" s="302" t="s">
+        <v>303</v>
+      </c>
+      <c r="E32" s="303" t="s">
+        <v>276</v>
+      </c>
+      <c r="F32" s="275" t="s">
+        <v>55</v>
+      </c>
+      <c r="G32" s="218"/>
+      <c r="H32" s="137" t="s">
+        <v>306</v>
+      </c>
+      <c r="I32" s="246"/>
+    </row>
+    <row r="33" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="205">
+        <v>31</v>
+      </c>
+      <c r="B33" s="296" t="s">
         <v>307</v>
       </c>
-      <c r="C29" s="311" t="s">
+      <c r="C33" s="310" t="s">
         <v>309</v>
       </c>
-      <c r="D29" s="309" t="s">
+      <c r="D33" s="308" t="s">
         <v>308</v>
       </c>
-      <c r="E29" s="313" t="s">
+      <c r="E33" s="312" t="s">
         <v>312</v>
       </c>
-      <c r="F29" s="310" t="s">
+      <c r="F33" s="309" t="s">
         <v>26</v>
       </c>
-      <c r="G29" s="218"/>
-      <c r="H29" s="292" t="s">
+      <c r="G33" s="218"/>
+      <c r="H33" s="291" t="s">
         <v>367</v>
       </c>
-      <c r="I29" s="247"/>
+      <c r="I33" s="246"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9926,1665 +10342,1665 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="393" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="394" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="395"/>
-    <col min="4" max="4" width="15.85546875" style="396" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" style="396" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" style="395" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" style="380" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="381" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="382"/>
+    <col min="4" max="4" width="15.85546875" style="383" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" style="383" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" style="382" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="346" t="s">
+      <c r="A1" s="336" t="s">
         <v>368</v>
       </c>
-      <c r="B1" s="347"/>
-      <c r="C1" s="347"/>
-      <c r="D1" s="347"/>
-      <c r="E1" s="347"/>
-      <c r="F1" s="347"/>
+      <c r="B1" s="392"/>
+      <c r="C1" s="392"/>
+      <c r="D1" s="392"/>
+      <c r="E1" s="392"/>
+      <c r="F1" s="392"/>
     </row>
     <row r="2" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="348" t="s">
+      <c r="A2" s="337" t="s">
         <v>369</v>
       </c>
-      <c r="B2" s="349" t="s">
+      <c r="B2" s="338" t="s">
         <v>370</v>
       </c>
-      <c r="C2" s="349" t="s">
+      <c r="C2" s="338" t="s">
         <v>371</v>
       </c>
-      <c r="D2" s="350" t="s">
+      <c r="D2" s="339" t="s">
         <v>372</v>
       </c>
-      <c r="E2" s="350" t="s">
+      <c r="E2" s="339" t="s">
         <v>373</v>
       </c>
-      <c r="F2" s="351" t="s">
+      <c r="F2" s="340" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="352">
+      <c r="A3" s="341">
         <v>1</v>
       </c>
-      <c r="B3" s="353" t="s">
+      <c r="B3" s="342" t="s">
         <v>375</v>
       </c>
-      <c r="C3" s="353">
+      <c r="C3" s="342">
         <v>2018</v>
       </c>
-      <c r="D3" s="354" t="s">
+      <c r="D3" s="343" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="355" t="s">
+      <c r="E3" s="344" t="s">
         <v>376</v>
       </c>
-      <c r="F3" s="353" t="s">
+      <c r="F3" s="342" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="356">
+      <c r="A4" s="345">
         <v>2</v>
       </c>
-      <c r="B4" s="357" t="s">
+      <c r="B4" s="346" t="s">
         <v>375</v>
       </c>
-      <c r="C4" s="357">
+      <c r="C4" s="346">
         <v>2018</v>
       </c>
-      <c r="D4" s="358" t="s">
+      <c r="D4" s="347" t="s">
         <v>378</v>
       </c>
-      <c r="E4" s="359" t="s">
+      <c r="E4" s="348" t="s">
         <v>379</v>
       </c>
-      <c r="F4" s="357" t="s">
+      <c r="F4" s="346" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="356">
+      <c r="A5" s="345">
         <v>3</v>
       </c>
-      <c r="B5" s="357" t="s">
+      <c r="B5" s="346" t="s">
         <v>375</v>
       </c>
-      <c r="C5" s="357">
+      <c r="C5" s="346">
         <v>2019</v>
       </c>
-      <c r="D5" s="358" t="s">
+      <c r="D5" s="347" t="s">
         <v>381</v>
       </c>
-      <c r="E5" s="359" t="s">
+      <c r="E5" s="348" t="s">
         <v>382</v>
       </c>
-      <c r="F5" s="357" t="s">
+      <c r="F5" s="346" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="356">
+      <c r="A6" s="345">
         <v>4</v>
       </c>
-      <c r="B6" s="357" t="s">
+      <c r="B6" s="346" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="357">
+      <c r="C6" s="346">
         <v>2018</v>
       </c>
-      <c r="D6" s="360" t="s">
+      <c r="D6" s="349" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="359" t="s">
+      <c r="E6" s="348" t="s">
         <v>384</v>
       </c>
-      <c r="F6" s="357" t="s">
+      <c r="F6" s="346" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="356">
+      <c r="A7" s="345">
         <v>5</v>
       </c>
-      <c r="B7" s="357" t="s">
+      <c r="B7" s="346" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="357">
+      <c r="C7" s="346">
         <v>2016</v>
       </c>
-      <c r="D7" s="360" t="s">
+      <c r="D7" s="349" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="359" t="s">
+      <c r="E7" s="348" t="s">
         <v>386</v>
       </c>
-      <c r="F7" s="357" t="s">
+      <c r="F7" s="346" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="356">
+      <c r="A8" s="345">
         <v>7</v>
       </c>
-      <c r="B8" s="357" t="s">
+      <c r="B8" s="346" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="357">
+      <c r="C8" s="346">
         <v>2015</v>
       </c>
-      <c r="D8" s="360" t="s">
+      <c r="D8" s="349" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="361" t="s">
+      <c r="E8" s="350" t="s">
         <v>387</v>
       </c>
-      <c r="F8" s="357" t="s">
+      <c r="F8" s="346" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="356">
+      <c r="A9" s="345">
         <v>8</v>
       </c>
-      <c r="B9" s="357" t="s">
+      <c r="B9" s="346" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="353">
+      <c r="C9" s="342">
         <v>2015</v>
       </c>
-      <c r="D9" s="360" t="s">
+      <c r="D9" s="349" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="361" t="s">
+      <c r="E9" s="350" t="s">
         <v>389</v>
       </c>
-      <c r="F9" s="357" t="s">
+      <c r="F9" s="346" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="356">
+      <c r="A10" s="345">
         <v>9</v>
       </c>
-      <c r="B10" s="357" t="s">
+      <c r="B10" s="346" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="357">
+      <c r="C10" s="346">
         <v>2015</v>
       </c>
-      <c r="D10" s="360" t="s">
+      <c r="D10" s="349" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="362" t="s">
+      <c r="E10" s="351" t="s">
         <v>391</v>
       </c>
-      <c r="F10" s="357" t="s">
+      <c r="F10" s="346" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="356"/>
-      <c r="B11" s="363" t="s">
+      <c r="A11" s="345"/>
+      <c r="B11" s="352" t="s">
         <v>393</v>
       </c>
-      <c r="C11" s="363">
+      <c r="C11" s="352">
         <v>2022</v>
       </c>
-      <c r="D11" s="358" t="s">
+      <c r="D11" s="347" t="s">
         <v>394</v>
       </c>
-      <c r="E11" s="362" t="s">
+      <c r="E11" s="351" t="s">
         <v>395</v>
       </c>
-      <c r="F11" s="357"/>
+      <c r="F11" s="346"/>
     </row>
     <row r="12" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="356"/>
-      <c r="B12" s="363" t="s">
+      <c r="A12" s="345"/>
+      <c r="B12" s="352" t="s">
         <v>396</v>
       </c>
-      <c r="C12" s="363">
+      <c r="C12" s="352">
         <v>2022</v>
       </c>
-      <c r="D12" s="358" t="s">
+      <c r="D12" s="347" t="s">
         <v>397</v>
       </c>
-      <c r="E12" s="362" t="s">
+      <c r="E12" s="351" t="s">
         <v>398</v>
       </c>
-      <c r="F12" s="357"/>
+      <c r="F12" s="346"/>
     </row>
     <row r="13" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="356"/>
-      <c r="B13" s="363" t="s">
+      <c r="A13" s="345"/>
+      <c r="B13" s="352" t="s">
         <v>399</v>
       </c>
-      <c r="C13" s="363">
+      <c r="C13" s="352">
         <v>2022</v>
       </c>
-      <c r="D13" s="358" t="s">
+      <c r="D13" s="347" t="s">
         <v>400</v>
       </c>
-      <c r="E13" s="364" t="s">
+      <c r="E13" s="353" t="s">
         <v>401</v>
       </c>
-      <c r="F13" s="357"/>
+      <c r="F13" s="346"/>
     </row>
     <row r="14" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="356">
+      <c r="A14" s="345">
         <v>10</v>
       </c>
-      <c r="B14" s="360" t="s">
+      <c r="B14" s="349" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="360">
+      <c r="C14" s="349">
         <v>2015</v>
       </c>
-      <c r="D14" s="365" t="s">
+      <c r="D14" s="354" t="s">
         <v>402</v>
       </c>
-      <c r="E14" s="359" t="s">
+      <c r="E14" s="348" t="s">
         <v>403</v>
       </c>
-      <c r="F14" s="360" t="s">
+      <c r="F14" s="349" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="356">
+      <c r="A15" s="345">
         <v>11</v>
       </c>
-      <c r="B15" s="360" t="s">
+      <c r="B15" s="349" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="360">
+      <c r="C15" s="349">
         <v>2015</v>
       </c>
-      <c r="D15" s="360" t="s">
+      <c r="D15" s="349" t="s">
         <v>404</v>
       </c>
-      <c r="E15" s="359" t="s">
+      <c r="E15" s="348" t="s">
         <v>405</v>
       </c>
-      <c r="F15" s="357" t="s">
+      <c r="F15" s="346" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="356">
+      <c r="A16" s="345">
         <v>12</v>
       </c>
-      <c r="B16" s="357" t="s">
+      <c r="B16" s="346" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="357">
+      <c r="C16" s="346">
         <v>2017</v>
       </c>
-      <c r="D16" s="360" t="s">
+      <c r="D16" s="349" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="366" t="s">
+      <c r="E16" s="355" t="s">
         <v>407</v>
       </c>
-      <c r="F16" s="357" t="s">
+      <c r="F16" s="346" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="356">
+      <c r="A17" s="345">
         <v>13</v>
       </c>
-      <c r="B17" s="357" t="s">
+      <c r="B17" s="346" t="s">
         <v>408</v>
       </c>
-      <c r="C17" s="357">
+      <c r="C17" s="346">
         <v>2017</v>
       </c>
-      <c r="D17" s="360" t="s">
+      <c r="D17" s="349" t="s">
         <v>409</v>
       </c>
-      <c r="E17" s="366" t="s">
+      <c r="E17" s="355" t="s">
         <v>410</v>
       </c>
-      <c r="F17" s="357" t="s">
+      <c r="F17" s="346" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="356">
+      <c r="A18" s="345">
         <v>14</v>
       </c>
-      <c r="B18" s="357" t="s">
+      <c r="B18" s="346" t="s">
         <v>411</v>
       </c>
-      <c r="C18" s="357">
+      <c r="C18" s="346">
         <v>2017</v>
       </c>
-      <c r="D18" s="360" t="s">
+      <c r="D18" s="349" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="362" t="s">
+      <c r="E18" s="351" t="s">
         <v>412</v>
       </c>
-      <c r="F18" s="357" t="s">
+      <c r="F18" s="346" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="356"/>
-      <c r="B19" s="357" t="s">
+      <c r="A19" s="345"/>
+      <c r="B19" s="346" t="s">
         <v>413</v>
       </c>
-      <c r="C19" s="357">
+      <c r="C19" s="346">
         <v>2022</v>
       </c>
-      <c r="D19" s="360" t="s">
+      <c r="D19" s="349" t="s">
         <v>414</v>
       </c>
-      <c r="E19" s="362" t="s">
+      <c r="E19" s="351" t="s">
         <v>415</v>
       </c>
-      <c r="F19" s="357"/>
+      <c r="F19" s="346"/>
     </row>
     <row r="20" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="356"/>
-      <c r="B20" s="357" t="s">
+      <c r="A20" s="345"/>
+      <c r="B20" s="346" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="357">
+      <c r="C20" s="346">
         <v>2022</v>
       </c>
-      <c r="D20" s="360" t="s">
+      <c r="D20" s="349" t="s">
         <v>416</v>
       </c>
-      <c r="E20" s="362" t="s">
+      <c r="E20" s="351" t="s">
         <v>417</v>
       </c>
-      <c r="F20" s="357"/>
+      <c r="F20" s="346"/>
     </row>
     <row r="21" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="356">
+      <c r="A21" s="345">
         <v>15</v>
       </c>
-      <c r="B21" s="357" t="s">
+      <c r="B21" s="346" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="357">
+      <c r="C21" s="346">
         <v>2006</v>
       </c>
-      <c r="D21" s="360" t="s">
+      <c r="D21" s="349" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="362" t="s">
+      <c r="E21" s="351" t="s">
         <v>418</v>
       </c>
-      <c r="F21" s="357" t="s">
+      <c r="F21" s="346" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="367">
+      <c r="A22" s="356">
         <v>16</v>
       </c>
-      <c r="B22" s="357" t="s">
+      <c r="B22" s="346" t="s">
         <v>419</v>
       </c>
-      <c r="C22" s="357">
+      <c r="C22" s="346">
         <v>2011</v>
       </c>
-      <c r="D22" s="360" t="s">
+      <c r="D22" s="349" t="s">
         <v>420</v>
       </c>
-      <c r="E22" s="366" t="s">
+      <c r="E22" s="355" t="s">
         <v>421</v>
       </c>
-      <c r="F22" s="357" t="s">
+      <c r="F22" s="346" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="367">
+      <c r="A23" s="356">
         <v>17</v>
       </c>
-      <c r="B23" s="357" t="s">
+      <c r="B23" s="346" t="s">
         <v>422</v>
       </c>
-      <c r="C23" s="357">
+      <c r="C23" s="346">
         <v>2020</v>
       </c>
-      <c r="D23" s="360" t="s">
+      <c r="D23" s="349" t="s">
         <v>423</v>
       </c>
-      <c r="E23" s="366" t="s">
+      <c r="E23" s="355" t="s">
         <v>424</v>
       </c>
-      <c r="F23" s="357" t="s">
+      <c r="F23" s="346" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="373" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="368">
+    <row r="24" spans="1:12" s="360" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="357">
         <v>18</v>
       </c>
-      <c r="B24" s="369" t="s">
+      <c r="B24" s="358" t="s">
         <v>425</v>
       </c>
-      <c r="C24" s="369">
+      <c r="C24" s="358">
         <v>2021</v>
       </c>
-      <c r="D24" s="369" t="s">
+      <c r="D24" s="358" t="s">
         <v>426</v>
       </c>
-      <c r="E24" s="370" t="s">
+      <c r="E24" s="359" t="s">
         <v>427</v>
       </c>
-      <c r="F24" s="360" t="s">
+      <c r="F24" s="349" t="s">
         <v>380</v>
       </c>
-      <c r="G24" s="371"/>
-      <c r="H24" s="372"/>
-      <c r="I24" s="372"/>
-      <c r="J24" s="372"/>
-      <c r="K24" s="372"/>
-      <c r="L24" s="372"/>
+      <c r="G24" s="393"/>
+      <c r="H24" s="394"/>
+      <c r="I24" s="394"/>
+      <c r="J24" s="394"/>
+      <c r="K24" s="394"/>
+      <c r="L24" s="394"/>
     </row>
     <row r="25" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="356">
+      <c r="A25" s="345">
         <v>19</v>
       </c>
-      <c r="B25" s="369" t="s">
+      <c r="B25" s="358" t="s">
         <v>425</v>
       </c>
-      <c r="C25" s="369">
+      <c r="C25" s="358">
         <v>2021</v>
       </c>
-      <c r="D25" s="369" t="s">
+      <c r="D25" s="358" t="s">
         <v>428</v>
       </c>
-      <c r="E25" s="370" t="s">
+      <c r="E25" s="359" t="s">
         <v>429</v>
       </c>
-      <c r="F25" s="357" t="s">
+      <c r="F25" s="346" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="356">
+      <c r="A26" s="345">
         <v>20</v>
       </c>
-      <c r="B26" s="369" t="s">
+      <c r="B26" s="358" t="s">
         <v>425</v>
       </c>
-      <c r="C26" s="369">
+      <c r="C26" s="358">
         <v>2022</v>
       </c>
-      <c r="D26" s="369" t="s">
+      <c r="D26" s="358" t="s">
         <v>431</v>
       </c>
-      <c r="E26" s="374" t="s">
+      <c r="E26" s="361" t="s">
         <v>432</v>
       </c>
-      <c r="F26" s="357" t="s">
+      <c r="F26" s="346" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="356">
+      <c r="A27" s="345">
         <v>21</v>
       </c>
-      <c r="B27" s="369" t="s">
+      <c r="B27" s="358" t="s">
         <v>433</v>
       </c>
-      <c r="C27" s="369">
+      <c r="C27" s="358">
         <v>2018</v>
       </c>
-      <c r="D27" s="369" t="s">
+      <c r="D27" s="358" t="s">
         <v>58</v>
       </c>
-      <c r="E27" s="366" t="s">
+      <c r="E27" s="355" t="s">
         <v>434</v>
       </c>
-      <c r="F27" s="357" t="s">
+      <c r="F27" s="346" t="s">
         <v>435</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="375"/>
-      <c r="B28" s="376"/>
-      <c r="C28" s="376"/>
-      <c r="D28" s="376"/>
-      <c r="E28" s="376"/>
-      <c r="F28" s="377"/>
+      <c r="A28" s="362"/>
+      <c r="B28" s="363"/>
+      <c r="C28" s="363"/>
+      <c r="D28" s="363"/>
+      <c r="E28" s="363"/>
+      <c r="F28" s="364"/>
     </row>
     <row r="29" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="356">
+      <c r="A29" s="345">
         <v>23</v>
       </c>
-      <c r="B29" s="369" t="s">
+      <c r="B29" s="358" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="369">
+      <c r="C29" s="358">
         <v>2021</v>
       </c>
-      <c r="D29" s="369" t="s">
+      <c r="D29" s="358" t="s">
         <v>436</v>
       </c>
-      <c r="E29" s="364" t="s">
+      <c r="E29" s="353" t="s">
         <v>437</v>
       </c>
-      <c r="F29" s="357" t="s">
+      <c r="F29" s="346" t="s">
         <v>438</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="356">
+      <c r="A30" s="345">
         <v>24</v>
       </c>
-      <c r="B30" s="369" t="s">
+      <c r="B30" s="358" t="s">
         <v>439</v>
       </c>
-      <c r="C30" s="369">
+      <c r="C30" s="358">
         <v>2012</v>
       </c>
-      <c r="D30" s="369" t="s">
+      <c r="D30" s="358" t="s">
         <v>440</v>
       </c>
-      <c r="E30" s="378" t="s">
+      <c r="E30" s="365" t="s">
         <v>441</v>
       </c>
-      <c r="F30" s="357" t="s">
+      <c r="F30" s="346" t="s">
         <v>438</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="356">
+      <c r="A31" s="345">
         <v>25</v>
       </c>
-      <c r="B31" s="369" t="s">
+      <c r="B31" s="358" t="s">
         <v>442</v>
       </c>
-      <c r="C31" s="369">
+      <c r="C31" s="358">
         <v>2010</v>
       </c>
-      <c r="D31" s="369" t="s">
+      <c r="D31" s="358" t="s">
         <v>443</v>
       </c>
-      <c r="E31" s="366" t="s">
+      <c r="E31" s="355" t="s">
         <v>444</v>
       </c>
-      <c r="F31" s="357" t="s">
+      <c r="F31" s="346" t="s">
         <v>438</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="379"/>
-      <c r="B32" s="376"/>
-      <c r="C32" s="376"/>
-      <c r="D32" s="376"/>
-      <c r="E32" s="376"/>
-      <c r="F32" s="380"/>
+      <c r="A32" s="366"/>
+      <c r="B32" s="363"/>
+      <c r="C32" s="363"/>
+      <c r="D32" s="363"/>
+      <c r="E32" s="363"/>
+      <c r="F32" s="367"/>
     </row>
     <row r="33" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="356">
+      <c r="A33" s="345">
         <v>26</v>
       </c>
-      <c r="B33" s="369" t="s">
+      <c r="B33" s="358" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="369">
+      <c r="C33" s="358">
         <v>2012</v>
       </c>
-      <c r="D33" s="369" t="s">
+      <c r="D33" s="358" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="366" t="s">
+      <c r="E33" s="355" t="s">
         <v>445</v>
       </c>
-      <c r="F33" s="357" t="s">
+      <c r="F33" s="346" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="356">
+      <c r="A34" s="345">
         <v>27</v>
       </c>
-      <c r="B34" s="381" t="s">
+      <c r="B34" s="368" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="369">
+      <c r="C34" s="358">
         <v>2020</v>
       </c>
-      <c r="D34" s="369" t="s">
+      <c r="D34" s="358" t="s">
         <v>446</v>
       </c>
-      <c r="E34" s="361" t="s">
+      <c r="E34" s="350" t="s">
         <v>447</v>
       </c>
-      <c r="F34" s="357" t="s">
+      <c r="F34" s="346" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="356">
+      <c r="A35" s="345">
         <v>28</v>
       </c>
-      <c r="B35" s="381" t="s">
+      <c r="B35" s="368" t="s">
         <v>449</v>
       </c>
-      <c r="C35" s="357">
+      <c r="C35" s="346">
         <v>2018</v>
       </c>
-      <c r="D35" s="360" t="s">
+      <c r="D35" s="349" t="s">
         <v>54</v>
       </c>
-      <c r="E35" s="359" t="s">
+      <c r="E35" s="348" t="s">
         <v>450</v>
       </c>
-      <c r="F35" s="357" t="s">
+      <c r="F35" s="346" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="382">
+      <c r="A36" s="369">
         <v>29</v>
       </c>
-      <c r="B36" s="383" t="s">
+      <c r="B36" s="370" t="s">
         <v>451</v>
       </c>
-      <c r="C36" s="384">
+      <c r="C36" s="371">
         <v>2019</v>
       </c>
-      <c r="D36" s="385" t="s">
+      <c r="D36" s="372" t="s">
         <v>452</v>
       </c>
-      <c r="E36" s="386" t="s">
+      <c r="E36" s="373" t="s">
         <v>453</v>
       </c>
-      <c r="F36" s="387" t="s">
+      <c r="F36" s="374" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="382">
+      <c r="A37" s="369">
         <v>30</v>
       </c>
-      <c r="B37" s="381" t="s">
+      <c r="B37" s="368" t="s">
         <v>454</v>
       </c>
-      <c r="C37" s="357">
+      <c r="C37" s="346">
         <v>2019</v>
       </c>
-      <c r="D37" s="388" t="s">
+      <c r="D37" s="375" t="s">
         <v>455</v>
       </c>
-      <c r="E37" s="388" t="s">
+      <c r="E37" s="375" t="s">
         <v>456</v>
       </c>
-      <c r="F37" s="389" t="s">
+      <c r="F37" s="376" t="s">
         <v>456</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A38"/>
-      <c r="B38" s="390"/>
-      <c r="C38" s="391"/>
-      <c r="D38" s="392"/>
-      <c r="E38" s="391"/>
-      <c r="F38" s="391"/>
+      <c r="B38" s="377"/>
+      <c r="C38" s="378"/>
+      <c r="D38" s="379"/>
+      <c r="E38" s="378"/>
+      <c r="F38" s="378"/>
     </row>
     <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A39"/>
-      <c r="B39" s="390"/>
-      <c r="C39" s="391"/>
-      <c r="D39" s="392"/>
-      <c r="E39" s="391"/>
-      <c r="F39" s="391"/>
+      <c r="B39" s="377"/>
+      <c r="C39" s="378"/>
+      <c r="D39" s="379"/>
+      <c r="E39" s="378"/>
+      <c r="F39" s="378"/>
     </row>
     <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A40"/>
-      <c r="B40" s="390"/>
-      <c r="C40" s="391"/>
-      <c r="D40" s="392"/>
-      <c r="E40" s="391"/>
-      <c r="F40" s="391"/>
+      <c r="B40" s="377"/>
+      <c r="C40" s="378"/>
+      <c r="D40" s="379"/>
+      <c r="E40" s="378"/>
+      <c r="F40" s="378"/>
     </row>
     <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A41"/>
-      <c r="B41" s="390"/>
-      <c r="C41" s="391"/>
-      <c r="D41" s="392"/>
-      <c r="E41" s="391"/>
-      <c r="F41" s="391"/>
+      <c r="B41" s="377"/>
+      <c r="C41" s="378"/>
+      <c r="D41" s="379"/>
+      <c r="E41" s="378"/>
+      <c r="F41" s="378"/>
     </row>
     <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A42"/>
-      <c r="B42" s="390"/>
-      <c r="C42" s="391"/>
-      <c r="D42" s="392"/>
-      <c r="E42" s="391"/>
-      <c r="F42" s="391"/>
+      <c r="B42" s="377"/>
+      <c r="C42" s="378"/>
+      <c r="D42" s="379"/>
+      <c r="E42" s="378"/>
+      <c r="F42" s="378"/>
     </row>
     <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A43"/>
-      <c r="B43" s="390"/>
-      <c r="C43" s="391"/>
-      <c r="D43" s="392"/>
-      <c r="E43" s="391"/>
-      <c r="F43" s="391"/>
+      <c r="B43" s="377"/>
+      <c r="C43" s="378"/>
+      <c r="D43" s="379"/>
+      <c r="E43" s="378"/>
+      <c r="F43" s="378"/>
     </row>
     <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A44"/>
-      <c r="B44" s="390"/>
-      <c r="C44" s="391"/>
-      <c r="D44" s="392"/>
-      <c r="E44" s="391"/>
-      <c r="F44" s="391"/>
+      <c r="B44" s="377"/>
+      <c r="C44" s="378"/>
+      <c r="D44" s="379"/>
+      <c r="E44" s="378"/>
+      <c r="F44" s="378"/>
     </row>
     <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A45"/>
-      <c r="B45" s="390"/>
-      <c r="C45" s="391"/>
-      <c r="D45" s="392"/>
-      <c r="E45" s="391"/>
-      <c r="F45" s="391"/>
+      <c r="B45" s="377"/>
+      <c r="C45" s="378"/>
+      <c r="D45" s="379"/>
+      <c r="E45" s="378"/>
+      <c r="F45" s="378"/>
     </row>
     <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A46"/>
-      <c r="B46" s="390"/>
-      <c r="C46" s="391"/>
-      <c r="D46" s="392"/>
-      <c r="E46" s="391"/>
-      <c r="F46" s="391"/>
+      <c r="B46" s="377"/>
+      <c r="C46" s="378"/>
+      <c r="D46" s="379"/>
+      <c r="E46" s="378"/>
+      <c r="F46" s="378"/>
     </row>
     <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A47"/>
-      <c r="B47" s="390"/>
-      <c r="C47" s="391"/>
-      <c r="D47" s="392"/>
-      <c r="E47" s="391"/>
-      <c r="F47" s="391"/>
+      <c r="B47" s="377"/>
+      <c r="C47" s="378"/>
+      <c r="D47" s="379"/>
+      <c r="E47" s="378"/>
+      <c r="F47" s="378"/>
     </row>
     <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A48"/>
-      <c r="B48" s="390"/>
-      <c r="C48" s="391"/>
-      <c r="D48" s="392"/>
-      <c r="E48" s="391"/>
-      <c r="F48" s="391"/>
+      <c r="B48" s="377"/>
+      <c r="C48" s="378"/>
+      <c r="D48" s="379"/>
+      <c r="E48" s="378"/>
+      <c r="F48" s="378"/>
     </row>
     <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A49"/>
-      <c r="B49" s="390"/>
-      <c r="C49" s="391"/>
-      <c r="D49" s="392"/>
-      <c r="E49" s="391"/>
-      <c r="F49" s="391"/>
+      <c r="B49" s="377"/>
+      <c r="C49" s="378"/>
+      <c r="D49" s="379"/>
+      <c r="E49" s="378"/>
+      <c r="F49" s="378"/>
     </row>
     <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A50"/>
-      <c r="B50" s="390"/>
-      <c r="C50" s="391"/>
-      <c r="D50" s="392"/>
-      <c r="E50" s="391"/>
-      <c r="F50" s="391"/>
+      <c r="B50" s="377"/>
+      <c r="C50" s="378"/>
+      <c r="D50" s="379"/>
+      <c r="E50" s="378"/>
+      <c r="F50" s="378"/>
     </row>
     <row r="51" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A51"/>
-      <c r="B51" s="390"/>
-      <c r="C51" s="391"/>
-      <c r="D51" s="392"/>
-      <c r="E51" s="391"/>
-      <c r="F51" s="391"/>
+      <c r="B51" s="377"/>
+      <c r="C51" s="378"/>
+      <c r="D51" s="379"/>
+      <c r="E51" s="378"/>
+      <c r="F51" s="378"/>
     </row>
     <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A52"/>
-      <c r="B52" s="390"/>
-      <c r="C52" s="391"/>
-      <c r="D52" s="392"/>
-      <c r="E52" s="391"/>
-      <c r="F52" s="391"/>
+      <c r="B52" s="377"/>
+      <c r="C52" s="378"/>
+      <c r="D52" s="379"/>
+      <c r="E52" s="378"/>
+      <c r="F52" s="378"/>
     </row>
     <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A53"/>
-      <c r="B53" s="390"/>
-      <c r="C53" s="391"/>
-      <c r="D53" s="392"/>
-      <c r="E53" s="391"/>
-      <c r="F53" s="391"/>
+      <c r="B53" s="377"/>
+      <c r="C53" s="378"/>
+      <c r="D53" s="379"/>
+      <c r="E53" s="378"/>
+      <c r="F53" s="378"/>
     </row>
     <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A54"/>
-      <c r="B54" s="390"/>
-      <c r="C54" s="391"/>
-      <c r="D54" s="392"/>
-      <c r="E54" s="391"/>
-      <c r="F54" s="391"/>
+      <c r="B54" s="377"/>
+      <c r="C54" s="378"/>
+      <c r="D54" s="379"/>
+      <c r="E54" s="378"/>
+      <c r="F54" s="378"/>
     </row>
     <row r="55" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A55"/>
-      <c r="B55" s="390"/>
-      <c r="C55" s="391"/>
-      <c r="D55" s="392"/>
-      <c r="E55" s="391"/>
-      <c r="F55" s="391"/>
+      <c r="B55" s="377"/>
+      <c r="C55" s="378"/>
+      <c r="D55" s="379"/>
+      <c r="E55" s="378"/>
+      <c r="F55" s="378"/>
     </row>
     <row r="56" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A56"/>
-      <c r="B56" s="390"/>
-      <c r="C56" s="391"/>
-      <c r="D56" s="392"/>
-      <c r="E56" s="391"/>
-      <c r="F56" s="391"/>
+      <c r="B56" s="377"/>
+      <c r="C56" s="378"/>
+      <c r="D56" s="379"/>
+      <c r="E56" s="378"/>
+      <c r="F56" s="378"/>
     </row>
     <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A57"/>
-      <c r="B57" s="390"/>
-      <c r="C57" s="391"/>
-      <c r="D57" s="392"/>
-      <c r="E57" s="391"/>
-      <c r="F57" s="391"/>
+      <c r="B57" s="377"/>
+      <c r="C57" s="378"/>
+      <c r="D57" s="379"/>
+      <c r="E57" s="378"/>
+      <c r="F57" s="378"/>
     </row>
     <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A58"/>
-      <c r="B58" s="390"/>
-      <c r="C58" s="391"/>
-      <c r="D58" s="392"/>
-      <c r="E58" s="391"/>
-      <c r="F58" s="391"/>
+      <c r="B58" s="377"/>
+      <c r="C58" s="378"/>
+      <c r="D58" s="379"/>
+      <c r="E58" s="378"/>
+      <c r="F58" s="378"/>
     </row>
     <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A59"/>
-      <c r="B59" s="390"/>
-      <c r="C59" s="391"/>
-      <c r="D59" s="392"/>
-      <c r="E59" s="391"/>
-      <c r="F59" s="391"/>
+      <c r="B59" s="377"/>
+      <c r="C59" s="378"/>
+      <c r="D59" s="379"/>
+      <c r="E59" s="378"/>
+      <c r="F59" s="378"/>
     </row>
     <row r="60" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A60"/>
-      <c r="B60" s="390"/>
-      <c r="C60" s="391"/>
-      <c r="D60" s="392"/>
-      <c r="E60" s="391"/>
-      <c r="F60" s="391"/>
+      <c r="B60" s="377"/>
+      <c r="C60" s="378"/>
+      <c r="D60" s="379"/>
+      <c r="E60" s="378"/>
+      <c r="F60" s="378"/>
     </row>
     <row r="61" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A61"/>
-      <c r="B61" s="390"/>
-      <c r="C61" s="391"/>
-      <c r="D61" s="392"/>
-      <c r="E61" s="391"/>
-      <c r="F61" s="391"/>
+      <c r="B61" s="377"/>
+      <c r="C61" s="378"/>
+      <c r="D61" s="379"/>
+      <c r="E61" s="378"/>
+      <c r="F61" s="378"/>
     </row>
     <row r="62" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A62"/>
-      <c r="B62" s="390"/>
-      <c r="C62" s="391"/>
-      <c r="D62" s="392"/>
-      <c r="E62" s="391"/>
-      <c r="F62" s="391"/>
+      <c r="B62" s="377"/>
+      <c r="C62" s="378"/>
+      <c r="D62" s="379"/>
+      <c r="E62" s="378"/>
+      <c r="F62" s="378"/>
     </row>
     <row r="63" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A63"/>
-      <c r="B63" s="390"/>
-      <c r="C63" s="391"/>
-      <c r="D63" s="392"/>
-      <c r="E63" s="391"/>
-      <c r="F63" s="391"/>
+      <c r="B63" s="377"/>
+      <c r="C63" s="378"/>
+      <c r="D63" s="379"/>
+      <c r="E63" s="378"/>
+      <c r="F63" s="378"/>
     </row>
     <row r="64" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A64"/>
-      <c r="B64" s="390"/>
-      <c r="C64" s="391"/>
-      <c r="D64" s="392"/>
-      <c r="E64" s="391"/>
-      <c r="F64" s="391"/>
+      <c r="B64" s="377"/>
+      <c r="C64" s="378"/>
+      <c r="D64" s="379"/>
+      <c r="E64" s="378"/>
+      <c r="F64" s="378"/>
     </row>
     <row r="65" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A65"/>
-      <c r="B65" s="390"/>
-      <c r="C65" s="391"/>
-      <c r="D65" s="392"/>
-      <c r="E65" s="391"/>
-      <c r="F65" s="391"/>
+      <c r="B65" s="377"/>
+      <c r="C65" s="378"/>
+      <c r="D65" s="379"/>
+      <c r="E65" s="378"/>
+      <c r="F65" s="378"/>
     </row>
     <row r="66" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A66"/>
-      <c r="B66" s="390"/>
-      <c r="C66" s="391"/>
-      <c r="D66" s="392"/>
-      <c r="E66" s="391"/>
-      <c r="F66" s="391"/>
+      <c r="B66" s="377"/>
+      <c r="C66" s="378"/>
+      <c r="D66" s="379"/>
+      <c r="E66" s="378"/>
+      <c r="F66" s="378"/>
     </row>
     <row r="67" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A67"/>
-      <c r="B67" s="390"/>
-      <c r="C67" s="391"/>
-      <c r="D67" s="392"/>
-      <c r="E67" s="391"/>
-      <c r="F67" s="391"/>
+      <c r="B67" s="377"/>
+      <c r="C67" s="378"/>
+      <c r="D67" s="379"/>
+      <c r="E67" s="378"/>
+      <c r="F67" s="378"/>
     </row>
     <row r="68" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A68"/>
-      <c r="B68" s="390"/>
-      <c r="C68" s="391"/>
-      <c r="D68" s="392"/>
-      <c r="E68" s="391"/>
-      <c r="F68" s="391"/>
+      <c r="B68" s="377"/>
+      <c r="C68" s="378"/>
+      <c r="D68" s="379"/>
+      <c r="E68" s="378"/>
+      <c r="F68" s="378"/>
     </row>
     <row r="69" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A69"/>
-      <c r="B69" s="390"/>
-      <c r="C69" s="391"/>
-      <c r="D69" s="392"/>
-      <c r="E69" s="391"/>
-      <c r="F69" s="391"/>
+      <c r="B69" s="377"/>
+      <c r="C69" s="378"/>
+      <c r="D69" s="379"/>
+      <c r="E69" s="378"/>
+      <c r="F69" s="378"/>
     </row>
     <row r="70" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A70"/>
-      <c r="B70" s="390"/>
-      <c r="C70" s="391"/>
-      <c r="D70" s="392"/>
-      <c r="E70" s="391"/>
-      <c r="F70" s="391"/>
+      <c r="B70" s="377"/>
+      <c r="C70" s="378"/>
+      <c r="D70" s="379"/>
+      <c r="E70" s="378"/>
+      <c r="F70" s="378"/>
     </row>
     <row r="71" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A71"/>
-      <c r="B71" s="390"/>
-      <c r="C71" s="391"/>
-      <c r="D71" s="392"/>
-      <c r="E71" s="391"/>
-      <c r="F71" s="391"/>
+      <c r="B71" s="377"/>
+      <c r="C71" s="378"/>
+      <c r="D71" s="379"/>
+      <c r="E71" s="378"/>
+      <c r="F71" s="378"/>
     </row>
     <row r="72" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A72"/>
-      <c r="B72" s="390"/>
-      <c r="C72" s="391"/>
-      <c r="D72" s="392"/>
-      <c r="E72" s="391"/>
-      <c r="F72" s="391"/>
+      <c r="B72" s="377"/>
+      <c r="C72" s="378"/>
+      <c r="D72" s="379"/>
+      <c r="E72" s="378"/>
+      <c r="F72" s="378"/>
     </row>
     <row r="73" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A73"/>
-      <c r="B73" s="390"/>
-      <c r="C73" s="391"/>
-      <c r="D73" s="392"/>
-      <c r="E73" s="391"/>
-      <c r="F73" s="391"/>
+      <c r="B73" s="377"/>
+      <c r="C73" s="378"/>
+      <c r="D73" s="379"/>
+      <c r="E73" s="378"/>
+      <c r="F73" s="378"/>
     </row>
     <row r="74" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A74"/>
-      <c r="B74" s="390"/>
-      <c r="C74" s="391"/>
-      <c r="D74" s="392"/>
-      <c r="E74" s="391"/>
-      <c r="F74" s="391"/>
+      <c r="B74" s="377"/>
+      <c r="C74" s="378"/>
+      <c r="D74" s="379"/>
+      <c r="E74" s="378"/>
+      <c r="F74" s="378"/>
     </row>
     <row r="75" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A75"/>
-      <c r="B75" s="390"/>
-      <c r="C75" s="391"/>
-      <c r="D75" s="392"/>
-      <c r="E75" s="391"/>
-      <c r="F75" s="391"/>
+      <c r="B75" s="377"/>
+      <c r="C75" s="378"/>
+      <c r="D75" s="379"/>
+      <c r="E75" s="378"/>
+      <c r="F75" s="378"/>
     </row>
     <row r="76" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A76"/>
-      <c r="B76" s="390"/>
-      <c r="C76" s="391"/>
-      <c r="D76" s="392"/>
-      <c r="E76" s="391"/>
-      <c r="F76" s="391"/>
+      <c r="B76" s="377"/>
+      <c r="C76" s="378"/>
+      <c r="D76" s="379"/>
+      <c r="E76" s="378"/>
+      <c r="F76" s="378"/>
     </row>
     <row r="77" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A77"/>
-      <c r="B77" s="390"/>
-      <c r="C77" s="391"/>
-      <c r="D77" s="392"/>
-      <c r="E77" s="391"/>
-      <c r="F77" s="391"/>
+      <c r="B77" s="377"/>
+      <c r="C77" s="378"/>
+      <c r="D77" s="379"/>
+      <c r="E77" s="378"/>
+      <c r="F77" s="378"/>
     </row>
     <row r="78" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A78"/>
-      <c r="B78" s="390"/>
-      <c r="C78" s="391"/>
-      <c r="D78" s="392"/>
-      <c r="E78" s="391"/>
-      <c r="F78" s="391"/>
+      <c r="B78" s="377"/>
+      <c r="C78" s="378"/>
+      <c r="D78" s="379"/>
+      <c r="E78" s="378"/>
+      <c r="F78" s="378"/>
     </row>
     <row r="79" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A79"/>
-      <c r="B79" s="390"/>
-      <c r="C79" s="391"/>
-      <c r="D79" s="392"/>
-      <c r="E79" s="391"/>
-      <c r="F79" s="391"/>
+      <c r="B79" s="377"/>
+      <c r="C79" s="378"/>
+      <c r="D79" s="379"/>
+      <c r="E79" s="378"/>
+      <c r="F79" s="378"/>
     </row>
     <row r="80" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A80"/>
-      <c r="B80" s="390"/>
-      <c r="C80" s="391"/>
-      <c r="D80" s="392"/>
-      <c r="E80" s="391"/>
-      <c r="F80" s="391"/>
+      <c r="B80" s="377"/>
+      <c r="C80" s="378"/>
+      <c r="D80" s="379"/>
+      <c r="E80" s="378"/>
+      <c r="F80" s="378"/>
     </row>
     <row r="81" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A81"/>
-      <c r="B81" s="390"/>
-      <c r="C81" s="391"/>
-      <c r="D81" s="392"/>
-      <c r="E81" s="391"/>
-      <c r="F81" s="391"/>
+      <c r="B81" s="377"/>
+      <c r="C81" s="378"/>
+      <c r="D81" s="379"/>
+      <c r="E81" s="378"/>
+      <c r="F81" s="378"/>
     </row>
     <row r="82" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A82"/>
-      <c r="B82" s="390"/>
-      <c r="C82" s="391"/>
-      <c r="D82" s="392"/>
-      <c r="E82" s="391"/>
-      <c r="F82" s="391"/>
+      <c r="B82" s="377"/>
+      <c r="C82" s="378"/>
+      <c r="D82" s="379"/>
+      <c r="E82" s="378"/>
+      <c r="F82" s="378"/>
     </row>
     <row r="83" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A83"/>
-      <c r="B83" s="390"/>
-      <c r="C83" s="391"/>
-      <c r="D83" s="392"/>
-      <c r="E83" s="391"/>
-      <c r="F83" s="391"/>
+      <c r="B83" s="377"/>
+      <c r="C83" s="378"/>
+      <c r="D83" s="379"/>
+      <c r="E83" s="378"/>
+      <c r="F83" s="378"/>
     </row>
     <row r="84" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A84"/>
-      <c r="B84" s="390"/>
-      <c r="C84" s="391"/>
-      <c r="D84" s="392"/>
-      <c r="E84" s="391"/>
-      <c r="F84" s="391"/>
+      <c r="B84" s="377"/>
+      <c r="C84" s="378"/>
+      <c r="D84" s="379"/>
+      <c r="E84" s="378"/>
+      <c r="F84" s="378"/>
     </row>
     <row r="85" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A85"/>
-      <c r="B85" s="390"/>
-      <c r="C85" s="391"/>
-      <c r="D85" s="392"/>
-      <c r="E85" s="391"/>
-      <c r="F85" s="391"/>
+      <c r="B85" s="377"/>
+      <c r="C85" s="378"/>
+      <c r="D85" s="379"/>
+      <c r="E85" s="378"/>
+      <c r="F85" s="378"/>
     </row>
     <row r="86" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A86"/>
-      <c r="B86" s="390"/>
-      <c r="C86" s="391"/>
-      <c r="D86" s="392"/>
-      <c r="E86" s="391"/>
-      <c r="F86" s="391"/>
+      <c r="B86" s="377"/>
+      <c r="C86" s="378"/>
+      <c r="D86" s="379"/>
+      <c r="E86" s="378"/>
+      <c r="F86" s="378"/>
     </row>
     <row r="87" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A87"/>
-      <c r="B87" s="390"/>
-      <c r="C87" s="391"/>
-      <c r="D87" s="392"/>
-      <c r="E87" s="391"/>
-      <c r="F87" s="391"/>
+      <c r="B87" s="377"/>
+      <c r="C87" s="378"/>
+      <c r="D87" s="379"/>
+      <c r="E87" s="378"/>
+      <c r="F87" s="378"/>
     </row>
     <row r="88" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A88"/>
-      <c r="B88" s="390"/>
-      <c r="C88" s="391"/>
-      <c r="D88" s="392"/>
-      <c r="E88" s="391"/>
-      <c r="F88" s="391"/>
+      <c r="B88" s="377"/>
+      <c r="C88" s="378"/>
+      <c r="D88" s="379"/>
+      <c r="E88" s="378"/>
+      <c r="F88" s="378"/>
     </row>
     <row r="89" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A89"/>
-      <c r="B89" s="390"/>
-      <c r="C89" s="391"/>
-      <c r="D89" s="392"/>
-      <c r="E89" s="391"/>
-      <c r="F89" s="391"/>
+      <c r="B89" s="377"/>
+      <c r="C89" s="378"/>
+      <c r="D89" s="379"/>
+      <c r="E89" s="378"/>
+      <c r="F89" s="378"/>
     </row>
     <row r="90" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A90"/>
-      <c r="B90" s="390"/>
-      <c r="C90" s="391"/>
-      <c r="D90" s="392"/>
-      <c r="E90" s="391"/>
-      <c r="F90" s="391"/>
+      <c r="B90" s="377"/>
+      <c r="C90" s="378"/>
+      <c r="D90" s="379"/>
+      <c r="E90" s="378"/>
+      <c r="F90" s="378"/>
     </row>
     <row r="91" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A91"/>
-      <c r="B91" s="390"/>
-      <c r="C91" s="391"/>
-      <c r="D91" s="392"/>
-      <c r="E91" s="391"/>
-      <c r="F91" s="391"/>
+      <c r="B91" s="377"/>
+      <c r="C91" s="378"/>
+      <c r="D91" s="379"/>
+      <c r="E91" s="378"/>
+      <c r="F91" s="378"/>
     </row>
     <row r="92" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A92"/>
-      <c r="B92" s="390"/>
-      <c r="C92" s="391"/>
-      <c r="D92" s="392"/>
-      <c r="E92" s="391"/>
-      <c r="F92" s="391"/>
+      <c r="B92" s="377"/>
+      <c r="C92" s="378"/>
+      <c r="D92" s="379"/>
+      <c r="E92" s="378"/>
+      <c r="F92" s="378"/>
     </row>
     <row r="93" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A93"/>
-      <c r="B93" s="390"/>
-      <c r="C93" s="391"/>
-      <c r="D93" s="392"/>
-      <c r="E93" s="391"/>
-      <c r="F93" s="391"/>
+      <c r="B93" s="377"/>
+      <c r="C93" s="378"/>
+      <c r="D93" s="379"/>
+      <c r="E93" s="378"/>
+      <c r="F93" s="378"/>
     </row>
     <row r="94" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A94"/>
-      <c r="B94" s="390"/>
-      <c r="C94" s="391"/>
-      <c r="D94" s="392"/>
-      <c r="E94" s="391"/>
-      <c r="F94" s="391"/>
+      <c r="B94" s="377"/>
+      <c r="C94" s="378"/>
+      <c r="D94" s="379"/>
+      <c r="E94" s="378"/>
+      <c r="F94" s="378"/>
     </row>
     <row r="95" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A95"/>
-      <c r="B95" s="390"/>
-      <c r="C95" s="391"/>
-      <c r="D95" s="392"/>
-      <c r="E95" s="391"/>
-      <c r="F95" s="391"/>
+      <c r="B95" s="377"/>
+      <c r="C95" s="378"/>
+      <c r="D95" s="379"/>
+      <c r="E95" s="378"/>
+      <c r="F95" s="378"/>
     </row>
     <row r="96" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A96"/>
-      <c r="B96" s="390"/>
-      <c r="C96" s="391"/>
-      <c r="D96" s="392"/>
-      <c r="E96" s="391"/>
-      <c r="F96" s="391"/>
+      <c r="B96" s="377"/>
+      <c r="C96" s="378"/>
+      <c r="D96" s="379"/>
+      <c r="E96" s="378"/>
+      <c r="F96" s="378"/>
     </row>
     <row r="97" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A97"/>
-      <c r="B97" s="390"/>
-      <c r="C97" s="391"/>
-      <c r="D97" s="392"/>
-      <c r="E97" s="391"/>
-      <c r="F97" s="391"/>
+      <c r="B97" s="377"/>
+      <c r="C97" s="378"/>
+      <c r="D97" s="379"/>
+      <c r="E97" s="378"/>
+      <c r="F97" s="378"/>
     </row>
     <row r="98" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A98"/>
-      <c r="B98" s="390"/>
-      <c r="C98" s="391"/>
-      <c r="D98" s="392"/>
-      <c r="E98" s="391"/>
-      <c r="F98" s="391"/>
+      <c r="B98" s="377"/>
+      <c r="C98" s="378"/>
+      <c r="D98" s="379"/>
+      <c r="E98" s="378"/>
+      <c r="F98" s="378"/>
     </row>
     <row r="99" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A99"/>
-      <c r="B99" s="390"/>
-      <c r="C99" s="391"/>
-      <c r="D99" s="392"/>
-      <c r="E99" s="391"/>
-      <c r="F99" s="391"/>
+      <c r="B99" s="377"/>
+      <c r="C99" s="378"/>
+      <c r="D99" s="379"/>
+      <c r="E99" s="378"/>
+      <c r="F99" s="378"/>
     </row>
     <row r="100" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A100"/>
-      <c r="B100" s="390"/>
-      <c r="C100" s="391"/>
-      <c r="D100" s="392"/>
-      <c r="E100" s="391"/>
-      <c r="F100" s="391"/>
+      <c r="B100" s="377"/>
+      <c r="C100" s="378"/>
+      <c r="D100" s="379"/>
+      <c r="E100" s="378"/>
+      <c r="F100" s="378"/>
     </row>
     <row r="101" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A101"/>
-      <c r="B101" s="390"/>
-      <c r="C101" s="391"/>
-      <c r="D101" s="392"/>
-      <c r="E101" s="391"/>
-      <c r="F101" s="391"/>
+      <c r="B101" s="377"/>
+      <c r="C101" s="378"/>
+      <c r="D101" s="379"/>
+      <c r="E101" s="378"/>
+      <c r="F101" s="378"/>
     </row>
     <row r="102" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A102"/>
-      <c r="B102" s="390"/>
-      <c r="C102" s="391"/>
-      <c r="D102" s="392"/>
-      <c r="E102" s="391"/>
-      <c r="F102" s="391"/>
+      <c r="B102" s="377"/>
+      <c r="C102" s="378"/>
+      <c r="D102" s="379"/>
+      <c r="E102" s="378"/>
+      <c r="F102" s="378"/>
     </row>
     <row r="103" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A103"/>
-      <c r="B103" s="390"/>
-      <c r="C103" s="391"/>
-      <c r="D103" s="392"/>
-      <c r="E103" s="391"/>
-      <c r="F103" s="391"/>
+      <c r="B103" s="377"/>
+      <c r="C103" s="378"/>
+      <c r="D103" s="379"/>
+      <c r="E103" s="378"/>
+      <c r="F103" s="378"/>
     </row>
     <row r="104" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A104"/>
-      <c r="B104" s="390"/>
-      <c r="C104" s="391"/>
-      <c r="D104" s="392"/>
-      <c r="E104" s="391"/>
-      <c r="F104" s="391"/>
+      <c r="B104" s="377"/>
+      <c r="C104" s="378"/>
+      <c r="D104" s="379"/>
+      <c r="E104" s="378"/>
+      <c r="F104" s="378"/>
     </row>
     <row r="105" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A105"/>
-      <c r="B105" s="390"/>
-      <c r="C105" s="391"/>
-      <c r="D105" s="392"/>
-      <c r="E105" s="391"/>
-      <c r="F105" s="391"/>
+      <c r="B105" s="377"/>
+      <c r="C105" s="378"/>
+      <c r="D105" s="379"/>
+      <c r="E105" s="378"/>
+      <c r="F105" s="378"/>
     </row>
     <row r="106" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A106"/>
-      <c r="B106" s="390"/>
-      <c r="C106" s="391"/>
-      <c r="D106" s="392"/>
-      <c r="E106" s="391"/>
-      <c r="F106" s="391"/>
+      <c r="B106" s="377"/>
+      <c r="C106" s="378"/>
+      <c r="D106" s="379"/>
+      <c r="E106" s="378"/>
+      <c r="F106" s="378"/>
     </row>
     <row r="107" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A107"/>
-      <c r="B107" s="390"/>
-      <c r="C107" s="391"/>
-      <c r="D107" s="392"/>
-      <c r="E107" s="391"/>
-      <c r="F107" s="391"/>
+      <c r="B107" s="377"/>
+      <c r="C107" s="378"/>
+      <c r="D107" s="379"/>
+      <c r="E107" s="378"/>
+      <c r="F107" s="378"/>
     </row>
     <row r="108" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A108"/>
-      <c r="B108" s="390"/>
-      <c r="C108" s="391"/>
-      <c r="D108" s="392"/>
-      <c r="E108" s="391"/>
-      <c r="F108" s="391"/>
+      <c r="B108" s="377"/>
+      <c r="C108" s="378"/>
+      <c r="D108" s="379"/>
+      <c r="E108" s="378"/>
+      <c r="F108" s="378"/>
     </row>
     <row r="109" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A109"/>
-      <c r="B109" s="390"/>
-      <c r="C109" s="391"/>
-      <c r="D109" s="392"/>
-      <c r="E109" s="391"/>
-      <c r="F109" s="391"/>
+      <c r="B109" s="377"/>
+      <c r="C109" s="378"/>
+      <c r="D109" s="379"/>
+      <c r="E109" s="378"/>
+      <c r="F109" s="378"/>
     </row>
     <row r="110" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A110"/>
-      <c r="B110" s="390"/>
-      <c r="C110" s="391"/>
-      <c r="D110" s="392"/>
-      <c r="E110" s="391"/>
-      <c r="F110" s="391"/>
+      <c r="B110" s="377"/>
+      <c r="C110" s="378"/>
+      <c r="D110" s="379"/>
+      <c r="E110" s="378"/>
+      <c r="F110" s="378"/>
     </row>
     <row r="111" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A111"/>
-      <c r="B111" s="390"/>
-      <c r="C111" s="391"/>
-      <c r="D111" s="392"/>
-      <c r="E111" s="391"/>
-      <c r="F111" s="391"/>
+      <c r="B111" s="377"/>
+      <c r="C111" s="378"/>
+      <c r="D111" s="379"/>
+      <c r="E111" s="378"/>
+      <c r="F111" s="378"/>
     </row>
     <row r="112" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A112"/>
-      <c r="B112" s="390"/>
-      <c r="C112" s="391"/>
-      <c r="D112" s="392"/>
-      <c r="E112" s="391"/>
-      <c r="F112" s="391"/>
+      <c r="B112" s="377"/>
+      <c r="C112" s="378"/>
+      <c r="D112" s="379"/>
+      <c r="E112" s="378"/>
+      <c r="F112" s="378"/>
     </row>
     <row r="113" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A113"/>
-      <c r="B113" s="390"/>
-      <c r="C113" s="391"/>
-      <c r="D113" s="392"/>
-      <c r="E113" s="391"/>
-      <c r="F113" s="391"/>
+      <c r="B113" s="377"/>
+      <c r="C113" s="378"/>
+      <c r="D113" s="379"/>
+      <c r="E113" s="378"/>
+      <c r="F113" s="378"/>
     </row>
     <row r="114" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A114"/>
-      <c r="B114" s="390"/>
-      <c r="C114" s="391"/>
-      <c r="D114" s="392"/>
-      <c r="E114" s="391"/>
-      <c r="F114" s="391"/>
+      <c r="B114" s="377"/>
+      <c r="C114" s="378"/>
+      <c r="D114" s="379"/>
+      <c r="E114" s="378"/>
+      <c r="F114" s="378"/>
     </row>
     <row r="115" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A115"/>
-      <c r="B115" s="390"/>
-      <c r="C115" s="391"/>
-      <c r="D115" s="392"/>
-      <c r="E115" s="391"/>
-      <c r="F115" s="391"/>
+      <c r="B115" s="377"/>
+      <c r="C115" s="378"/>
+      <c r="D115" s="379"/>
+      <c r="E115" s="378"/>
+      <c r="F115" s="378"/>
     </row>
     <row r="116" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A116"/>
-      <c r="B116" s="390"/>
-      <c r="C116" s="391"/>
-      <c r="D116" s="392"/>
-      <c r="E116" s="391"/>
-      <c r="F116" s="391"/>
+      <c r="B116" s="377"/>
+      <c r="C116" s="378"/>
+      <c r="D116" s="379"/>
+      <c r="E116" s="378"/>
+      <c r="F116" s="378"/>
     </row>
     <row r="117" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A117"/>
-      <c r="B117" s="390"/>
-      <c r="C117" s="391"/>
-      <c r="D117" s="392"/>
-      <c r="E117" s="391"/>
-      <c r="F117" s="391"/>
+      <c r="B117" s="377"/>
+      <c r="C117" s="378"/>
+      <c r="D117" s="379"/>
+      <c r="E117" s="378"/>
+      <c r="F117" s="378"/>
     </row>
     <row r="118" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A118"/>
-      <c r="B118" s="390"/>
-      <c r="C118" s="391"/>
-      <c r="D118" s="392"/>
-      <c r="E118" s="391"/>
-      <c r="F118" s="391"/>
+      <c r="B118" s="377"/>
+      <c r="C118" s="378"/>
+      <c r="D118" s="379"/>
+      <c r="E118" s="378"/>
+      <c r="F118" s="378"/>
     </row>
     <row r="119" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A119"/>
-      <c r="B119" s="390"/>
-      <c r="C119" s="391"/>
-      <c r="D119" s="392"/>
-      <c r="E119" s="391"/>
-      <c r="F119" s="391"/>
+      <c r="B119" s="377"/>
+      <c r="C119" s="378"/>
+      <c r="D119" s="379"/>
+      <c r="E119" s="378"/>
+      <c r="F119" s="378"/>
     </row>
     <row r="120" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A120"/>
-      <c r="B120" s="390"/>
-      <c r="C120" s="391"/>
-      <c r="D120" s="392"/>
-      <c r="E120" s="391"/>
-      <c r="F120" s="391"/>
+      <c r="B120" s="377"/>
+      <c r="C120" s="378"/>
+      <c r="D120" s="379"/>
+      <c r="E120" s="378"/>
+      <c r="F120" s="378"/>
     </row>
     <row r="121" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A121"/>
-      <c r="B121" s="390"/>
-      <c r="C121" s="391"/>
-      <c r="D121" s="392"/>
-      <c r="E121" s="391"/>
-      <c r="F121" s="391"/>
+      <c r="B121" s="377"/>
+      <c r="C121" s="378"/>
+      <c r="D121" s="379"/>
+      <c r="E121" s="378"/>
+      <c r="F121" s="378"/>
     </row>
     <row r="122" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A122"/>
-      <c r="B122" s="390"/>
-      <c r="C122" s="391"/>
-      <c r="D122" s="392"/>
-      <c r="E122" s="391"/>
-      <c r="F122" s="391"/>
+      <c r="B122" s="377"/>
+      <c r="C122" s="378"/>
+      <c r="D122" s="379"/>
+      <c r="E122" s="378"/>
+      <c r="F122" s="378"/>
     </row>
     <row r="123" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A123"/>
-      <c r="B123" s="390"/>
-      <c r="C123" s="391"/>
-      <c r="D123" s="392"/>
-      <c r="E123" s="391"/>
-      <c r="F123" s="391"/>
+      <c r="B123" s="377"/>
+      <c r="C123" s="378"/>
+      <c r="D123" s="379"/>
+      <c r="E123" s="378"/>
+      <c r="F123" s="378"/>
     </row>
     <row r="124" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A124"/>
-      <c r="B124" s="390"/>
-      <c r="C124" s="391"/>
-      <c r="D124" s="392"/>
-      <c r="E124" s="391"/>
-      <c r="F124" s="391"/>
+      <c r="B124" s="377"/>
+      <c r="C124" s="378"/>
+      <c r="D124" s="379"/>
+      <c r="E124" s="378"/>
+      <c r="F124" s="378"/>
     </row>
     <row r="125" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A125"/>
-      <c r="B125" s="390"/>
-      <c r="C125" s="391"/>
-      <c r="D125" s="392"/>
-      <c r="E125" s="391"/>
-      <c r="F125" s="391"/>
+      <c r="B125" s="377"/>
+      <c r="C125" s="378"/>
+      <c r="D125" s="379"/>
+      <c r="E125" s="378"/>
+      <c r="F125" s="378"/>
     </row>
     <row r="126" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A126"/>
-      <c r="B126" s="390"/>
-      <c r="C126" s="391"/>
-      <c r="D126" s="392"/>
-      <c r="E126" s="391"/>
-      <c r="F126" s="391"/>
+      <c r="B126" s="377"/>
+      <c r="C126" s="378"/>
+      <c r="D126" s="379"/>
+      <c r="E126" s="378"/>
+      <c r="F126" s="378"/>
     </row>
     <row r="127" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A127"/>
-      <c r="B127" s="390"/>
-      <c r="C127" s="391"/>
-      <c r="D127" s="392"/>
-      <c r="E127" s="391"/>
-      <c r="F127" s="391"/>
+      <c r="B127" s="377"/>
+      <c r="C127" s="378"/>
+      <c r="D127" s="379"/>
+      <c r="E127" s="378"/>
+      <c r="F127" s="378"/>
     </row>
     <row r="128" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A128"/>
-      <c r="B128" s="390"/>
-      <c r="C128" s="391"/>
-      <c r="D128" s="392"/>
-      <c r="E128" s="391"/>
-      <c r="F128" s="391"/>
+      <c r="B128" s="377"/>
+      <c r="C128" s="378"/>
+      <c r="D128" s="379"/>
+      <c r="E128" s="378"/>
+      <c r="F128" s="378"/>
     </row>
     <row r="129" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A129"/>
-      <c r="B129" s="390"/>
-      <c r="C129" s="391"/>
-      <c r="D129" s="392"/>
-      <c r="E129" s="391"/>
-      <c r="F129" s="391"/>
+      <c r="B129" s="377"/>
+      <c r="C129" s="378"/>
+      <c r="D129" s="379"/>
+      <c r="E129" s="378"/>
+      <c r="F129" s="378"/>
     </row>
     <row r="130" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A130"/>
-      <c r="B130" s="390"/>
-      <c r="C130" s="391"/>
-      <c r="D130" s="392"/>
-      <c r="E130" s="391"/>
-      <c r="F130" s="391"/>
+      <c r="B130" s="377"/>
+      <c r="C130" s="378"/>
+      <c r="D130" s="379"/>
+      <c r="E130" s="378"/>
+      <c r="F130" s="378"/>
     </row>
     <row r="131" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A131"/>
-      <c r="B131" s="390"/>
-      <c r="C131" s="391"/>
-      <c r="D131" s="392"/>
-      <c r="E131" s="391"/>
-      <c r="F131" s="391"/>
+      <c r="B131" s="377"/>
+      <c r="C131" s="378"/>
+      <c r="D131" s="379"/>
+      <c r="E131" s="378"/>
+      <c r="F131" s="378"/>
     </row>
     <row r="132" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A132"/>
-      <c r="B132" s="390"/>
-      <c r="C132" s="391"/>
-      <c r="D132" s="392"/>
-      <c r="E132" s="391"/>
-      <c r="F132" s="391"/>
+      <c r="B132" s="377"/>
+      <c r="C132" s="378"/>
+      <c r="D132" s="379"/>
+      <c r="E132" s="378"/>
+      <c r="F132" s="378"/>
     </row>
     <row r="133" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A133"/>
-      <c r="B133" s="390"/>
-      <c r="C133" s="391"/>
-      <c r="D133" s="392"/>
-      <c r="E133" s="391"/>
-      <c r="F133" s="391"/>
+      <c r="B133" s="377"/>
+      <c r="C133" s="378"/>
+      <c r="D133" s="379"/>
+      <c r="E133" s="378"/>
+      <c r="F133" s="378"/>
     </row>
     <row r="134" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A134"/>
-      <c r="B134" s="390"/>
-      <c r="C134" s="391"/>
-      <c r="D134" s="392"/>
-      <c r="E134" s="391"/>
-      <c r="F134" s="391"/>
+      <c r="B134" s="377"/>
+      <c r="C134" s="378"/>
+      <c r="D134" s="379"/>
+      <c r="E134" s="378"/>
+      <c r="F134" s="378"/>
     </row>
     <row r="135" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A135"/>
-      <c r="B135" s="390"/>
-      <c r="C135" s="391"/>
-      <c r="D135" s="392"/>
-      <c r="E135" s="391"/>
-      <c r="F135" s="391"/>
+      <c r="B135" s="377"/>
+      <c r="C135" s="378"/>
+      <c r="D135" s="379"/>
+      <c r="E135" s="378"/>
+      <c r="F135" s="378"/>
     </row>
     <row r="136" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A136"/>
-      <c r="B136" s="390"/>
-      <c r="C136" s="391"/>
-      <c r="D136" s="392"/>
-      <c r="E136" s="391"/>
-      <c r="F136" s="391"/>
+      <c r="B136" s="377"/>
+      <c r="C136" s="378"/>
+      <c r="D136" s="379"/>
+      <c r="E136" s="378"/>
+      <c r="F136" s="378"/>
     </row>
     <row r="137" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A137"/>
-      <c r="B137" s="390"/>
-      <c r="C137" s="391"/>
-      <c r="D137" s="392"/>
-      <c r="E137" s="391"/>
-      <c r="F137" s="391"/>
+      <c r="B137" s="377"/>
+      <c r="C137" s="378"/>
+      <c r="D137" s="379"/>
+      <c r="E137" s="378"/>
+      <c r="F137" s="378"/>
     </row>
     <row r="138" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A138"/>
-      <c r="B138" s="390"/>
-      <c r="C138" s="391"/>
-      <c r="D138" s="392"/>
-      <c r="E138" s="391"/>
-      <c r="F138" s="391"/>
+      <c r="B138" s="377"/>
+      <c r="C138" s="378"/>
+      <c r="D138" s="379"/>
+      <c r="E138" s="378"/>
+      <c r="F138" s="378"/>
     </row>
     <row r="139" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A139"/>
-      <c r="B139" s="390"/>
-      <c r="C139" s="391"/>
-      <c r="D139" s="392"/>
-      <c r="E139" s="391"/>
-      <c r="F139" s="391"/>
+      <c r="B139" s="377"/>
+      <c r="C139" s="378"/>
+      <c r="D139" s="379"/>
+      <c r="E139" s="378"/>
+      <c r="F139" s="378"/>
     </row>
     <row r="140" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A140"/>
-      <c r="B140" s="390"/>
-      <c r="C140" s="391"/>
-      <c r="D140" s="392"/>
-      <c r="E140" s="391"/>
-      <c r="F140" s="391"/>
+      <c r="B140" s="377"/>
+      <c r="C140" s="378"/>
+      <c r="D140" s="379"/>
+      <c r="E140" s="378"/>
+      <c r="F140" s="378"/>
     </row>
     <row r="141" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A141"/>
-      <c r="B141" s="390"/>
-      <c r="C141" s="391"/>
-      <c r="D141" s="392"/>
-      <c r="E141" s="391"/>
-      <c r="F141" s="391"/>
+      <c r="B141" s="377"/>
+      <c r="C141" s="378"/>
+      <c r="D141" s="379"/>
+      <c r="E141" s="378"/>
+      <c r="F141" s="378"/>
     </row>
     <row r="142" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A142"/>
-      <c r="B142" s="390"/>
-      <c r="C142" s="391"/>
-      <c r="D142" s="392"/>
-      <c r="E142" s="391"/>
-      <c r="F142" s="391"/>
+      <c r="B142" s="377"/>
+      <c r="C142" s="378"/>
+      <c r="D142" s="379"/>
+      <c r="E142" s="378"/>
+      <c r="F142" s="378"/>
     </row>
     <row r="143" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A143"/>
-      <c r="B143" s="390"/>
-      <c r="C143" s="391"/>
-      <c r="D143" s="392"/>
-      <c r="E143" s="391"/>
-      <c r="F143" s="391"/>
+      <c r="B143" s="377"/>
+      <c r="C143" s="378"/>
+      <c r="D143" s="379"/>
+      <c r="E143" s="378"/>
+      <c r="F143" s="378"/>
     </row>
     <row r="144" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A144"/>
-      <c r="B144" s="390"/>
-      <c r="C144" s="391"/>
-      <c r="D144" s="392"/>
-      <c r="E144" s="391"/>
-      <c r="F144" s="391"/>
+      <c r="B144" s="377"/>
+      <c r="C144" s="378"/>
+      <c r="D144" s="379"/>
+      <c r="E144" s="378"/>
+      <c r="F144" s="378"/>
     </row>
     <row r="145" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A145"/>
-      <c r="B145" s="390"/>
-      <c r="C145" s="391"/>
-      <c r="D145" s="392"/>
-      <c r="E145" s="391"/>
-      <c r="F145" s="391"/>
+      <c r="B145" s="377"/>
+      <c r="C145" s="378"/>
+      <c r="D145" s="379"/>
+      <c r="E145" s="378"/>
+      <c r="F145" s="378"/>
     </row>
     <row r="146" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A146"/>
-      <c r="B146" s="390"/>
-      <c r="C146" s="391"/>
-      <c r="D146" s="392"/>
-      <c r="E146" s="391"/>
-      <c r="F146" s="391"/>
+      <c r="B146" s="377"/>
+      <c r="C146" s="378"/>
+      <c r="D146" s="379"/>
+      <c r="E146" s="378"/>
+      <c r="F146" s="378"/>
     </row>
     <row r="147" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A147"/>
-      <c r="B147" s="390"/>
-      <c r="C147" s="391"/>
-      <c r="D147" s="392"/>
-      <c r="E147" s="391"/>
-      <c r="F147" s="391"/>
+      <c r="B147" s="377"/>
+      <c r="C147" s="378"/>
+      <c r="D147" s="379"/>
+      <c r="E147" s="378"/>
+      <c r="F147" s="378"/>
     </row>
     <row r="148" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A148"/>
-      <c r="B148" s="390"/>
-      <c r="C148" s="391"/>
-      <c r="D148" s="392"/>
-      <c r="E148" s="391"/>
-      <c r="F148" s="391"/>
+      <c r="B148" s="377"/>
+      <c r="C148" s="378"/>
+      <c r="D148" s="379"/>
+      <c r="E148" s="378"/>
+      <c r="F148" s="378"/>
     </row>
     <row r="149" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A149"/>
-      <c r="B149" s="390"/>
-      <c r="C149" s="391"/>
-      <c r="D149" s="392"/>
-      <c r="E149" s="391"/>
-      <c r="F149" s="391"/>
+      <c r="B149" s="377"/>
+      <c r="C149" s="378"/>
+      <c r="D149" s="379"/>
+      <c r="E149" s="378"/>
+      <c r="F149" s="378"/>
     </row>
     <row r="150" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A150"/>
-      <c r="B150" s="390"/>
-      <c r="C150" s="391"/>
-      <c r="D150" s="392"/>
-      <c r="E150" s="391"/>
-      <c r="F150" s="391"/>
+      <c r="B150" s="377"/>
+      <c r="C150" s="378"/>
+      <c r="D150" s="379"/>
+      <c r="E150" s="378"/>
+      <c r="F150" s="378"/>
     </row>
     <row r="151" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A151"/>
-      <c r="B151" s="390"/>
-      <c r="C151" s="391"/>
-      <c r="D151" s="392"/>
-      <c r="E151" s="391"/>
-      <c r="F151" s="391"/>
+      <c r="B151" s="377"/>
+      <c r="C151" s="378"/>
+      <c r="D151" s="379"/>
+      <c r="E151" s="378"/>
+      <c r="F151" s="378"/>
     </row>
     <row r="152" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A152"/>
-      <c r="B152" s="390"/>
-      <c r="C152" s="391"/>
-      <c r="D152" s="392"/>
-      <c r="E152" s="391"/>
-      <c r="F152" s="391"/>
+      <c r="B152" s="377"/>
+      <c r="C152" s="378"/>
+      <c r="D152" s="379"/>
+      <c r="E152" s="378"/>
+      <c r="F152" s="378"/>
     </row>
     <row r="153" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A153"/>
-      <c r="B153" s="390"/>
-      <c r="C153" s="391"/>
-      <c r="D153" s="392"/>
-      <c r="E153" s="391"/>
-      <c r="F153" s="391"/>
+      <c r="B153" s="377"/>
+      <c r="C153" s="378"/>
+      <c r="D153" s="379"/>
+      <c r="E153" s="378"/>
+      <c r="F153" s="378"/>
     </row>
     <row r="154" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A154"/>
-      <c r="B154" s="390"/>
-      <c r="C154" s="391"/>
-      <c r="D154" s="392"/>
-      <c r="E154" s="391"/>
-      <c r="F154" s="391"/>
+      <c r="B154" s="377"/>
+      <c r="C154" s="378"/>
+      <c r="D154" s="379"/>
+      <c r="E154" s="378"/>
+      <c r="F154" s="378"/>
     </row>
     <row r="155" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A155"/>
-      <c r="B155" s="390"/>
-      <c r="C155" s="391"/>
-      <c r="D155" s="392"/>
-      <c r="E155" s="391"/>
-      <c r="F155" s="391"/>
+      <c r="B155" s="377"/>
+      <c r="C155" s="378"/>
+      <c r="D155" s="379"/>
+      <c r="E155" s="378"/>
+      <c r="F155" s="378"/>
     </row>
     <row r="156" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A156"/>
-      <c r="B156" s="390"/>
-      <c r="C156" s="391"/>
-      <c r="D156" s="392"/>
-      <c r="E156" s="391"/>
-      <c r="F156" s="391"/>
+      <c r="B156" s="377"/>
+      <c r="C156" s="378"/>
+      <c r="D156" s="379"/>
+      <c r="E156" s="378"/>
+      <c r="F156" s="378"/>
     </row>
     <row r="157" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A157"/>
-      <c r="B157" s="390"/>
-      <c r="C157" s="391"/>
-      <c r="D157" s="392"/>
-      <c r="E157" s="391"/>
-      <c r="F157" s="391"/>
+      <c r="B157" s="377"/>
+      <c r="C157" s="378"/>
+      <c r="D157" s="379"/>
+      <c r="E157" s="378"/>
+      <c r="F157" s="378"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -11612,7 +12028,7 @@
   <sheetData>
     <row r="3" spans="3:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:3" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="337" t="s">
+      <c r="C4" s="335" t="s">
         <v>185</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CIERRE 28 Sept 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
+++ b/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="474">
   <si>
     <t xml:space="preserve">RELACION DE UNIDADES Y ASIGNACION </t>
   </si>
@@ -1491,6 +1491,12 @@
   </si>
   <si>
     <t>6-Sept-22      245,739 KM</t>
+  </si>
+  <si>
+    <t>9-SEPT-2022   294,000 KM</t>
+  </si>
+  <si>
+    <t>MIGUEL</t>
   </si>
 </sst>
 </file>
@@ -3426,6 +3432,21 @@
     <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3457,21 +3478,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="47" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4856,14 +4862,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="384" t="s">
+      <c r="B1" s="389" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="384"/>
-      <c r="D1" s="384"/>
-      <c r="E1" s="385"/>
-      <c r="F1" s="384"/>
-      <c r="G1" s="384"/>
+      <c r="C1" s="389"/>
+      <c r="D1" s="389"/>
+      <c r="E1" s="390"/>
+      <c r="F1" s="389"/>
+      <c r="G1" s="389"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -5224,10 +5230,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="386" t="s">
+      <c r="L12" s="391" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="387"/>
+      <c r="M12" s="392"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -6422,14 +6428,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="384" t="s">
+      <c r="B1" s="389" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="384"/>
-      <c r="D1" s="384"/>
-      <c r="E1" s="385"/>
-      <c r="F1" s="384"/>
-      <c r="G1" s="384"/>
+      <c r="C1" s="389"/>
+      <c r="D1" s="389"/>
+      <c r="E1" s="390"/>
+      <c r="F1" s="389"/>
+      <c r="G1" s="389"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -6768,10 +6774,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="386" t="s">
+      <c r="L12" s="391" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="387"/>
+      <c r="M12" s="392"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -7748,14 +7754,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="388" t="s">
+      <c r="B1" s="393" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="388"/>
-      <c r="D1" s="388"/>
-      <c r="E1" s="389"/>
-      <c r="F1" s="388"/>
-      <c r="G1" s="388"/>
+      <c r="C1" s="393"/>
+      <c r="D1" s="393"/>
+      <c r="E1" s="394"/>
+      <c r="F1" s="393"/>
+      <c r="G1" s="393"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
@@ -8086,8 +8092,8 @@
       <c r="H12" s="228"/>
       <c r="I12" s="137"/>
       <c r="J12" s="137"/>
-      <c r="K12" s="390"/>
-      <c r="L12" s="391"/>
+      <c r="K12" s="395"/>
+      <c r="L12" s="396"/>
       <c r="M12" s="213"/>
       <c r="N12" s="213"/>
       <c r="O12" s="213"/>
@@ -9155,8 +9161,8 @@
   </sheetPr>
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -9183,14 +9189,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="388" t="s">
+      <c r="B1" s="393" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="388"/>
-      <c r="D1" s="388"/>
-      <c r="E1" s="389"/>
-      <c r="F1" s="388"/>
-      <c r="G1" s="388"/>
+      <c r="C1" s="393"/>
+      <c r="D1" s="393"/>
+      <c r="E1" s="394"/>
+      <c r="F1" s="393"/>
+      <c r="G1" s="393"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
@@ -9611,10 +9617,10 @@
       <c r="H14" s="331" t="s">
         <v>321</v>
       </c>
-      <c r="I14" s="399" t="s">
+      <c r="I14" s="388" t="s">
         <v>348</v>
       </c>
-      <c r="J14" s="398" t="s">
+      <c r="J14" s="387" t="s">
         <v>471</v>
       </c>
       <c r="K14" s="266"/>
@@ -9643,17 +9649,21 @@
       <c r="E15" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="329"/>
+      <c r="F15" s="329" t="s">
+        <v>51</v>
+      </c>
       <c r="G15" s="233" t="s">
         <v>82</v>
       </c>
       <c r="H15" s="137" t="s">
         <v>328</v>
       </c>
-      <c r="I15" s="287" t="s">
+      <c r="I15" s="269" t="s">
         <v>359</v>
       </c>
-      <c r="J15" s="137"/>
+      <c r="J15" s="100" t="s">
+        <v>472</v>
+      </c>
       <c r="K15" s="106"/>
       <c r="L15" s="137"/>
       <c r="M15" s="137"/>
@@ -9908,7 +9918,7 @@
         <v>74</v>
       </c>
       <c r="F22" s="330" t="s">
-        <v>51</v>
+        <v>473</v>
       </c>
       <c r="G22" s="218" t="s">
         <v>86</v>
@@ -10071,7 +10081,7 @@
       <c r="E26" s="298" t="s">
         <v>74</v>
       </c>
-      <c r="F26" s="396" t="s">
+      <c r="F26" s="385" t="s">
         <v>388</v>
       </c>
       <c r="G26" s="218"/>
@@ -10105,7 +10115,7 @@
       <c r="E27" s="298" t="s">
         <v>74</v>
       </c>
-      <c r="F27" s="397"/>
+      <c r="F27" s="386"/>
       <c r="G27" s="218"/>
       <c r="H27" s="304"/>
       <c r="I27" s="269"/>
@@ -10137,7 +10147,7 @@
       <c r="E28" s="298" t="s">
         <v>74</v>
       </c>
-      <c r="F28" s="397"/>
+      <c r="F28" s="386"/>
       <c r="G28" s="218"/>
       <c r="H28" s="304"/>
       <c r="I28" s="269"/>
@@ -10169,7 +10179,7 @@
       <c r="E29" s="298" t="s">
         <v>74</v>
       </c>
-      <c r="F29" s="397"/>
+      <c r="F29" s="386"/>
       <c r="G29" s="218"/>
       <c r="H29" s="304"/>
       <c r="I29" s="269"/>
@@ -10195,7 +10205,7 @@
       <c r="C30" s="248" t="s">
         <v>195</v>
       </c>
-      <c r="D30" s="395" t="s">
+      <c r="D30" s="384" t="s">
         <v>462</v>
       </c>
       <c r="E30" s="298" t="s">
@@ -10354,11 +10364,11 @@
       <c r="A1" s="336" t="s">
         <v>368</v>
       </c>
-      <c r="B1" s="392"/>
-      <c r="C1" s="392"/>
-      <c r="D1" s="392"/>
-      <c r="E1" s="392"/>
-      <c r="F1" s="392"/>
+      <c r="B1" s="397"/>
+      <c r="C1" s="397"/>
+      <c r="D1" s="397"/>
+      <c r="E1" s="397"/>
+      <c r="F1" s="397"/>
     </row>
     <row r="2" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="337" t="s">
@@ -10799,12 +10809,12 @@
       <c r="F24" s="349" t="s">
         <v>380</v>
       </c>
-      <c r="G24" s="393"/>
-      <c r="H24" s="394"/>
-      <c r="I24" s="394"/>
-      <c r="J24" s="394"/>
-      <c r="K24" s="394"/>
-      <c r="L24" s="394"/>
+      <c r="G24" s="398"/>
+      <c r="H24" s="399"/>
+      <c r="I24" s="399"/>
+      <c r="J24" s="399"/>
+      <c r="K24" s="399"/>
+      <c r="L24" s="399"/>
     </row>
     <row r="25" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="345">

</xml_diff>

<commit_message>
cierre 20 oct 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
+++ b/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="478">
   <si>
     <t xml:space="preserve">RELACION DE UNIDADES Y ASIGNACION </t>
   </si>
@@ -1506,6 +1506,9 @@
   </si>
   <si>
     <t>28-Mar-22    11,931.00 KM</t>
+  </si>
+  <si>
+    <t>20-Oct-22  YA LE TOCA SERVICIO  70,082 KM</t>
   </si>
 </sst>
 </file>
@@ -2376,7 +2379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="401">
+  <cellXfs count="402">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3499,6 +3502,9 @@
     </xf>
     <xf numFmtId="0" fontId="47" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3508,10 +3514,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF9966FF"/>
       <color rgb="FFFFCCFF"/>
       <color rgb="FF00FF00"/>
       <color rgb="FF00FFFF"/>
-      <color rgb="FF9966FF"/>
       <color rgb="FFCC6600"/>
       <color rgb="FFFF9900"/>
       <color rgb="FF9999FF"/>
@@ -6236,7 +6242,7 @@
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
     </row>
-    <row r="34" spans="1:20" ht="71.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:20" ht="85.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="15">
         <v>31</v>
       </c>
@@ -7821,7 +7827,7 @@
       <c r="M2" s="254"/>
       <c r="N2" s="254"/>
     </row>
-    <row r="3" spans="1:19" ht="71.25" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:19" ht="94.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="205">
         <v>1</v>
       </c>
@@ -9181,8 +9187,8 @@
   </sheetPr>
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -10249,7 +10255,9 @@
       <c r="K30" s="334" t="s">
         <v>365</v>
       </c>
-      <c r="L30" s="137"/>
+      <c r="L30" s="401" t="s">
+        <v>477</v>
+      </c>
       <c r="M30" s="137"/>
       <c r="N30" s="213"/>
       <c r="O30" s="213"/>

</xml_diff>

<commit_message>
cierre 25 oct 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
+++ b/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="479">
   <si>
     <t xml:space="preserve">RELACION DE UNIDADES Y ASIGNACION </t>
   </si>
@@ -1509,6 +1509,9 @@
   </si>
   <si>
     <t>20-Oct-22  YA LE TOCA SERVICIO  70,082 KM</t>
+  </si>
+  <si>
+    <t>13-Oct-22  cambio tacometro</t>
   </si>
 </sst>
 </file>
@@ -2379,7 +2382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="402">
+  <cellXfs count="403">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3470,6 +3473,9 @@
     <xf numFmtId="15" fontId="50" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3503,7 +3509,7 @@
     <xf numFmtId="0" fontId="47" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3514,13 +3520,13 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF9999FF"/>
       <color rgb="FF9966FF"/>
       <color rgb="FFFFCCFF"/>
       <color rgb="FF00FF00"/>
       <color rgb="FF00FFFF"/>
       <color rgb="FFCC6600"/>
       <color rgb="FFFF9900"/>
-      <color rgb="FF9999FF"/>
       <color rgb="FFFF00FF"/>
       <color rgb="FF3399FF"/>
       <color rgb="FF99CCFF"/>
@@ -4888,14 +4894,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="390" t="s">
+      <c r="B1" s="391" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="390"/>
-      <c r="D1" s="390"/>
-      <c r="E1" s="391"/>
-      <c r="F1" s="390"/>
-      <c r="G1" s="390"/>
+      <c r="C1" s="391"/>
+      <c r="D1" s="391"/>
+      <c r="E1" s="392"/>
+      <c r="F1" s="391"/>
+      <c r="G1" s="391"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -5256,10 +5262,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="392" t="s">
+      <c r="L12" s="393" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="393"/>
+      <c r="M12" s="394"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -6242,7 +6248,7 @@
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
     </row>
-    <row r="34" spans="1:20" ht="85.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:20" ht="71.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="15">
         <v>31</v>
       </c>
@@ -6454,14 +6460,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="390" t="s">
+      <c r="B1" s="391" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="390"/>
-      <c r="D1" s="390"/>
-      <c r="E1" s="391"/>
-      <c r="F1" s="390"/>
-      <c r="G1" s="390"/>
+      <c r="C1" s="391"/>
+      <c r="D1" s="391"/>
+      <c r="E1" s="392"/>
+      <c r="F1" s="391"/>
+      <c r="G1" s="391"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -6800,10 +6806,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="392" t="s">
+      <c r="L12" s="393" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="393"/>
+      <c r="M12" s="394"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -7780,14 +7786,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="394" t="s">
+      <c r="B1" s="395" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="394"/>
-      <c r="D1" s="394"/>
-      <c r="E1" s="395"/>
-      <c r="F1" s="394"/>
-      <c r="G1" s="394"/>
+      <c r="C1" s="395"/>
+      <c r="D1" s="395"/>
+      <c r="E1" s="396"/>
+      <c r="F1" s="395"/>
+      <c r="G1" s="395"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
@@ -7827,7 +7833,7 @@
       <c r="M2" s="254"/>
       <c r="N2" s="254"/>
     </row>
-    <row r="3" spans="1:19" ht="94.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:19" ht="71.25" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="205">
         <v>1</v>
       </c>
@@ -8118,8 +8124,8 @@
       <c r="H12" s="228"/>
       <c r="I12" s="137"/>
       <c r="J12" s="137"/>
-      <c r="K12" s="396"/>
-      <c r="L12" s="397"/>
+      <c r="K12" s="397"/>
+      <c r="L12" s="398"/>
       <c r="M12" s="213"/>
       <c r="N12" s="213"/>
       <c r="O12" s="213"/>
@@ -9187,8 +9193,8 @@
   </sheetPr>
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -9215,14 +9221,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="394" t="s">
+      <c r="B1" s="395" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="394"/>
-      <c r="D1" s="394"/>
-      <c r="E1" s="395"/>
-      <c r="F1" s="394"/>
-      <c r="G1" s="394"/>
+      <c r="C1" s="395"/>
+      <c r="D1" s="395"/>
+      <c r="E1" s="396"/>
+      <c r="F1" s="395"/>
+      <c r="G1" s="395"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
@@ -9803,7 +9809,9 @@
       <c r="I18" s="291" t="s">
         <v>366</v>
       </c>
-      <c r="J18" s="137"/>
+      <c r="J18" s="402" t="s">
+        <v>478</v>
+      </c>
       <c r="K18" s="213"/>
       <c r="L18" s="213"/>
       <c r="M18" s="213"/>
@@ -10255,7 +10263,7 @@
       <c r="K30" s="334" t="s">
         <v>365</v>
       </c>
-      <c r="L30" s="401" t="s">
+      <c r="L30" s="390" t="s">
         <v>477</v>
       </c>
       <c r="M30" s="137"/>
@@ -10398,11 +10406,11 @@
       <c r="A1" s="336" t="s">
         <v>368</v>
       </c>
-      <c r="B1" s="398"/>
-      <c r="C1" s="398"/>
-      <c r="D1" s="398"/>
-      <c r="E1" s="398"/>
-      <c r="F1" s="398"/>
+      <c r="B1" s="399"/>
+      <c r="C1" s="399"/>
+      <c r="D1" s="399"/>
+      <c r="E1" s="399"/>
+      <c r="F1" s="399"/>
     </row>
     <row r="2" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="337" t="s">
@@ -10843,12 +10851,12 @@
       <c r="F24" s="349" t="s">
         <v>380</v>
       </c>
-      <c r="G24" s="399"/>
-      <c r="H24" s="400"/>
-      <c r="I24" s="400"/>
-      <c r="J24" s="400"/>
-      <c r="K24" s="400"/>
-      <c r="L24" s="400"/>
+      <c r="G24" s="400"/>
+      <c r="H24" s="401"/>
+      <c r="I24" s="401"/>
+      <c r="J24" s="401"/>
+      <c r="K24" s="401"/>
+      <c r="L24" s="401"/>
     </row>
     <row r="25" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="345">

</xml_diff>

<commit_message>
cierre  17 ago 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
+++ b/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="535">
   <si>
     <t xml:space="preserve">RELACION DE UNIDADES Y ASIGNACION </t>
   </si>
@@ -1728,6 +1728,9 @@
   </si>
   <si>
     <t>1-ABR-2023     276,634  KM</t>
+  </si>
+  <si>
+    <t>OSIRIS</t>
   </si>
 </sst>
 </file>
@@ -3892,6 +3895,9 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="48" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3923,9 +3929,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="47" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5887,14 +5890,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="458" t="s">
+      <c r="B1" s="459" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="458"/>
-      <c r="D1" s="458"/>
-      <c r="E1" s="459"/>
-      <c r="F1" s="458"/>
-      <c r="G1" s="458"/>
+      <c r="C1" s="459"/>
+      <c r="D1" s="459"/>
+      <c r="E1" s="460"/>
+      <c r="F1" s="459"/>
+      <c r="G1" s="459"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -6255,10 +6258,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="460" t="s">
+      <c r="L12" s="461" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="461"/>
+      <c r="M12" s="462"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -7453,14 +7456,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="458" t="s">
+      <c r="B1" s="459" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="458"/>
-      <c r="D1" s="458"/>
-      <c r="E1" s="459"/>
-      <c r="F1" s="458"/>
-      <c r="G1" s="458"/>
+      <c r="C1" s="459"/>
+      <c r="D1" s="459"/>
+      <c r="E1" s="460"/>
+      <c r="F1" s="459"/>
+      <c r="G1" s="459"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -7799,10 +7802,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="460" t="s">
+      <c r="L12" s="461" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="461"/>
+      <c r="M12" s="462"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -8779,14 +8782,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="462" t="s">
+      <c r="B1" s="463" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="462"/>
-      <c r="D1" s="462"/>
-      <c r="E1" s="463"/>
-      <c r="F1" s="462"/>
-      <c r="G1" s="462"/>
+      <c r="C1" s="463"/>
+      <c r="D1" s="463"/>
+      <c r="E1" s="464"/>
+      <c r="F1" s="463"/>
+      <c r="G1" s="463"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
@@ -9117,8 +9120,8 @@
       <c r="H12" s="228"/>
       <c r="I12" s="137"/>
       <c r="J12" s="137"/>
-      <c r="K12" s="464"/>
-      <c r="L12" s="465"/>
+      <c r="K12" s="465"/>
+      <c r="L12" s="466"/>
       <c r="M12" s="213"/>
       <c r="N12" s="213"/>
       <c r="O12" s="213"/>
@@ -10186,8 +10189,8 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -10206,14 +10209,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="462" t="s">
+      <c r="B1" s="463" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="462"/>
-      <c r="D1" s="462"/>
-      <c r="E1" s="463"/>
-      <c r="F1" s="462"/>
-      <c r="G1" s="462"/>
+      <c r="C1" s="463"/>
+      <c r="D1" s="463"/>
+      <c r="E1" s="464"/>
+      <c r="F1" s="463"/>
+      <c r="G1" s="463"/>
     </row>
     <row r="2" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
@@ -10734,7 +10737,7 @@
       <c r="E21" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F21" s="469" t="s">
+      <c r="F21" s="458" t="s">
         <v>387</v>
       </c>
       <c r="G21" s="407"/>
@@ -10760,7 +10763,7 @@
         <v>74</v>
       </c>
       <c r="F22" s="400" t="s">
-        <v>7</v>
+        <v>534</v>
       </c>
       <c r="G22" s="407" t="s">
         <v>94</v>
@@ -11136,14 +11139,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="462" t="s">
+      <c r="B1" s="463" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="462"/>
-      <c r="D1" s="462"/>
-      <c r="E1" s="463"/>
-      <c r="F1" s="462"/>
-      <c r="G1" s="462"/>
+      <c r="C1" s="463"/>
+      <c r="D1" s="463"/>
+      <c r="E1" s="464"/>
+      <c r="F1" s="463"/>
+      <c r="G1" s="463"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
@@ -12353,11 +12356,11 @@
       <c r="A1" s="335" t="s">
         <v>367</v>
       </c>
-      <c r="B1" s="466"/>
-      <c r="C1" s="466"/>
-      <c r="D1" s="466"/>
-      <c r="E1" s="466"/>
-      <c r="F1" s="466"/>
+      <c r="B1" s="467"/>
+      <c r="C1" s="467"/>
+      <c r="D1" s="467"/>
+      <c r="E1" s="467"/>
+      <c r="F1" s="467"/>
     </row>
     <row r="2" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="336" t="s">
@@ -12798,12 +12801,12 @@
       <c r="F24" s="348" t="s">
         <v>379</v>
       </c>
-      <c r="G24" s="467"/>
-      <c r="H24" s="468"/>
-      <c r="I24" s="468"/>
-      <c r="J24" s="468"/>
-      <c r="K24" s="468"/>
-      <c r="L24" s="468"/>
+      <c r="G24" s="468"/>
+      <c r="H24" s="469"/>
+      <c r="I24" s="469"/>
+      <c r="J24" s="469"/>
+      <c r="K24" s="469"/>
+      <c r="L24" s="469"/>
     </row>
     <row r="25" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="344">

</xml_diff>

<commit_message>
CIERRE 23 SEPT 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
+++ b/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="539">
   <si>
     <t xml:space="preserve">RELACION DE UNIDADES Y ASIGNACION </t>
   </si>
@@ -1740,6 +1740,9 @@
   </si>
   <si>
     <t>30-Ago-23    192,573 KM</t>
+  </si>
+  <si>
+    <t>1-Sept-23    105,134 KM</t>
   </si>
 </sst>
 </file>
@@ -10198,8 +10201,8 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -10921,8 +10924,11 @@
       <c r="H27" s="428" t="s">
         <v>497</v>
       </c>
-      <c r="I27" s="313" t="s">
+      <c r="I27" s="246" t="s">
         <v>520</v>
+      </c>
+      <c r="J27" s="452" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
CIERRE 21 OCT 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
+++ b/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1323" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="549">
   <si>
     <t xml:space="preserve">RELACION DE UNIDADES Y ASIGNACION </t>
   </si>
@@ -1752,6 +1752,27 @@
   </si>
   <si>
     <t xml:space="preserve">4-May-23     4,089 KM                ( 20,000 ) </t>
+  </si>
+  <si>
+    <t>3-May-23    257,270  KM</t>
+  </si>
+  <si>
+    <t>9-Mar-23    263,000 KM</t>
+  </si>
+  <si>
+    <t>5-Sept-23    275,101 KM</t>
+  </si>
+  <si>
+    <t>5-Sept-23    86,551 KM</t>
+  </si>
+  <si>
+    <t>22-May-23  166,735  KM</t>
+  </si>
+  <si>
+    <t>19-Oct-23    289,142 KM</t>
+  </si>
+  <si>
+    <t>25-Jul-23     32,000 KM</t>
   </si>
 </sst>
 </file>
@@ -2640,7 +2661,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="473">
+  <cellXfs count="476">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3781,9 +3802,6 @@
     <xf numFmtId="0" fontId="48" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="48" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3926,8 +3944,17 @@
     <xf numFmtId="0" fontId="48" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3962,17 +3989,18 @@
     <xf numFmtId="0" fontId="47" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="12" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3982,9 +4010,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF9999FF"/>
       <color rgb="FF9966FF"/>
       <color rgb="FFCC6600"/>
-      <color rgb="FF9999FF"/>
       <color rgb="FF0000FF"/>
       <color rgb="FF0066FF"/>
       <color rgb="FF99CCFF"/>
@@ -5933,14 +5961,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="458" t="s">
+      <c r="B1" s="460" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="458"/>
-      <c r="D1" s="458"/>
-      <c r="E1" s="459"/>
-      <c r="F1" s="458"/>
-      <c r="G1" s="458"/>
+      <c r="C1" s="460"/>
+      <c r="D1" s="460"/>
+      <c r="E1" s="461"/>
+      <c r="F1" s="460"/>
+      <c r="G1" s="460"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -6301,10 +6329,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="460" t="s">
+      <c r="L12" s="462" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="461"/>
+      <c r="M12" s="463"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -7499,14 +7527,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="458" t="s">
+      <c r="B1" s="460" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="458"/>
-      <c r="D1" s="458"/>
-      <c r="E1" s="459"/>
-      <c r="F1" s="458"/>
-      <c r="G1" s="458"/>
+      <c r="C1" s="460"/>
+      <c r="D1" s="460"/>
+      <c r="E1" s="461"/>
+      <c r="F1" s="460"/>
+      <c r="G1" s="460"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -7845,10 +7873,10 @@
       <c r="K12" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="460" t="s">
+      <c r="L12" s="462" t="s">
         <v>197</v>
       </c>
-      <c r="M12" s="461"/>
+      <c r="M12" s="463"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -8825,14 +8853,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="462" t="s">
+      <c r="B1" s="464" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="462"/>
-      <c r="D1" s="462"/>
-      <c r="E1" s="463"/>
-      <c r="F1" s="462"/>
-      <c r="G1" s="462"/>
+      <c r="C1" s="464"/>
+      <c r="D1" s="464"/>
+      <c r="E1" s="465"/>
+      <c r="F1" s="464"/>
+      <c r="G1" s="464"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
@@ -9163,8 +9191,8 @@
       <c r="H12" s="228"/>
       <c r="I12" s="137"/>
       <c r="J12" s="137"/>
-      <c r="K12" s="464"/>
-      <c r="L12" s="465"/>
+      <c r="K12" s="466"/>
+      <c r="L12" s="467"/>
       <c r="M12" s="213"/>
       <c r="N12" s="213"/>
       <c r="O12" s="213"/>
@@ -10232,8 +10260,8 @@
   </sheetPr>
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -10253,14 +10281,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="462" t="s">
+      <c r="B1" s="464" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="462"/>
-      <c r="D1" s="462"/>
-      <c r="E1" s="463"/>
-      <c r="F1" s="462"/>
-      <c r="G1" s="462"/>
+      <c r="C1" s="464"/>
+      <c r="D1" s="464"/>
+      <c r="E1" s="465"/>
+      <c r="F1" s="464"/>
+      <c r="G1" s="464"/>
     </row>
     <row r="2" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
@@ -10489,7 +10517,7 @@
       <c r="G10" s="401" t="s">
         <v>94</v>
       </c>
-      <c r="H10" s="427" t="s">
+      <c r="H10" s="426" t="s">
         <v>514</v>
       </c>
       <c r="I10" s="286" t="s">
@@ -10516,7 +10544,7 @@
         <v>110</v>
       </c>
       <c r="G11" s="401"/>
-      <c r="H11" s="450" t="s">
+      <c r="H11" s="449" t="s">
         <v>507</v>
       </c>
       <c r="I11" s="286" t="s">
@@ -10545,10 +10573,13 @@
       <c r="G12" s="406" t="s">
         <v>84</v>
       </c>
-      <c r="H12" s="65" t="s">
+      <c r="H12" s="92" t="s">
         <v>492</v>
       </c>
-      <c r="I12" s="268"/>
+      <c r="I12" s="286" t="s">
+        <v>542</v>
+      </c>
+      <c r="J12" s="472"/>
     </row>
     <row r="13" spans="1:10" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="205">
@@ -10572,10 +10603,15 @@
       <c r="G13" s="406" t="s">
         <v>71</v>
       </c>
-      <c r="H13" s="408" t="s">
+      <c r="H13" s="473" t="s">
         <v>494</v>
       </c>
-      <c r="I13" s="387"/>
+      <c r="I13" s="387" t="s">
+        <v>543</v>
+      </c>
+      <c r="J13" s="100" t="s">
+        <v>544</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="205">
@@ -10593,19 +10629,19 @@
       <c r="E14" s="405" t="s">
         <v>74</v>
       </c>
-      <c r="F14" s="409" t="s">
+      <c r="F14" s="408" t="s">
         <v>51</v>
       </c>
       <c r="G14" s="401" t="s">
         <v>82</v>
       </c>
-      <c r="H14" s="450" t="s">
+      <c r="H14" s="449" t="s">
         <v>495</v>
       </c>
       <c r="I14" s="268" t="s">
         <v>522</v>
       </c>
-      <c r="J14" s="451" t="s">
+      <c r="J14" s="450" t="s">
         <v>523</v>
       </c>
     </row>
@@ -10625,13 +10661,13 @@
       <c r="E15" s="405" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="410" t="s">
+      <c r="F15" s="409" t="s">
         <v>19</v>
       </c>
       <c r="G15" s="401" t="s">
         <v>83</v>
       </c>
-      <c r="H15" s="450" t="s">
+      <c r="H15" s="449" t="s">
         <v>485</v>
       </c>
       <c r="I15" s="286" t="s">
@@ -10654,37 +10690,39 @@
       <c r="E16" s="405" t="s">
         <v>74</v>
       </c>
-      <c r="F16" s="411" t="s">
+      <c r="F16" s="410" t="s">
         <v>5</v>
       </c>
       <c r="G16" s="401" t="s">
         <v>79</v>
       </c>
-      <c r="H16" s="403" t="s">
+      <c r="H16" s="449" t="s">
         <v>508</v>
       </c>
-      <c r="I16" s="199"/>
-    </row>
-    <row r="17" spans="1:15" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I16" s="450" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="65.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="205">
         <v>15</v>
       </c>
-      <c r="B17" s="412" t="s">
+      <c r="B17" s="411" t="s">
         <v>53</v>
       </c>
       <c r="C17" s="397">
         <v>2018</v>
       </c>
-      <c r="D17" s="413" t="s">
+      <c r="D17" s="412" t="s">
         <v>54</v>
       </c>
       <c r="E17" s="399" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="414" t="s">
+      <c r="F17" s="413" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="415"/>
+      <c r="G17" s="414"/>
       <c r="H17" s="65" t="s">
         <v>476</v>
       </c>
@@ -10694,23 +10732,23 @@
       <c r="A18" s="205">
         <v>16</v>
       </c>
-      <c r="B18" s="416" t="s">
+      <c r="B18" s="415" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="417">
+      <c r="C18" s="416">
         <v>2006</v>
       </c>
-      <c r="D18" s="418" t="s">
+      <c r="D18" s="417" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="419" t="s">
+      <c r="E18" s="418" t="s">
         <v>74</v>
       </c>
-      <c r="F18" s="414" t="s">
+      <c r="F18" s="413" t="s">
         <v>17</v>
       </c>
       <c r="G18" s="406"/>
-      <c r="H18" s="420" t="s">
+      <c r="H18" s="419" t="s">
         <v>254</v>
       </c>
       <c r="I18" s="213"/>
@@ -10719,28 +10757,28 @@
       <c r="A19" s="205">
         <v>17</v>
       </c>
-      <c r="B19" s="412" t="s">
+      <c r="B19" s="411" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="421">
+      <c r="C19" s="420">
         <v>2018</v>
       </c>
-      <c r="D19" s="422" t="s">
+      <c r="D19" s="421" t="s">
         <v>505</v>
       </c>
-      <c r="E19" s="419" t="s">
+      <c r="E19" s="418" t="s">
         <v>74</v>
       </c>
-      <c r="F19" s="423" t="s">
+      <c r="F19" s="422" t="s">
         <v>199</v>
       </c>
-      <c r="G19" s="424" t="s">
+      <c r="G19" s="423" t="s">
         <v>95</v>
       </c>
       <c r="H19" s="403" t="s">
         <v>506</v>
       </c>
-      <c r="I19" s="457" t="s">
+      <c r="I19" s="471" t="s">
         <v>534</v>
       </c>
     </row>
@@ -10760,16 +10798,18 @@
       <c r="E20" s="405" t="s">
         <v>74</v>
       </c>
-      <c r="F20" s="423" t="s">
+      <c r="F20" s="422" t="s">
         <v>151</v>
       </c>
       <c r="G20" s="406" t="s">
         <v>85</v>
       </c>
-      <c r="H20" s="403" t="s">
+      <c r="H20" s="449" t="s">
         <v>355</v>
       </c>
-      <c r="I20" s="148"/>
+      <c r="I20" s="474" t="s">
+        <v>546</v>
+      </c>
     </row>
     <row r="21" spans="1:15" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="205">
@@ -10787,14 +10827,16 @@
       <c r="E21" s="236" t="s">
         <v>74</v>
       </c>
-      <c r="F21" s="456" t="s">
+      <c r="F21" s="455" t="s">
         <v>387</v>
       </c>
       <c r="G21" s="406"/>
-      <c r="H21" s="403" t="s">
+      <c r="H21" s="449" t="s">
         <v>531</v>
       </c>
-      <c r="I21" s="148"/>
+      <c r="I21" s="474" t="s">
+        <v>547</v>
+      </c>
     </row>
     <row r="22" spans="1:15" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="205">
@@ -10818,13 +10860,13 @@
       <c r="G22" s="406" t="s">
         <v>94</v>
       </c>
-      <c r="H22" s="449" t="s">
+      <c r="H22" s="448" t="s">
         <v>486</v>
       </c>
       <c r="I22" s="268" t="s">
         <v>517</v>
       </c>
-      <c r="J22" s="451" t="s">
+      <c r="J22" s="450" t="s">
         <v>527</v>
       </c>
     </row>
@@ -10838,18 +10880,20 @@
       <c r="C23" s="397">
         <v>2022</v>
       </c>
-      <c r="D23" s="418" t="s">
+      <c r="D23" s="417" t="s">
         <v>462</v>
       </c>
-      <c r="E23" s="425" t="s">
+      <c r="E23" s="424" t="s">
         <v>74</v>
       </c>
-      <c r="F23" s="426" t="s">
+      <c r="F23" s="425" t="s">
         <v>387</v>
       </c>
       <c r="G23" s="406"/>
-      <c r="H23" s="427"/>
-      <c r="I23" s="469"/>
+      <c r="H23" s="403" t="s">
+        <v>548</v>
+      </c>
+      <c r="I23" s="475"/>
       <c r="J23" s="212"/>
       <c r="K23" s="212"/>
       <c r="L23" s="212"/>
@@ -10867,20 +10911,20 @@
       <c r="C24" s="397">
         <v>2022</v>
       </c>
-      <c r="D24" s="418" t="s">
+      <c r="D24" s="417" t="s">
         <v>466</v>
       </c>
-      <c r="E24" s="425" t="s">
+      <c r="E24" s="424" t="s">
         <v>74</v>
       </c>
-      <c r="F24" s="428" t="s">
+      <c r="F24" s="427" t="s">
         <v>7</v>
       </c>
       <c r="G24" s="406"/>
-      <c r="H24" s="450" t="s">
+      <c r="H24" s="449" t="s">
         <v>512</v>
       </c>
-      <c r="I24" s="454" t="s">
+      <c r="I24" s="453" t="s">
         <v>518</v>
       </c>
       <c r="J24" s="100" t="s">
@@ -10902,20 +10946,20 @@
       <c r="C25" s="397">
         <v>2022</v>
       </c>
-      <c r="D25" s="418" t="s">
+      <c r="D25" s="417" t="s">
         <v>467</v>
       </c>
-      <c r="E25" s="425" t="s">
+      <c r="E25" s="424" t="s">
         <v>74</v>
       </c>
-      <c r="F25" s="428" t="s">
+      <c r="F25" s="427" t="s">
         <v>9</v>
       </c>
       <c r="G25" s="406"/>
-      <c r="H25" s="427" t="s">
+      <c r="H25" s="426" t="s">
         <v>540</v>
       </c>
-      <c r="I25" s="470" t="s">
+      <c r="I25" s="457" t="s">
         <v>515</v>
       </c>
       <c r="J25" s="105" t="s">
@@ -10937,20 +10981,20 @@
       <c r="C26" s="397">
         <v>2022</v>
       </c>
-      <c r="D26" s="418" t="s">
+      <c r="D26" s="417" t="s">
         <v>468</v>
       </c>
-      <c r="E26" s="425" t="s">
+      <c r="E26" s="424" t="s">
         <v>74</v>
       </c>
-      <c r="F26" s="428" t="s">
+      <c r="F26" s="427" t="s">
         <v>19</v>
       </c>
       <c r="G26" s="406"/>
-      <c r="H26" s="450" t="s">
+      <c r="H26" s="449" t="s">
         <v>504</v>
       </c>
-      <c r="I26" s="469" t="s">
+      <c r="I26" s="456" t="s">
         <v>539</v>
       </c>
       <c r="J26" s="65" t="s">
@@ -10966,23 +11010,23 @@
       <c r="A27" s="205">
         <v>25</v>
       </c>
-      <c r="B27" s="429" t="s">
+      <c r="B27" s="428" t="s">
         <v>184</v>
       </c>
-      <c r="C27" s="430" t="s">
+      <c r="C27" s="429" t="s">
         <v>195</v>
       </c>
-      <c r="D27" s="431" t="s">
+      <c r="D27" s="430" t="s">
         <v>461</v>
       </c>
-      <c r="E27" s="425" t="s">
+      <c r="E27" s="424" t="s">
         <v>74</v>
       </c>
-      <c r="F27" s="432" t="s">
+      <c r="F27" s="431" t="s">
         <v>318</v>
       </c>
       <c r="G27" s="406"/>
-      <c r="H27" s="427" t="s">
+      <c r="H27" s="426" t="s">
         <v>497</v>
       </c>
       <c r="I27" s="394" t="s">
@@ -11001,26 +11045,26 @@
       <c r="A28" s="205">
         <v>26</v>
       </c>
-      <c r="B28" s="433" t="s">
+      <c r="B28" s="432" t="s">
         <v>311</v>
       </c>
-      <c r="C28" s="434" t="s">
+      <c r="C28" s="433" t="s">
         <v>275</v>
       </c>
-      <c r="D28" s="435" t="s">
+      <c r="D28" s="434" t="s">
         <v>302</v>
       </c>
-      <c r="E28" s="436" t="s">
+      <c r="E28" s="435" t="s">
         <v>276</v>
       </c>
-      <c r="F28" s="437" t="s">
+      <c r="F28" s="436" t="s">
         <v>304</v>
       </c>
       <c r="G28" s="406"/>
-      <c r="H28" s="450" t="s">
+      <c r="H28" s="449" t="s">
         <v>510</v>
       </c>
-      <c r="I28" s="471" t="s">
+      <c r="I28" s="458" t="s">
         <v>533</v>
       </c>
       <c r="J28" s="212"/>
@@ -11034,23 +11078,23 @@
       <c r="A29" s="205">
         <v>27</v>
       </c>
-      <c r="B29" s="433" t="s">
+      <c r="B29" s="432" t="s">
         <v>310</v>
       </c>
-      <c r="C29" s="430" t="s">
+      <c r="C29" s="429" t="s">
         <v>275</v>
       </c>
-      <c r="D29" s="435" t="s">
+      <c r="D29" s="434" t="s">
         <v>303</v>
       </c>
-      <c r="E29" s="436" t="s">
+      <c r="E29" s="435" t="s">
         <v>276</v>
       </c>
-      <c r="F29" s="437" t="s">
+      <c r="F29" s="436" t="s">
         <v>55</v>
       </c>
       <c r="G29" s="406"/>
-      <c r="H29" s="438" t="s">
+      <c r="H29" s="437" t="s">
         <v>509</v>
       </c>
       <c r="I29" s="394"/>
@@ -11065,26 +11109,26 @@
       <c r="A30" s="205">
         <v>28</v>
       </c>
-      <c r="B30" s="439" t="s">
+      <c r="B30" s="438" t="s">
         <v>307</v>
       </c>
-      <c r="C30" s="434" t="s">
+      <c r="C30" s="433" t="s">
         <v>309</v>
       </c>
-      <c r="D30" s="440" t="s">
+      <c r="D30" s="439" t="s">
         <v>308</v>
       </c>
-      <c r="E30" s="441" t="s">
+      <c r="E30" s="440" t="s">
         <v>312</v>
       </c>
-      <c r="F30" s="442" t="s">
+      <c r="F30" s="441" t="s">
         <v>26</v>
       </c>
       <c r="G30" s="406"/>
-      <c r="H30" s="455" t="s">
+      <c r="H30" s="454" t="s">
         <v>487</v>
       </c>
-      <c r="I30" s="451" t="s">
+      <c r="I30" s="450" t="s">
         <v>529</v>
       </c>
       <c r="J30" s="212"/>
@@ -11098,29 +11142,29 @@
       <c r="A31" s="205">
         <v>29</v>
       </c>
-      <c r="B31" s="443" t="s">
+      <c r="B31" s="442" t="s">
         <v>478</v>
       </c>
-      <c r="C31" s="434" t="s">
+      <c r="C31" s="433" t="s">
         <v>480</v>
       </c>
-      <c r="D31" s="440" t="s">
+      <c r="D31" s="439" t="s">
         <v>482</v>
       </c>
-      <c r="E31" s="441" t="s">
+      <c r="E31" s="440" t="s">
         <v>481</v>
       </c>
-      <c r="F31" s="442" t="s">
+      <c r="F31" s="441" t="s">
         <v>479</v>
       </c>
       <c r="G31" s="406"/>
-      <c r="H31" s="448" t="s">
+      <c r="H31" s="447" t="s">
         <v>488</v>
       </c>
       <c r="I31" s="394" t="s">
         <v>516</v>
       </c>
-      <c r="J31" s="472" t="s">
+      <c r="J31" s="459" t="s">
         <v>524</v>
       </c>
     </row>
@@ -11128,23 +11172,23 @@
       <c r="A32" s="205">
         <v>30</v>
       </c>
-      <c r="B32" s="443" t="s">
+      <c r="B32" s="442" t="s">
         <v>412</v>
       </c>
-      <c r="C32" s="445" t="s">
+      <c r="C32" s="444" t="s">
         <v>503</v>
       </c>
-      <c r="D32" s="440" t="s">
+      <c r="D32" s="439" t="s">
         <v>499</v>
       </c>
-      <c r="E32" s="446" t="s">
+      <c r="E32" s="445" t="s">
         <v>500</v>
       </c>
-      <c r="F32" s="447" t="s">
+      <c r="F32" s="446" t="s">
         <v>501</v>
       </c>
       <c r="G32" s="406"/>
-      <c r="H32" s="453" t="s">
+      <c r="H32" s="452" t="s">
         <v>502</v>
       </c>
       <c r="I32" s="394" t="s">
@@ -11158,21 +11202,21 @@
       <c r="A33" s="205">
         <v>31</v>
       </c>
-      <c r="B33" s="443" t="s">
+      <c r="B33" s="442" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="434"/>
-      <c r="D33" s="440" t="s">
+      <c r="C33" s="433"/>
+      <c r="D33" s="439" t="s">
         <v>482</v>
       </c>
-      <c r="E33" s="441" t="s">
+      <c r="E33" s="440" t="s">
         <v>498</v>
       </c>
-      <c r="F33" s="442" t="s">
+      <c r="F33" s="441" t="s">
         <v>479</v>
       </c>
       <c r="G33" s="406"/>
-      <c r="H33" s="444" t="s">
+      <c r="H33" s="443" t="s">
         <v>488</v>
       </c>
       <c r="I33" s="246"/>
@@ -11244,14 +11288,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="462" t="s">
+      <c r="B1" s="464" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="462"/>
-      <c r="D1" s="462"/>
-      <c r="E1" s="463"/>
-      <c r="F1" s="462"/>
-      <c r="G1" s="462"/>
+      <c r="C1" s="464"/>
+      <c r="D1" s="464"/>
+      <c r="E1" s="465"/>
+      <c r="F1" s="464"/>
+      <c r="G1" s="464"/>
     </row>
     <row r="2" spans="1:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="200"/>
@@ -12461,11 +12505,11 @@
       <c r="A1" s="335" t="s">
         <v>367</v>
       </c>
-      <c r="B1" s="466"/>
-      <c r="C1" s="466"/>
-      <c r="D1" s="466"/>
-      <c r="E1" s="466"/>
-      <c r="F1" s="466"/>
+      <c r="B1" s="468"/>
+      <c r="C1" s="468"/>
+      <c r="D1" s="468"/>
+      <c r="E1" s="468"/>
+      <c r="F1" s="468"/>
     </row>
     <row r="2" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="336" t="s">
@@ -12906,12 +12950,12 @@
       <c r="F24" s="348" t="s">
         <v>379</v>
       </c>
-      <c r="G24" s="467"/>
-      <c r="H24" s="468"/>
-      <c r="I24" s="468"/>
-      <c r="J24" s="468"/>
-      <c r="K24" s="468"/>
-      <c r="L24" s="468"/>
+      <c r="G24" s="469"/>
+      <c r="H24" s="470"/>
+      <c r="I24" s="470"/>
+      <c r="J24" s="470"/>
+      <c r="K24" s="470"/>
+      <c r="L24" s="470"/>
     </row>
     <row r="25" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="344">
@@ -13031,7 +13075,7 @@
       <c r="C31" s="357">
         <v>2010</v>
       </c>
-      <c r="D31" s="452" t="s">
+      <c r="D31" s="451" t="s">
         <v>442</v>
       </c>
       <c r="E31" s="354" t="s">

</xml_diff>

<commit_message>
CIERRE 28 DIC 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
+++ b/01 DOCUEMENTOS/CAMIONETAS  2 0 2 0.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1341" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="567">
   <si>
     <t xml:space="preserve">RELACION DE UNIDADES Y ASIGNACION </t>
   </si>
@@ -1821,6 +1821,12 @@
   </si>
   <si>
     <t>15-Dic-23   283,066 KM</t>
+  </si>
+  <si>
+    <t>RAM 4000</t>
+  </si>
+  <si>
+    <t>SP-85416</t>
   </si>
 </sst>
 </file>
@@ -2219,7 +2225,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="27">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2365,6 +2371,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFF99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2768,7 +2780,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="500">
+  <cellXfs count="507">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4169,6 +4181,25 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="47" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="48" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="26" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="48" fillId="27" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="26" fillId="27" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="27" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4179,6 +4210,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCCFF99"/>
       <color rgb="FF9999FF"/>
       <color rgb="FF9966FF"/>
       <color rgb="FFCC6600"/>
@@ -4188,7 +4220,6 @@
       <color rgb="FFFFCCFF"/>
       <color rgb="FF00FF00"/>
       <color rgb="FF00FFFF"/>
-      <color rgb="FFFF9900"/>
     </mruColors>
   </colors>
   <extLst>
@@ -10429,8 +10460,8 @@
   </sheetPr>
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -11432,11 +11463,45 @@
       </c>
       <c r="I34" s="246"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A35" s="205"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A36" s="205"/>
+    <row r="35" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="205">
+        <v>32</v>
+      </c>
+      <c r="B35" s="441" t="s">
+        <v>565</v>
+      </c>
+      <c r="C35" s="500">
+        <v>2023</v>
+      </c>
+      <c r="D35" s="504" t="s">
+        <v>566</v>
+      </c>
+      <c r="E35" s="505" t="s">
+        <v>74</v>
+      </c>
+      <c r="F35" s="506" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" s="503"/>
+      <c r="H35" s="446"/>
+      <c r="I35" s="246"/>
+    </row>
+    <row r="36" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="205">
+        <v>32</v>
+      </c>
+      <c r="B36" s="441" t="s">
+        <v>565</v>
+      </c>
+      <c r="C36" s="500">
+        <v>2023</v>
+      </c>
+      <c r="D36" s="501"/>
+      <c r="E36" s="502"/>
+      <c r="F36" s="440"/>
+      <c r="G36" s="503"/>
+      <c r="H36" s="446"/>
+      <c r="I36" s="246"/>
     </row>
   </sheetData>
   <sortState ref="B3:J10">

</xml_diff>